<commit_message>
Conferência Mapeamento LN - FAT e SKU
</commit_message>
<xml_diff>
--- a/Documentação/Planilhas/Conferencia_FAT.xlsx
+++ b/Documentação/Planilhas/Conferencia_FAT.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="538">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="535">
   <si>
     <t>1</t>
   </si>
@@ -967,9 +967,6 @@
     <t>12</t>
   </si>
   <si>
-    <t>2014-09-02 08:39:49.000</t>
-  </si>
-  <si>
     <t>17.5240</t>
   </si>
   <si>
@@ -1018,9 +1015,6 @@
     <t>18.8900</t>
   </si>
   <si>
-    <t>18.89</t>
-  </si>
-  <si>
     <t>0.31</t>
   </si>
   <si>
@@ -1033,9 +1027,6 @@
     <t>0.6764</t>
   </si>
   <si>
-    <t>2014-09-02 11:15:36.000</t>
-  </si>
-  <si>
     <t>8.4782</t>
   </si>
   <si>
@@ -1078,9 +1069,6 @@
     <t>473.8900</t>
   </si>
   <si>
-    <t>473.89</t>
-  </si>
-  <si>
     <t>7.82</t>
   </si>
   <si>
@@ -1096,9 +1084,6 @@
     <t>33987051892</t>
   </si>
   <si>
-    <t>2014-09-02 14:25:30.000</t>
-  </si>
-  <si>
     <t>360.4358</t>
   </si>
   <si>
@@ -1144,9 +1129,6 @@
     <t>550.4400</t>
   </si>
   <si>
-    <t>550.44</t>
-  </si>
-  <si>
     <t>9.08</t>
   </si>
   <si>
@@ -1168,9 +1150,6 @@
     <t>16940282831</t>
   </si>
   <si>
-    <t>2014-09-02 16:00:00.000</t>
-  </si>
-  <si>
     <t>356.0494</t>
   </si>
   <si>
@@ -1222,9 +1201,6 @@
     <t>544.8900</t>
   </si>
   <si>
-    <t>544.89</t>
-  </si>
-  <si>
     <t>32690119897</t>
   </si>
   <si>
@@ -1282,9 +1258,6 @@
     <t>103.8900</t>
   </si>
   <si>
-    <t>103.89</t>
-  </si>
-  <si>
     <t>1.71</t>
   </si>
   <si>
@@ -1348,9 +1321,6 @@
     <t>1362.8900</t>
   </si>
   <si>
-    <t>1362.89</t>
-  </si>
-  <si>
     <t>22.49</t>
   </si>
   <si>
@@ -1414,9 +1384,6 @@
     <t>2057.4000</t>
   </si>
   <si>
-    <t>2057.40</t>
-  </si>
-  <si>
     <t>39147387823</t>
   </si>
   <si>
@@ -1537,9 +1504,6 @@
     <t>183.8900</t>
   </si>
   <si>
-    <t>183.89</t>
-  </si>
-  <si>
     <t>3.03</t>
   </si>
   <si>
@@ -1658,6 +1622,33 @@
   </si>
   <si>
     <t>Está vindo branco na view</t>
+  </si>
+  <si>
+    <t>2014-09-17 11:18:50.000</t>
+  </si>
+  <si>
+    <t>2014-09-17 11:18:47.000</t>
+  </si>
+  <si>
+    <t>2014-09-19 12:29:47.000</t>
+  </si>
+  <si>
+    <t>2014-09-17 11:18:51.000</t>
+  </si>
+  <si>
+    <t>2014-09-19 12:30:57.000</t>
+  </si>
+  <si>
+    <t>2014-09-19 12:29:23.000</t>
+  </si>
+  <si>
+    <t>2014-09-17 11:18:49.000</t>
+  </si>
+  <si>
+    <t>2014-09-19 12:28:38.000</t>
+  </si>
+  <si>
+    <t>2014-09-17 11:18:52.000</t>
   </si>
 </sst>
 </file>
@@ -1718,7 +1709,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1758,12 +1749,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFA7E7E"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1938,7 +1923,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2023,60 +2008,6 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2086,43 +2017,13 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2161,8 +2062,89 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2840,7 +2822,7 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="20" t="s">
-        <v>508</v>
+        <v>496</v>
       </c>
       <c r="B19" s="21"/>
       <c r="C19" s="21"/>
@@ -2932,8 +2914,8 @@
   </sheetPr>
   <dimension ref="A1:CD80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AF8" sqref="AF8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AG11" sqref="AG11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -3299,7 +3281,7 @@
     </row>
     <row r="7" spans="1:82" s="9" customFormat="1">
       <c r="A7" s="13" t="s">
-        <v>286</v>
+        <v>417</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>87</v>
@@ -3326,16 +3308,16 @@
         <v>86</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>287</v>
+        <v>418</v>
       </c>
       <c r="K7" s="13" t="s">
-        <v>288</v>
+        <v>397</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>289</v>
+        <v>526</v>
       </c>
       <c r="M7" s="13" t="s">
-        <v>290</v>
+        <v>419</v>
       </c>
       <c r="N7" s="13" t="s">
         <v>291</v>
@@ -3347,34 +3329,34 @@
         <v>158</v>
       </c>
       <c r="Q7" s="13" t="s">
-        <v>292</v>
+        <v>420</v>
       </c>
       <c r="R7" s="13" t="s">
-        <v>292</v>
+        <v>420</v>
       </c>
       <c r="S7" s="13" t="s">
         <v>293</v>
       </c>
       <c r="T7" s="13" t="s">
-        <v>294</v>
+        <v>421</v>
       </c>
       <c r="U7" s="13" t="s">
-        <v>294</v>
+        <v>421</v>
       </c>
       <c r="V7" s="13" t="s">
         <v>91</v>
       </c>
       <c r="W7" s="13" t="s">
-        <v>295</v>
+        <v>422</v>
       </c>
       <c r="X7" s="13" t="s">
         <v>25</v>
       </c>
       <c r="Y7" s="13" t="s">
-        <v>296</v>
+        <v>423</v>
       </c>
       <c r="Z7" s="13" t="s">
-        <v>297</v>
+        <v>424</v>
       </c>
       <c r="AA7" s="13" t="s">
         <v>88</v>
@@ -3391,8 +3373,8 @@
       <c r="AE7" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="AF7" s="76" t="s">
-        <v>88</v>
+      <c r="AF7" s="13" t="s">
+        <v>85</v>
       </c>
       <c r="AG7" s="13" t="s">
         <v>85</v>
@@ -3410,25 +3392,25 @@
         <v>88</v>
       </c>
       <c r="AL7" s="13" t="s">
-        <v>298</v>
+        <v>425</v>
       </c>
       <c r="AM7" s="13" t="s">
-        <v>299</v>
+        <v>426</v>
       </c>
       <c r="AN7" s="13" t="s">
-        <v>300</v>
+        <v>427</v>
       </c>
       <c r="AO7" s="13" t="s">
         <v>88</v>
       </c>
       <c r="AP7" s="13" t="s">
-        <v>301</v>
+        <v>428</v>
       </c>
       <c r="AQ7" s="13" t="s">
-        <v>302</v>
+        <v>429</v>
       </c>
       <c r="AR7" s="13" t="s">
-        <v>303</v>
+        <v>430</v>
       </c>
       <c r="AS7" s="13" t="s">
         <v>88</v>
@@ -3452,13 +3434,13 @@
         <v>93</v>
       </c>
       <c r="AZ7" s="13" t="s">
-        <v>304</v>
+        <v>431</v>
       </c>
       <c r="BA7" s="13" t="s">
         <v>93</v>
       </c>
       <c r="BB7" s="13" t="s">
-        <v>304</v>
+        <v>431</v>
       </c>
       <c r="BC7" s="13" t="s">
         <v>195</v>
@@ -3473,28 +3455,28 @@
         <v>306</v>
       </c>
       <c r="BG7" s="13" t="s">
-        <v>307</v>
+        <v>398</v>
       </c>
       <c r="BH7" s="13" t="s">
-        <v>308</v>
+        <v>432</v>
       </c>
       <c r="BI7" s="13" t="s">
         <v>25</v>
       </c>
       <c r="BJ7" s="13" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="BK7" s="13" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="BL7" s="13" t="s">
-        <v>310</v>
+        <v>433</v>
       </c>
       <c r="BM7" s="13" t="s">
         <v>0</v>
       </c>
       <c r="BN7" s="13" t="s">
-        <v>311</v>
+        <v>434</v>
       </c>
       <c r="BO7" s="13" t="s">
         <v>0</v>
@@ -3506,7 +3488,7 @@
         <v>89</v>
       </c>
       <c r="BR7" s="13" t="s">
-        <v>312</v>
+        <v>435</v>
       </c>
       <c r="BS7" s="13" t="s">
         <v>85</v>
@@ -3515,13 +3497,13 @@
         <v>85</v>
       </c>
       <c r="BU7" s="13" t="s">
-        <v>313</v>
+        <v>436</v>
       </c>
       <c r="BV7" s="13" t="s">
-        <v>295</v>
+        <v>422</v>
       </c>
       <c r="BW7" s="13" t="s">
-        <v>314</v>
+        <v>416</v>
       </c>
       <c r="BX7" s="13" t="s">
         <v>0</v>
@@ -3547,7 +3529,7 @@
     </row>
     <row r="8" spans="1:82" s="9" customFormat="1">
       <c r="A8" s="8" t="s">
-        <v>315</v>
+        <v>437</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>87</v>
@@ -3574,16 +3556,16 @@
         <v>86</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>316</v>
+        <v>438</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>317</v>
+        <v>397</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>318</v>
+        <v>527</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>319</v>
+        <v>439</v>
       </c>
       <c r="N8" s="8" t="s">
         <v>291</v>
@@ -3595,34 +3577,34 @@
         <v>158</v>
       </c>
       <c r="Q8" s="8" t="s">
-        <v>292</v>
+        <v>440</v>
       </c>
       <c r="R8" s="8" t="s">
-        <v>292</v>
+        <v>441</v>
       </c>
       <c r="S8" s="8" t="s">
         <v>293</v>
       </c>
       <c r="T8" s="8" t="s">
-        <v>320</v>
+        <v>442</v>
       </c>
       <c r="U8" s="8" t="s">
-        <v>320</v>
+        <v>442</v>
       </c>
       <c r="V8" s="8" t="s">
         <v>91</v>
       </c>
       <c r="W8" s="8" t="s">
-        <v>321</v>
+        <v>443</v>
       </c>
       <c r="X8" s="8" t="s">
         <v>25</v>
       </c>
       <c r="Y8" s="8" t="s">
-        <v>322</v>
+        <v>444</v>
       </c>
       <c r="Z8" s="8" t="s">
-        <v>323</v>
+        <v>445</v>
       </c>
       <c r="AA8" s="8" t="s">
         <v>88</v>
@@ -3639,8 +3621,8 @@
       <c r="AE8" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="AF8" s="76" t="s">
-        <v>324</v>
+      <c r="AF8" s="8" t="s">
+        <v>85</v>
       </c>
       <c r="AG8" s="8" t="s">
         <v>85</v>
@@ -3658,25 +3640,25 @@
         <v>88</v>
       </c>
       <c r="AL8" s="8" t="s">
-        <v>325</v>
+        <v>85</v>
       </c>
       <c r="AM8" s="8" t="s">
-        <v>326</v>
+        <v>88</v>
       </c>
       <c r="AN8" s="8" t="s">
-        <v>300</v>
+        <v>88</v>
       </c>
       <c r="AO8" s="8" t="s">
         <v>88</v>
       </c>
       <c r="AP8" s="8" t="s">
-        <v>327</v>
+        <v>85</v>
       </c>
       <c r="AQ8" s="8" t="s">
-        <v>328</v>
+        <v>88</v>
       </c>
       <c r="AR8" s="8" t="s">
-        <v>303</v>
+        <v>88</v>
       </c>
       <c r="AS8" s="8" t="s">
         <v>88</v>
@@ -3700,13 +3682,13 @@
         <v>93</v>
       </c>
       <c r="AZ8" s="8" t="s">
-        <v>304</v>
+        <v>446</v>
       </c>
       <c r="BA8" s="8" t="s">
         <v>93</v>
       </c>
       <c r="BB8" s="8" t="s">
-        <v>304</v>
+        <v>446</v>
       </c>
       <c r="BC8" s="8" t="s">
         <v>195</v>
@@ -3721,28 +3703,28 @@
         <v>306</v>
       </c>
       <c r="BG8" s="8" t="s">
-        <v>329</v>
+        <v>398</v>
       </c>
       <c r="BH8" s="8" t="s">
-        <v>330</v>
+        <v>447</v>
       </c>
       <c r="BI8" s="8" t="s">
         <v>25</v>
       </c>
       <c r="BJ8" s="8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="BK8" s="8" t="s">
         <v>0</v>
       </c>
       <c r="BL8" s="8" t="s">
-        <v>331</v>
+        <v>448</v>
       </c>
       <c r="BM8" s="8" t="s">
         <v>0</v>
       </c>
       <c r="BN8" s="8" t="s">
-        <v>332</v>
+        <v>449</v>
       </c>
       <c r="BO8" s="8" t="s">
         <v>0</v>
@@ -3754,7 +3736,7 @@
         <v>89</v>
       </c>
       <c r="BR8" s="8" t="s">
-        <v>333</v>
+        <v>450</v>
       </c>
       <c r="BS8" s="8" t="s">
         <v>85</v>
@@ -3763,22 +3745,22 @@
         <v>85</v>
       </c>
       <c r="BU8" s="8" t="s">
-        <v>313</v>
+        <v>415</v>
       </c>
       <c r="BV8" s="8" t="s">
-        <v>321</v>
+        <v>443</v>
       </c>
       <c r="BW8" s="8" t="s">
-        <v>314</v>
+        <v>416</v>
       </c>
       <c r="BX8" s="8" t="s">
-        <v>91</v>
+        <v>0</v>
       </c>
       <c r="BY8" s="8" t="s">
-        <v>88</v>
+        <v>451</v>
       </c>
       <c r="BZ8" s="8" t="s">
-        <v>88</v>
+        <v>451</v>
       </c>
       <c r="CA8" s="8" t="s">
         <v>88</v>
@@ -3795,7 +3777,7 @@
     </row>
     <row r="9" spans="1:82" s="9" customFormat="1">
       <c r="A9" s="8" t="s">
-        <v>194</v>
+        <v>374</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>87</v>
@@ -3822,16 +3804,16 @@
         <v>86</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>334</v>
+        <v>375</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>335</v>
+        <v>376</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>336</v>
+        <v>377</v>
       </c>
       <c r="M9" s="8" t="s">
-        <v>337</v>
+        <v>378</v>
       </c>
       <c r="N9" s="8" t="s">
         <v>291</v>
@@ -3843,34 +3825,34 @@
         <v>158</v>
       </c>
       <c r="Q9" s="8" t="s">
-        <v>338</v>
+        <v>379</v>
       </c>
       <c r="R9" s="8" t="s">
-        <v>339</v>
+        <v>379</v>
       </c>
       <c r="S9" s="8" t="s">
-        <v>293</v>
+        <v>380</v>
       </c>
       <c r="T9" s="8" t="s">
-        <v>340</v>
+        <v>381</v>
       </c>
       <c r="U9" s="8" t="s">
-        <v>340</v>
+        <v>381</v>
       </c>
       <c r="V9" s="8" t="s">
         <v>91</v>
       </c>
       <c r="W9" s="8" t="s">
-        <v>341</v>
+        <v>382</v>
       </c>
       <c r="X9" s="8" t="s">
         <v>25</v>
       </c>
       <c r="Y9" s="8" t="s">
-        <v>342</v>
+        <v>383</v>
       </c>
       <c r="Z9" s="8" t="s">
-        <v>343</v>
+        <v>384</v>
       </c>
       <c r="AA9" s="8" t="s">
         <v>88</v>
@@ -3887,8 +3869,8 @@
       <c r="AE9" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="AF9" s="76" t="s">
-        <v>344</v>
+      <c r="AF9" s="8" t="s">
+        <v>85</v>
       </c>
       <c r="AG9" s="8" t="s">
         <v>85</v>
@@ -3906,25 +3888,25 @@
         <v>88</v>
       </c>
       <c r="AL9" s="8" t="s">
-        <v>345</v>
+        <v>85</v>
       </c>
       <c r="AM9" s="8" t="s">
-        <v>346</v>
+        <v>88</v>
       </c>
       <c r="AN9" s="8" t="s">
-        <v>300</v>
+        <v>88</v>
       </c>
       <c r="AO9" s="8" t="s">
         <v>88</v>
       </c>
       <c r="AP9" s="8" t="s">
-        <v>347</v>
+        <v>85</v>
       </c>
       <c r="AQ9" s="8" t="s">
-        <v>348</v>
+        <v>88</v>
       </c>
       <c r="AR9" s="8" t="s">
-        <v>303</v>
+        <v>88</v>
       </c>
       <c r="AS9" s="8" t="s">
         <v>88</v>
@@ -3948,19 +3930,19 @@
         <v>93</v>
       </c>
       <c r="AZ9" s="8" t="s">
-        <v>349</v>
+        <v>385</v>
       </c>
       <c r="BA9" s="8" t="s">
         <v>93</v>
       </c>
       <c r="BB9" s="8" t="s">
-        <v>349</v>
+        <v>385</v>
       </c>
       <c r="BC9" s="8" t="s">
-        <v>90</v>
+        <v>386</v>
       </c>
       <c r="BD9" s="8" t="s">
-        <v>90</v>
+        <v>386</v>
       </c>
       <c r="BE9" s="8" t="s">
         <v>305</v>
@@ -3969,28 +3951,28 @@
         <v>306</v>
       </c>
       <c r="BG9" s="8" t="s">
-        <v>350</v>
+        <v>387</v>
       </c>
       <c r="BH9" s="8" t="s">
-        <v>351</v>
+        <v>388</v>
       </c>
       <c r="BI9" s="8" t="s">
         <v>25</v>
       </c>
       <c r="BJ9" s="8" t="s">
-        <v>309</v>
+        <v>389</v>
       </c>
       <c r="BK9" s="8" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="BL9" s="8" t="s">
-        <v>352</v>
+        <v>390</v>
       </c>
       <c r="BM9" s="8" t="s">
         <v>0</v>
       </c>
       <c r="BN9" s="8" t="s">
-        <v>353</v>
+        <v>391</v>
       </c>
       <c r="BO9" s="8" t="s">
         <v>0</v>
@@ -4002,7 +3984,7 @@
         <v>89</v>
       </c>
       <c r="BR9" s="8" t="s">
-        <v>354</v>
+        <v>392</v>
       </c>
       <c r="BS9" s="8" t="s">
         <v>85</v>
@@ -4011,13 +3993,13 @@
         <v>85</v>
       </c>
       <c r="BU9" s="8" t="s">
-        <v>313</v>
+        <v>393</v>
       </c>
       <c r="BV9" s="8" t="s">
-        <v>341</v>
+        <v>382</v>
       </c>
       <c r="BW9" s="8" t="s">
-        <v>355</v>
+        <v>394</v>
       </c>
       <c r="BX9" s="8" t="s">
         <v>0</v>
@@ -4043,7 +4025,7 @@
     </row>
     <row r="10" spans="1:82" s="9" customFormat="1">
       <c r="A10" s="8" t="s">
-        <v>356</v>
+        <v>194</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>87</v>
@@ -4070,16 +4052,16 @@
         <v>86</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>357</v>
+        <v>331</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>358</v>
+        <v>332</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>359</v>
+        <v>333</v>
       </c>
       <c r="M10" s="8" t="s">
-        <v>360</v>
+        <v>334</v>
       </c>
       <c r="N10" s="8" t="s">
         <v>291</v>
@@ -4091,34 +4073,34 @@
         <v>158</v>
       </c>
       <c r="Q10" s="8" t="s">
-        <v>361</v>
+        <v>335</v>
       </c>
       <c r="R10" s="8" t="s">
-        <v>361</v>
+        <v>336</v>
       </c>
       <c r="S10" s="8" t="s">
         <v>293</v>
       </c>
       <c r="T10" s="8" t="s">
-        <v>362</v>
+        <v>337</v>
       </c>
       <c r="U10" s="8" t="s">
-        <v>362</v>
+        <v>337</v>
       </c>
       <c r="V10" s="8" t="s">
         <v>91</v>
       </c>
       <c r="W10" s="8" t="s">
-        <v>363</v>
+        <v>338</v>
       </c>
       <c r="X10" s="8" t="s">
         <v>25</v>
       </c>
       <c r="Y10" s="8" t="s">
-        <v>364</v>
+        <v>339</v>
       </c>
       <c r="Z10" s="8" t="s">
-        <v>365</v>
+        <v>340</v>
       </c>
       <c r="AA10" s="8" t="s">
         <v>88</v>
@@ -4135,8 +4117,8 @@
       <c r="AE10" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="AF10" s="76" t="s">
-        <v>366</v>
+      <c r="AF10" s="8" t="s">
+        <v>85</v>
       </c>
       <c r="AG10" s="8" t="s">
         <v>85</v>
@@ -4154,28 +4136,28 @@
         <v>88</v>
       </c>
       <c r="AL10" s="8" t="s">
-        <v>367</v>
+        <v>341</v>
       </c>
       <c r="AM10" s="8" t="s">
-        <v>368</v>
+        <v>342</v>
       </c>
       <c r="AN10" s="8" t="s">
         <v>300</v>
       </c>
       <c r="AO10" s="8" t="s">
-        <v>369</v>
+        <v>88</v>
       </c>
       <c r="AP10" s="8" t="s">
-        <v>370</v>
+        <v>343</v>
       </c>
       <c r="AQ10" s="8" t="s">
-        <v>371</v>
+        <v>344</v>
       </c>
       <c r="AR10" s="8" t="s">
         <v>303</v>
       </c>
       <c r="AS10" s="8" t="s">
-        <v>372</v>
+        <v>88</v>
       </c>
       <c r="AT10" s="8" t="s">
         <v>88</v>
@@ -4196,19 +4178,19 @@
         <v>93</v>
       </c>
       <c r="AZ10" s="8" t="s">
-        <v>373</v>
+        <v>345</v>
       </c>
       <c r="BA10" s="8" t="s">
         <v>93</v>
       </c>
       <c r="BB10" s="8" t="s">
-        <v>373</v>
+        <v>345</v>
       </c>
       <c r="BC10" s="8" t="s">
-        <v>195</v>
+        <v>90</v>
       </c>
       <c r="BD10" s="8" t="s">
-        <v>195</v>
+        <v>90</v>
       </c>
       <c r="BE10" s="8" t="s">
         <v>305</v>
@@ -4217,28 +4199,28 @@
         <v>306</v>
       </c>
       <c r="BG10" s="8" t="s">
-        <v>374</v>
+        <v>528</v>
       </c>
       <c r="BH10" s="8" t="s">
-        <v>375</v>
+        <v>346</v>
       </c>
       <c r="BI10" s="8" t="s">
         <v>25</v>
       </c>
       <c r="BJ10" s="8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="BK10" s="8" t="s">
         <v>26</v>
       </c>
       <c r="BL10" s="8" t="s">
-        <v>376</v>
+        <v>347</v>
       </c>
       <c r="BM10" s="8" t="s">
         <v>0</v>
       </c>
       <c r="BN10" s="8" t="s">
-        <v>377</v>
+        <v>348</v>
       </c>
       <c r="BO10" s="8" t="s">
         <v>0</v>
@@ -4250,7 +4232,7 @@
         <v>89</v>
       </c>
       <c r="BR10" s="8" t="s">
-        <v>378</v>
+        <v>349</v>
       </c>
       <c r="BS10" s="8" t="s">
         <v>85</v>
@@ -4259,22 +4241,22 @@
         <v>85</v>
       </c>
       <c r="BU10" s="8" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="BV10" s="8" t="s">
-        <v>363</v>
+        <v>338</v>
       </c>
       <c r="BW10" s="8" t="s">
-        <v>379</v>
+        <v>350</v>
       </c>
       <c r="BX10" s="8" t="s">
         <v>0</v>
       </c>
       <c r="BY10" s="8" t="s">
-        <v>380</v>
+        <v>88</v>
       </c>
       <c r="BZ10" s="8" t="s">
-        <v>380</v>
+        <v>88</v>
       </c>
       <c r="CA10" s="8" t="s">
         <v>88</v>
@@ -4291,7 +4273,7 @@
     </row>
     <row r="11" spans="1:82" s="9" customFormat="1">
       <c r="A11" s="8" t="s">
-        <v>381</v>
+        <v>452</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>87</v>
@@ -4318,16 +4300,16 @@
         <v>86</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>382</v>
+        <v>453</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>383</v>
+        <v>454</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>384</v>
+        <v>529</v>
       </c>
       <c r="M11" s="8" t="s">
-        <v>385</v>
+        <v>455</v>
       </c>
       <c r="N11" s="8" t="s">
         <v>291</v>
@@ -4339,43 +4321,43 @@
         <v>158</v>
       </c>
       <c r="Q11" s="8" t="s">
-        <v>386</v>
+        <v>456</v>
       </c>
       <c r="R11" s="8" t="s">
-        <v>386</v>
+        <v>456</v>
       </c>
       <c r="S11" s="8" t="s">
-        <v>387</v>
+        <v>457</v>
       </c>
       <c r="T11" s="8" t="s">
-        <v>388</v>
+        <v>458</v>
       </c>
       <c r="U11" s="8" t="s">
-        <v>388</v>
+        <v>458</v>
       </c>
       <c r="V11" s="8" t="s">
         <v>91</v>
       </c>
       <c r="W11" s="8" t="s">
-        <v>389</v>
+        <v>459</v>
       </c>
       <c r="X11" s="8" t="s">
         <v>25</v>
       </c>
       <c r="Y11" s="8" t="s">
-        <v>390</v>
+        <v>460</v>
       </c>
       <c r="Z11" s="8" t="s">
-        <v>391</v>
+        <v>461</v>
       </c>
       <c r="AA11" s="8" t="s">
         <v>88</v>
       </c>
       <c r="AB11" s="8" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="AC11" s="8" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="AD11" s="8" t="s">
         <v>88</v>
@@ -4383,44 +4365,44 @@
       <c r="AE11" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="AF11" s="76" t="s">
-        <v>392</v>
+      <c r="AF11" s="8" t="s">
+        <v>462</v>
       </c>
       <c r="AG11" s="8" t="s">
-        <v>85</v>
+        <v>463</v>
       </c>
       <c r="AH11" s="8" t="s">
         <v>85</v>
       </c>
       <c r="AI11" s="8" t="s">
-        <v>88</v>
+        <v>464</v>
       </c>
       <c r="AJ11" s="8" t="s">
-        <v>88</v>
+        <v>465</v>
       </c>
       <c r="AK11" s="8" t="s">
         <v>88</v>
       </c>
       <c r="AL11" s="8" t="s">
-        <v>85</v>
+        <v>466</v>
       </c>
       <c r="AM11" s="8" t="s">
-        <v>88</v>
+        <v>467</v>
       </c>
       <c r="AN11" s="8" t="s">
-        <v>88</v>
+        <v>300</v>
       </c>
       <c r="AO11" s="8" t="s">
         <v>88</v>
       </c>
       <c r="AP11" s="8" t="s">
-        <v>85</v>
+        <v>468</v>
       </c>
       <c r="AQ11" s="8" t="s">
-        <v>88</v>
+        <v>469</v>
       </c>
       <c r="AR11" s="8" t="s">
-        <v>88</v>
+        <v>303</v>
       </c>
       <c r="AS11" s="8" t="s">
         <v>88</v>
@@ -4444,19 +4426,19 @@
         <v>93</v>
       </c>
       <c r="AZ11" s="8" t="s">
-        <v>393</v>
+        <v>470</v>
       </c>
       <c r="BA11" s="8" t="s">
         <v>93</v>
       </c>
       <c r="BB11" s="8" t="s">
-        <v>393</v>
+        <v>470</v>
       </c>
       <c r="BC11" s="8" t="s">
-        <v>394</v>
+        <v>471</v>
       </c>
       <c r="BD11" s="8" t="s">
-        <v>394</v>
+        <v>471</v>
       </c>
       <c r="BE11" s="8" t="s">
         <v>305</v>
@@ -4465,28 +4447,28 @@
         <v>306</v>
       </c>
       <c r="BG11" s="8" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="BH11" s="8" t="s">
-        <v>396</v>
+        <v>472</v>
       </c>
       <c r="BI11" s="8" t="s">
         <v>25</v>
       </c>
       <c r="BJ11" s="8" t="s">
-        <v>397</v>
+        <v>473</v>
       </c>
       <c r="BK11" s="8" t="s">
         <v>0</v>
       </c>
       <c r="BL11" s="8" t="s">
-        <v>398</v>
+        <v>474</v>
       </c>
       <c r="BM11" s="8" t="s">
         <v>0</v>
       </c>
       <c r="BN11" s="8" t="s">
-        <v>399</v>
+        <v>475</v>
       </c>
       <c r="BO11" s="8" t="s">
         <v>0</v>
@@ -4498,7 +4480,7 @@
         <v>89</v>
       </c>
       <c r="BR11" s="8" t="s">
-        <v>400</v>
+        <v>476</v>
       </c>
       <c r="BS11" s="8" t="s">
         <v>85</v>
@@ -4507,13 +4489,13 @@
         <v>85</v>
       </c>
       <c r="BU11" s="8" t="s">
-        <v>401</v>
+        <v>312</v>
       </c>
       <c r="BV11" s="8" t="s">
-        <v>389</v>
+        <v>459</v>
       </c>
       <c r="BW11" s="8" t="s">
-        <v>402</v>
+        <v>477</v>
       </c>
       <c r="BX11" s="8" t="s">
         <v>0</v>
@@ -4539,10 +4521,10 @@
     </row>
     <row r="12" spans="1:82" s="9" customFormat="1">
       <c r="A12" s="8" t="s">
-        <v>403</v>
+        <v>351</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>0</v>
@@ -4566,16 +4548,16 @@
         <v>86</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>404</v>
+        <v>352</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>405</v>
+        <v>353</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>406</v>
+        <v>354</v>
       </c>
       <c r="M12" s="8" t="s">
-        <v>407</v>
+        <v>355</v>
       </c>
       <c r="N12" s="8" t="s">
         <v>291</v>
@@ -4587,34 +4569,34 @@
         <v>158</v>
       </c>
       <c r="Q12" s="8" t="s">
-        <v>408</v>
+        <v>356</v>
       </c>
       <c r="R12" s="8" t="s">
-        <v>408</v>
+        <v>356</v>
       </c>
       <c r="S12" s="8" t="s">
         <v>293</v>
       </c>
       <c r="T12" s="8" t="s">
-        <v>159</v>
+        <v>357</v>
       </c>
       <c r="U12" s="8" t="s">
-        <v>159</v>
+        <v>357</v>
       </c>
       <c r="V12" s="8" t="s">
         <v>91</v>
       </c>
       <c r="W12" s="8" t="s">
-        <v>409</v>
+        <v>358</v>
       </c>
       <c r="X12" s="8" t="s">
         <v>25</v>
       </c>
       <c r="Y12" s="8" t="s">
-        <v>410</v>
+        <v>359</v>
       </c>
       <c r="Z12" s="8" t="s">
-        <v>411</v>
+        <v>360</v>
       </c>
       <c r="AA12" s="8" t="s">
         <v>88</v>
@@ -4631,8 +4613,8 @@
       <c r="AE12" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="AF12" s="76" t="s">
-        <v>412</v>
+      <c r="AF12" s="8" t="s">
+        <v>85</v>
       </c>
       <c r="AG12" s="8" t="s">
         <v>85</v>
@@ -4650,28 +4632,28 @@
         <v>88</v>
       </c>
       <c r="AL12" s="8" t="s">
-        <v>413</v>
+        <v>361</v>
       </c>
       <c r="AM12" s="8" t="s">
-        <v>414</v>
+        <v>362</v>
       </c>
       <c r="AN12" s="8" t="s">
-        <v>415</v>
+        <v>300</v>
       </c>
       <c r="AO12" s="8" t="s">
-        <v>88</v>
+        <v>363</v>
       </c>
       <c r="AP12" s="8" t="s">
-        <v>416</v>
+        <v>364</v>
       </c>
       <c r="AQ12" s="8" t="s">
-        <v>417</v>
+        <v>365</v>
       </c>
       <c r="AR12" s="8" t="s">
-        <v>418</v>
+        <v>303</v>
       </c>
       <c r="AS12" s="8" t="s">
-        <v>88</v>
+        <v>366</v>
       </c>
       <c r="AT12" s="8" t="s">
         <v>88</v>
@@ -4692,13 +4674,13 @@
         <v>93</v>
       </c>
       <c r="AZ12" s="8" t="s">
-        <v>419</v>
+        <v>367</v>
       </c>
       <c r="BA12" s="8" t="s">
         <v>93</v>
       </c>
       <c r="BB12" s="8" t="s">
-        <v>419</v>
+        <v>367</v>
       </c>
       <c r="BC12" s="8" t="s">
         <v>195</v>
@@ -4713,28 +4695,28 @@
         <v>306</v>
       </c>
       <c r="BG12" s="8" t="s">
-        <v>406</v>
+        <v>530</v>
       </c>
       <c r="BH12" s="8" t="s">
-        <v>420</v>
+        <v>368</v>
       </c>
       <c r="BI12" s="8" t="s">
         <v>25</v>
       </c>
       <c r="BJ12" s="8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="BK12" s="8" t="s">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="BL12" s="8" t="s">
-        <v>421</v>
+        <v>369</v>
       </c>
       <c r="BM12" s="8" t="s">
         <v>0</v>
       </c>
       <c r="BN12" s="8" t="s">
-        <v>422</v>
+        <v>370</v>
       </c>
       <c r="BO12" s="8" t="s">
         <v>0</v>
@@ -4746,7 +4728,7 @@
         <v>89</v>
       </c>
       <c r="BR12" s="8" t="s">
-        <v>423</v>
+        <v>371</v>
       </c>
       <c r="BS12" s="8" t="s">
         <v>85</v>
@@ -4755,22 +4737,22 @@
         <v>85</v>
       </c>
       <c r="BU12" s="8" t="s">
-        <v>424</v>
+        <v>312</v>
       </c>
       <c r="BV12" s="8" t="s">
-        <v>409</v>
+        <v>358</v>
       </c>
       <c r="BW12" s="8" t="s">
-        <v>425</v>
+        <v>372</v>
       </c>
       <c r="BX12" s="8" t="s">
         <v>0</v>
       </c>
       <c r="BY12" s="8" t="s">
-        <v>88</v>
+        <v>373</v>
       </c>
       <c r="BZ12" s="8" t="s">
-        <v>88</v>
+        <v>373</v>
       </c>
       <c r="CA12" s="8" t="s">
         <v>88</v>
@@ -4787,10 +4769,10 @@
     </row>
     <row r="13" spans="1:82" s="9" customFormat="1">
       <c r="A13" s="8" t="s">
-        <v>426</v>
+        <v>314</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>0</v>
@@ -4814,16 +4796,16 @@
         <v>86</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>427</v>
+        <v>315</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>405</v>
+        <v>316</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>406</v>
+        <v>317</v>
       </c>
       <c r="M13" s="8" t="s">
-        <v>428</v>
+        <v>318</v>
       </c>
       <c r="N13" s="8" t="s">
         <v>291</v>
@@ -4835,34 +4817,34 @@
         <v>158</v>
       </c>
       <c r="Q13" s="8" t="s">
-        <v>429</v>
+        <v>292</v>
       </c>
       <c r="R13" s="8" t="s">
-        <v>429</v>
+        <v>292</v>
       </c>
       <c r="S13" s="8" t="s">
         <v>293</v>
       </c>
       <c r="T13" s="8" t="s">
-        <v>430</v>
+        <v>319</v>
       </c>
       <c r="U13" s="8" t="s">
-        <v>430</v>
+        <v>319</v>
       </c>
       <c r="V13" s="8" t="s">
         <v>91</v>
       </c>
       <c r="W13" s="8" t="s">
-        <v>431</v>
+        <v>320</v>
       </c>
       <c r="X13" s="8" t="s">
         <v>25</v>
       </c>
       <c r="Y13" s="8" t="s">
-        <v>432</v>
+        <v>321</v>
       </c>
       <c r="Z13" s="8" t="s">
-        <v>433</v>
+        <v>322</v>
       </c>
       <c r="AA13" s="8" t="s">
         <v>88</v>
@@ -4879,8 +4861,8 @@
       <c r="AE13" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="AF13" s="76" t="s">
-        <v>434</v>
+      <c r="AF13" s="8" t="s">
+        <v>85</v>
       </c>
       <c r="AG13" s="8" t="s">
         <v>85</v>
@@ -4898,25 +4880,25 @@
         <v>88</v>
       </c>
       <c r="AL13" s="8" t="s">
-        <v>435</v>
+        <v>323</v>
       </c>
       <c r="AM13" s="8" t="s">
-        <v>436</v>
+        <v>324</v>
       </c>
       <c r="AN13" s="8" t="s">
-        <v>437</v>
+        <v>300</v>
       </c>
       <c r="AO13" s="8" t="s">
         <v>88</v>
       </c>
       <c r="AP13" s="8" t="s">
-        <v>438</v>
+        <v>325</v>
       </c>
       <c r="AQ13" s="8" t="s">
-        <v>439</v>
+        <v>326</v>
       </c>
       <c r="AR13" s="8" t="s">
-        <v>440</v>
+        <v>303</v>
       </c>
       <c r="AS13" s="8" t="s">
         <v>88</v>
@@ -4940,13 +4922,13 @@
         <v>93</v>
       </c>
       <c r="AZ13" s="8" t="s">
-        <v>441</v>
+        <v>304</v>
       </c>
       <c r="BA13" s="8" t="s">
         <v>93</v>
       </c>
       <c r="BB13" s="8" t="s">
-        <v>441</v>
+        <v>304</v>
       </c>
       <c r="BC13" s="8" t="s">
         <v>195</v>
@@ -4961,28 +4943,28 @@
         <v>306</v>
       </c>
       <c r="BG13" s="8" t="s">
-        <v>406</v>
+        <v>531</v>
       </c>
       <c r="BH13" s="8" t="s">
-        <v>442</v>
+        <v>327</v>
       </c>
       <c r="BI13" s="8" t="s">
         <v>25</v>
       </c>
       <c r="BJ13" s="8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="BK13" s="8" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="BL13" s="8" t="s">
-        <v>443</v>
+        <v>328</v>
       </c>
       <c r="BM13" s="8" t="s">
         <v>0</v>
       </c>
       <c r="BN13" s="8" t="s">
-        <v>444</v>
+        <v>329</v>
       </c>
       <c r="BO13" s="8" t="s">
         <v>0</v>
@@ -4994,7 +4976,7 @@
         <v>89</v>
       </c>
       <c r="BR13" s="8" t="s">
-        <v>445</v>
+        <v>330</v>
       </c>
       <c r="BS13" s="8" t="s">
         <v>85</v>
@@ -5003,16 +4985,16 @@
         <v>85</v>
       </c>
       <c r="BU13" s="8" t="s">
-        <v>446</v>
+        <v>312</v>
       </c>
       <c r="BV13" s="8" t="s">
-        <v>431</v>
+        <v>320</v>
       </c>
       <c r="BW13" s="8" t="s">
-        <v>425</v>
+        <v>313</v>
       </c>
       <c r="BX13" s="8" t="s">
-        <v>0</v>
+        <v>91</v>
       </c>
       <c r="BY13" s="8" t="s">
         <v>88</v>
@@ -5035,10 +5017,10 @@
     </row>
     <row r="14" spans="1:82" s="9" customFormat="1">
       <c r="A14" s="8" t="s">
-        <v>447</v>
+        <v>395</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>0</v>
@@ -5062,16 +5044,16 @@
         <v>86</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>448</v>
+        <v>396</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>406</v>
+        <v>532</v>
       </c>
       <c r="M14" s="8" t="s">
-        <v>449</v>
+        <v>399</v>
       </c>
       <c r="N14" s="8" t="s">
         <v>291</v>
@@ -5083,34 +5065,34 @@
         <v>158</v>
       </c>
       <c r="Q14" s="8" t="s">
-        <v>450</v>
+        <v>400</v>
       </c>
       <c r="R14" s="8" t="s">
-        <v>451</v>
+        <v>400</v>
       </c>
       <c r="S14" s="8" t="s">
         <v>293</v>
       </c>
       <c r="T14" s="8" t="s">
-        <v>452</v>
+        <v>159</v>
       </c>
       <c r="U14" s="8" t="s">
-        <v>452</v>
+        <v>159</v>
       </c>
       <c r="V14" s="8" t="s">
         <v>91</v>
       </c>
       <c r="W14" s="8" t="s">
-        <v>453</v>
+        <v>401</v>
       </c>
       <c r="X14" s="8" t="s">
         <v>25</v>
       </c>
       <c r="Y14" s="8" t="s">
-        <v>454</v>
+        <v>402</v>
       </c>
       <c r="Z14" s="8" t="s">
-        <v>455</v>
+        <v>403</v>
       </c>
       <c r="AA14" s="8" t="s">
         <v>88</v>
@@ -5127,8 +5109,8 @@
       <c r="AE14" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="AF14" s="76" t="s">
-        <v>456</v>
+      <c r="AF14" s="8" t="s">
+        <v>85</v>
       </c>
       <c r="AG14" s="8" t="s">
         <v>85</v>
@@ -5146,25 +5128,25 @@
         <v>88</v>
       </c>
       <c r="AL14" s="8" t="s">
-        <v>85</v>
+        <v>404</v>
       </c>
       <c r="AM14" s="8" t="s">
-        <v>88</v>
+        <v>405</v>
       </c>
       <c r="AN14" s="8" t="s">
-        <v>88</v>
+        <v>406</v>
       </c>
       <c r="AO14" s="8" t="s">
         <v>88</v>
       </c>
       <c r="AP14" s="8" t="s">
-        <v>85</v>
+        <v>407</v>
       </c>
       <c r="AQ14" s="8" t="s">
-        <v>88</v>
+        <v>408</v>
       </c>
       <c r="AR14" s="8" t="s">
-        <v>88</v>
+        <v>409</v>
       </c>
       <c r="AS14" s="8" t="s">
         <v>88</v>
@@ -5188,13 +5170,13 @@
         <v>93</v>
       </c>
       <c r="AZ14" s="8" t="s">
-        <v>457</v>
+        <v>410</v>
       </c>
       <c r="BA14" s="8" t="s">
         <v>93</v>
       </c>
       <c r="BB14" s="8" t="s">
-        <v>457</v>
+        <v>410</v>
       </c>
       <c r="BC14" s="8" t="s">
         <v>195</v>
@@ -5209,28 +5191,28 @@
         <v>306</v>
       </c>
       <c r="BG14" s="8" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="BH14" s="8" t="s">
-        <v>458</v>
+        <v>411</v>
       </c>
       <c r="BI14" s="8" t="s">
         <v>25</v>
       </c>
       <c r="BJ14" s="8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="BK14" s="8" t="s">
         <v>0</v>
       </c>
       <c r="BL14" s="8" t="s">
-        <v>459</v>
+        <v>412</v>
       </c>
       <c r="BM14" s="8" t="s">
         <v>0</v>
       </c>
       <c r="BN14" s="8" t="s">
-        <v>460</v>
+        <v>413</v>
       </c>
       <c r="BO14" s="8" t="s">
         <v>0</v>
@@ -5242,7 +5224,7 @@
         <v>89</v>
       </c>
       <c r="BR14" s="8" t="s">
-        <v>461</v>
+        <v>414</v>
       </c>
       <c r="BS14" s="8" t="s">
         <v>85</v>
@@ -5251,22 +5233,22 @@
         <v>85</v>
       </c>
       <c r="BU14" s="8" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="BV14" s="8" t="s">
-        <v>453</v>
+        <v>401</v>
       </c>
       <c r="BW14" s="8" t="s">
-        <v>425</v>
+        <v>416</v>
       </c>
       <c r="BX14" s="8" t="s">
         <v>0</v>
       </c>
       <c r="BY14" s="8" t="s">
-        <v>462</v>
+        <v>88</v>
       </c>
       <c r="BZ14" s="8" t="s">
-        <v>462</v>
+        <v>88</v>
       </c>
       <c r="CA14" s="8" t="s">
         <v>88</v>
@@ -5283,10 +5265,10 @@
     </row>
     <row r="15" spans="1:82" s="9" customFormat="1">
       <c r="A15" s="8" t="s">
-        <v>463</v>
+        <v>286</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>0</v>
@@ -5310,16 +5292,16 @@
         <v>86</v>
       </c>
       <c r="J15" s="8" t="s">
-        <v>464</v>
+        <v>287</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>465</v>
+        <v>288</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>406</v>
+        <v>289</v>
       </c>
       <c r="M15" s="8" t="s">
-        <v>466</v>
+        <v>290</v>
       </c>
       <c r="N15" s="8" t="s">
         <v>291</v>
@@ -5331,43 +5313,43 @@
         <v>158</v>
       </c>
       <c r="Q15" s="8" t="s">
-        <v>467</v>
+        <v>292</v>
       </c>
       <c r="R15" s="8" t="s">
-        <v>467</v>
+        <v>292</v>
       </c>
       <c r="S15" s="8" t="s">
-        <v>468</v>
+        <v>293</v>
       </c>
       <c r="T15" s="8" t="s">
-        <v>469</v>
+        <v>294</v>
       </c>
       <c r="U15" s="8" t="s">
-        <v>469</v>
+        <v>294</v>
       </c>
       <c r="V15" s="8" t="s">
         <v>91</v>
       </c>
       <c r="W15" s="8" t="s">
-        <v>470</v>
+        <v>295</v>
       </c>
       <c r="X15" s="8" t="s">
         <v>25</v>
       </c>
       <c r="Y15" s="8" t="s">
-        <v>471</v>
+        <v>296</v>
       </c>
       <c r="Z15" s="8" t="s">
-        <v>472</v>
+        <v>297</v>
       </c>
       <c r="AA15" s="8" t="s">
         <v>88</v>
       </c>
       <c r="AB15" s="8" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="AC15" s="8" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="AD15" s="8" t="s">
         <v>88</v>
@@ -5375,29 +5357,29 @@
       <c r="AE15" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="AF15" s="76" t="s">
-        <v>473</v>
+      <c r="AF15" s="8" t="s">
+        <v>85</v>
       </c>
       <c r="AG15" s="8" t="s">
-        <v>474</v>
+        <v>85</v>
       </c>
       <c r="AH15" s="8" t="s">
         <v>85</v>
       </c>
       <c r="AI15" s="8" t="s">
-        <v>475</v>
+        <v>88</v>
       </c>
       <c r="AJ15" s="8" t="s">
-        <v>476</v>
+        <v>88</v>
       </c>
       <c r="AK15" s="8" t="s">
         <v>88</v>
       </c>
       <c r="AL15" s="8" t="s">
-        <v>477</v>
+        <v>298</v>
       </c>
       <c r="AM15" s="8" t="s">
-        <v>478</v>
+        <v>299</v>
       </c>
       <c r="AN15" s="8" t="s">
         <v>300</v>
@@ -5406,10 +5388,10 @@
         <v>88</v>
       </c>
       <c r="AP15" s="8" t="s">
-        <v>479</v>
+        <v>301</v>
       </c>
       <c r="AQ15" s="8" t="s">
-        <v>480</v>
+        <v>302</v>
       </c>
       <c r="AR15" s="8" t="s">
         <v>303</v>
@@ -5436,19 +5418,19 @@
         <v>93</v>
       </c>
       <c r="AZ15" s="8" t="s">
-        <v>481</v>
+        <v>304</v>
       </c>
       <c r="BA15" s="8" t="s">
         <v>93</v>
       </c>
       <c r="BB15" s="8" t="s">
-        <v>481</v>
+        <v>304</v>
       </c>
       <c r="BC15" s="8" t="s">
-        <v>482</v>
+        <v>195</v>
       </c>
       <c r="BD15" s="8" t="s">
-        <v>482</v>
+        <v>195</v>
       </c>
       <c r="BE15" s="8" t="s">
         <v>305</v>
@@ -5457,28 +5439,28 @@
         <v>306</v>
       </c>
       <c r="BG15" s="8" t="s">
-        <v>406</v>
+        <v>533</v>
       </c>
       <c r="BH15" s="8" t="s">
-        <v>483</v>
+        <v>307</v>
       </c>
       <c r="BI15" s="8" t="s">
         <v>25</v>
       </c>
       <c r="BJ15" s="8" t="s">
-        <v>484</v>
+        <v>308</v>
       </c>
       <c r="BK15" s="8" t="s">
         <v>0</v>
       </c>
       <c r="BL15" s="8" t="s">
-        <v>485</v>
+        <v>309</v>
       </c>
       <c r="BM15" s="8" t="s">
         <v>0</v>
       </c>
       <c r="BN15" s="8" t="s">
-        <v>486</v>
+        <v>310</v>
       </c>
       <c r="BO15" s="8" t="s">
         <v>0</v>
@@ -5490,7 +5472,7 @@
         <v>89</v>
       </c>
       <c r="BR15" s="8" t="s">
-        <v>487</v>
+        <v>311</v>
       </c>
       <c r="BS15" s="8" t="s">
         <v>85</v>
@@ -5499,13 +5481,13 @@
         <v>85</v>
       </c>
       <c r="BU15" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="BV15" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="BW15" s="8" t="s">
         <v>313</v>
-      </c>
-      <c r="BV15" s="8" t="s">
-        <v>470</v>
-      </c>
-      <c r="BW15" s="8" t="s">
-        <v>488</v>
       </c>
       <c r="BX15" s="8" t="s">
         <v>0</v>
@@ -5531,10 +5513,10 @@
     </row>
     <row r="16" spans="1:82" s="9" customFormat="1">
       <c r="A16" s="8" t="s">
-        <v>489</v>
+        <v>478</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>0</v>
@@ -5558,16 +5540,16 @@
         <v>86</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>490</v>
+        <v>479</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>465</v>
+        <v>454</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>406</v>
+        <v>534</v>
       </c>
       <c r="M16" s="8" t="s">
-        <v>491</v>
+        <v>480</v>
       </c>
       <c r="N16" s="8" t="s">
         <v>291</v>
@@ -5579,34 +5561,34 @@
         <v>158</v>
       </c>
       <c r="Q16" s="8" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="R16" s="8" t="s">
-        <v>492</v>
+        <v>481</v>
       </c>
       <c r="S16" s="8" t="s">
         <v>293</v>
       </c>
       <c r="T16" s="8" t="s">
-        <v>493</v>
+        <v>482</v>
       </c>
       <c r="U16" s="8" t="s">
-        <v>493</v>
+        <v>482</v>
       </c>
       <c r="V16" s="8" t="s">
         <v>91</v>
       </c>
       <c r="W16" s="8" t="s">
-        <v>494</v>
+        <v>483</v>
       </c>
       <c r="X16" s="8" t="s">
         <v>25</v>
       </c>
       <c r="Y16" s="8" t="s">
-        <v>495</v>
+        <v>484</v>
       </c>
       <c r="Z16" s="8" t="s">
-        <v>496</v>
+        <v>485</v>
       </c>
       <c r="AA16" s="8" t="s">
         <v>88</v>
@@ -5623,8 +5605,8 @@
       <c r="AE16" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="AF16" s="76" t="s">
-        <v>497</v>
+      <c r="AF16" s="8" t="s">
+        <v>85</v>
       </c>
       <c r="AG16" s="8" t="s">
         <v>85</v>
@@ -5642,25 +5624,25 @@
         <v>88</v>
       </c>
       <c r="AL16" s="8" t="s">
-        <v>498</v>
+        <v>486</v>
       </c>
       <c r="AM16" s="8" t="s">
-        <v>499</v>
+        <v>487</v>
       </c>
       <c r="AN16" s="8" t="s">
-        <v>415</v>
+        <v>406</v>
       </c>
       <c r="AO16" s="8" t="s">
         <v>88</v>
       </c>
       <c r="AP16" s="8" t="s">
-        <v>500</v>
+        <v>488</v>
       </c>
       <c r="AQ16" s="8" t="s">
-        <v>501</v>
+        <v>489</v>
       </c>
       <c r="AR16" s="8" t="s">
-        <v>418</v>
+        <v>409</v>
       </c>
       <c r="AS16" s="8" t="s">
         <v>88</v>
@@ -5684,19 +5666,19 @@
         <v>93</v>
       </c>
       <c r="AZ16" s="8" t="s">
-        <v>502</v>
+        <v>490</v>
       </c>
       <c r="BA16" s="8" t="s">
         <v>93</v>
       </c>
       <c r="BB16" s="8" t="s">
-        <v>502</v>
+        <v>490</v>
       </c>
       <c r="BC16" s="8" t="s">
-        <v>503</v>
+        <v>491</v>
       </c>
       <c r="BD16" s="8" t="s">
-        <v>503</v>
+        <v>491</v>
       </c>
       <c r="BE16" s="8" t="s">
         <v>305</v>
@@ -5705,28 +5687,28 @@
         <v>306</v>
       </c>
       <c r="BG16" s="8" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="BH16" s="8" t="s">
-        <v>504</v>
+        <v>492</v>
       </c>
       <c r="BI16" s="8" t="s">
         <v>25</v>
       </c>
       <c r="BJ16" s="8" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="BK16" s="8" t="s">
         <v>0</v>
       </c>
       <c r="BL16" s="8" t="s">
-        <v>505</v>
+        <v>493</v>
       </c>
       <c r="BM16" s="8" t="s">
         <v>0</v>
       </c>
       <c r="BN16" s="8" t="s">
-        <v>506</v>
+        <v>494</v>
       </c>
       <c r="BO16" s="8" t="s">
         <v>0</v>
@@ -5738,7 +5720,7 @@
         <v>89</v>
       </c>
       <c r="BR16" s="8" t="s">
-        <v>507</v>
+        <v>495</v>
       </c>
       <c r="BS16" s="8" t="s">
         <v>85</v>
@@ -5747,13 +5729,13 @@
         <v>85</v>
       </c>
       <c r="BU16" s="8" t="s">
-        <v>424</v>
+        <v>415</v>
       </c>
       <c r="BV16" s="8" t="s">
-        <v>494</v>
+        <v>483</v>
       </c>
       <c r="BW16" s="8" t="s">
-        <v>425</v>
+        <v>416</v>
       </c>
       <c r="BX16" s="8" t="s">
         <v>0</v>
@@ -5778,83 +5760,83 @@
       </c>
     </row>
     <row r="18" spans="1:82" ht="15" customHeight="1">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="60" t="s">
         <v>213</v>
       </c>
-      <c r="B18" s="35"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="35"/>
-      <c r="L18" s="35"/>
-      <c r="M18" s="35"/>
-      <c r="N18" s="35"/>
-      <c r="O18" s="35"/>
-      <c r="P18" s="35"/>
-      <c r="Q18" s="35"/>
-      <c r="R18" s="35"/>
-      <c r="S18" s="35"/>
-      <c r="T18" s="35"/>
-      <c r="U18" s="35"/>
-      <c r="V18" s="35"/>
-      <c r="W18" s="35"/>
-      <c r="X18" s="35"/>
-      <c r="Y18" s="35"/>
-      <c r="Z18" s="35"/>
-      <c r="AA18" s="35"/>
-      <c r="AB18" s="35"/>
-      <c r="AC18" s="35"/>
-      <c r="AD18" s="35"/>
-      <c r="AE18" s="35"/>
-      <c r="AF18" s="35"/>
-      <c r="AG18" s="35"/>
-      <c r="AH18" s="35"/>
-      <c r="AI18" s="35"/>
-      <c r="AJ18" s="35"/>
-      <c r="AK18" s="35"/>
-      <c r="AL18" s="35"/>
-      <c r="AM18" s="35"/>
-      <c r="AN18" s="35"/>
-      <c r="AO18" s="35"/>
-      <c r="AP18" s="35"/>
-      <c r="AQ18" s="35"/>
-      <c r="AR18" s="35"/>
-      <c r="AS18" s="35"/>
-      <c r="AT18" s="35"/>
-      <c r="AU18" s="35"/>
-      <c r="AV18" s="35"/>
-      <c r="AW18" s="35"/>
-      <c r="AX18" s="36"/>
-      <c r="AY18" s="34" t="s">
+      <c r="B18" s="61"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="61"/>
+      <c r="F18" s="61"/>
+      <c r="G18" s="61"/>
+      <c r="H18" s="61"/>
+      <c r="I18" s="61"/>
+      <c r="J18" s="61"/>
+      <c r="K18" s="61"/>
+      <c r="L18" s="61"/>
+      <c r="M18" s="61"/>
+      <c r="N18" s="61"/>
+      <c r="O18" s="61"/>
+      <c r="P18" s="61"/>
+      <c r="Q18" s="61"/>
+      <c r="R18" s="61"/>
+      <c r="S18" s="61"/>
+      <c r="T18" s="61"/>
+      <c r="U18" s="61"/>
+      <c r="V18" s="61"/>
+      <c r="W18" s="61"/>
+      <c r="X18" s="61"/>
+      <c r="Y18" s="61"/>
+      <c r="Z18" s="61"/>
+      <c r="AA18" s="61"/>
+      <c r="AB18" s="61"/>
+      <c r="AC18" s="61"/>
+      <c r="AD18" s="61"/>
+      <c r="AE18" s="61"/>
+      <c r="AF18" s="61"/>
+      <c r="AG18" s="61"/>
+      <c r="AH18" s="61"/>
+      <c r="AI18" s="61"/>
+      <c r="AJ18" s="61"/>
+      <c r="AK18" s="61"/>
+      <c r="AL18" s="61"/>
+      <c r="AM18" s="61"/>
+      <c r="AN18" s="61"/>
+      <c r="AO18" s="61"/>
+      <c r="AP18" s="61"/>
+      <c r="AQ18" s="61"/>
+      <c r="AR18" s="61"/>
+      <c r="AS18" s="61"/>
+      <c r="AT18" s="61"/>
+      <c r="AU18" s="61"/>
+      <c r="AV18" s="61"/>
+      <c r="AW18" s="61"/>
+      <c r="AX18" s="62"/>
+      <c r="AY18" s="60" t="s">
         <v>244</v>
       </c>
-      <c r="AZ18" s="35"/>
-      <c r="BA18" s="35"/>
-      <c r="BB18" s="35"/>
-      <c r="BC18" s="35"/>
-      <c r="BD18" s="36"/>
-      <c r="BE18" s="51" t="s">
+      <c r="AZ18" s="61"/>
+      <c r="BA18" s="61"/>
+      <c r="BB18" s="61"/>
+      <c r="BC18" s="61"/>
+      <c r="BD18" s="62"/>
+      <c r="BE18" s="57" t="s">
         <v>247</v>
       </c>
-      <c r="BF18" s="51" t="s">
+      <c r="BF18" s="57" t="s">
         <v>248</v>
       </c>
-      <c r="BG18" s="51" t="s">
+      <c r="BG18" s="57" t="s">
         <v>245</v>
       </c>
-      <c r="BH18" s="51" t="s">
+      <c r="BH18" s="57" t="s">
         <v>254</v>
       </c>
-      <c r="BI18" s="54" t="s">
+      <c r="BI18" s="69" t="s">
         <v>249</v>
       </c>
-      <c r="BJ18" s="54"/>
-      <c r="BK18" s="51" t="s">
+      <c r="BJ18" s="69"/>
+      <c r="BK18" s="57" t="s">
         <v>250</v>
       </c>
       <c r="BL18" s="20" t="s">
@@ -5862,191 +5844,191 @@
       </c>
       <c r="BM18" s="21"/>
       <c r="BN18" s="22"/>
-      <c r="BO18" s="33" t="s">
+      <c r="BO18" s="70" t="s">
         <v>252</v>
       </c>
-      <c r="BP18" s="33"/>
-      <c r="BQ18" s="33"/>
-      <c r="BR18" s="33"/>
-      <c r="BS18" s="33"/>
-      <c r="BT18" s="33"/>
-      <c r="BU18" s="33"/>
-      <c r="BV18" s="33"/>
-      <c r="BW18" s="33"/>
-      <c r="BX18" s="33"/>
-      <c r="BY18" s="33"/>
-      <c r="BZ18" s="33"/>
-      <c r="CA18" s="33"/>
-      <c r="CB18" s="67" t="s">
-        <v>514</v>
-      </c>
-      <c r="CC18" s="68"/>
+      <c r="BP18" s="70"/>
+      <c r="BQ18" s="70"/>
+      <c r="BR18" s="70"/>
+      <c r="BS18" s="70"/>
+      <c r="BT18" s="70"/>
+      <c r="BU18" s="70"/>
+      <c r="BV18" s="70"/>
+      <c r="BW18" s="70"/>
+      <c r="BX18" s="70"/>
+      <c r="BY18" s="70"/>
+      <c r="BZ18" s="70"/>
+      <c r="CA18" s="70"/>
+      <c r="CB18" s="39" t="s">
+        <v>502</v>
+      </c>
+      <c r="CC18" s="40"/>
     </row>
     <row r="19" spans="1:82" ht="11.25" customHeight="1">
-      <c r="A19" s="37"/>
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="38"/>
-      <c r="J19" s="38"/>
-      <c r="K19" s="38"/>
-      <c r="L19" s="38"/>
-      <c r="M19" s="38"/>
-      <c r="N19" s="38"/>
-      <c r="O19" s="38"/>
-      <c r="P19" s="38"/>
-      <c r="Q19" s="38"/>
-      <c r="R19" s="38"/>
-      <c r="S19" s="38"/>
-      <c r="T19" s="38"/>
-      <c r="U19" s="38"/>
-      <c r="V19" s="38"/>
-      <c r="W19" s="38"/>
-      <c r="X19" s="38"/>
-      <c r="Y19" s="38"/>
-      <c r="Z19" s="38"/>
-      <c r="AA19" s="38"/>
-      <c r="AB19" s="38"/>
-      <c r="AC19" s="38"/>
-      <c r="AD19" s="38"/>
-      <c r="AE19" s="38"/>
-      <c r="AF19" s="38"/>
-      <c r="AG19" s="38"/>
-      <c r="AH19" s="38"/>
-      <c r="AI19" s="38"/>
-      <c r="AJ19" s="38"/>
-      <c r="AK19" s="38"/>
-      <c r="AL19" s="38"/>
-      <c r="AM19" s="38"/>
-      <c r="AN19" s="38"/>
-      <c r="AO19" s="38"/>
-      <c r="AP19" s="38"/>
-      <c r="AQ19" s="38"/>
-      <c r="AR19" s="38"/>
-      <c r="AS19" s="38"/>
-      <c r="AT19" s="38"/>
-      <c r="AU19" s="38"/>
-      <c r="AV19" s="38"/>
-      <c r="AW19" s="38"/>
-      <c r="AX19" s="39"/>
-      <c r="AY19" s="37"/>
-      <c r="AZ19" s="38"/>
-      <c r="BA19" s="38"/>
-      <c r="BB19" s="38"/>
-      <c r="BC19" s="38"/>
-      <c r="BD19" s="39"/>
-      <c r="BE19" s="52"/>
-      <c r="BF19" s="52"/>
-      <c r="BG19" s="52"/>
-      <c r="BH19" s="52"/>
-      <c r="BI19" s="54"/>
-      <c r="BJ19" s="54"/>
-      <c r="BK19" s="52"/>
+      <c r="A19" s="63"/>
+      <c r="B19" s="64"/>
+      <c r="C19" s="64"/>
+      <c r="D19" s="64"/>
+      <c r="E19" s="64"/>
+      <c r="F19" s="64"/>
+      <c r="G19" s="64"/>
+      <c r="H19" s="64"/>
+      <c r="I19" s="64"/>
+      <c r="J19" s="64"/>
+      <c r="K19" s="64"/>
+      <c r="L19" s="64"/>
+      <c r="M19" s="64"/>
+      <c r="N19" s="64"/>
+      <c r="O19" s="64"/>
+      <c r="P19" s="64"/>
+      <c r="Q19" s="64"/>
+      <c r="R19" s="64"/>
+      <c r="S19" s="64"/>
+      <c r="T19" s="64"/>
+      <c r="U19" s="64"/>
+      <c r="V19" s="64"/>
+      <c r="W19" s="64"/>
+      <c r="X19" s="64"/>
+      <c r="Y19" s="64"/>
+      <c r="Z19" s="64"/>
+      <c r="AA19" s="64"/>
+      <c r="AB19" s="64"/>
+      <c r="AC19" s="64"/>
+      <c r="AD19" s="64"/>
+      <c r="AE19" s="64"/>
+      <c r="AF19" s="64"/>
+      <c r="AG19" s="64"/>
+      <c r="AH19" s="64"/>
+      <c r="AI19" s="64"/>
+      <c r="AJ19" s="64"/>
+      <c r="AK19" s="64"/>
+      <c r="AL19" s="64"/>
+      <c r="AM19" s="64"/>
+      <c r="AN19" s="64"/>
+      <c r="AO19" s="64"/>
+      <c r="AP19" s="64"/>
+      <c r="AQ19" s="64"/>
+      <c r="AR19" s="64"/>
+      <c r="AS19" s="64"/>
+      <c r="AT19" s="64"/>
+      <c r="AU19" s="64"/>
+      <c r="AV19" s="64"/>
+      <c r="AW19" s="64"/>
+      <c r="AX19" s="65"/>
+      <c r="AY19" s="63"/>
+      <c r="AZ19" s="64"/>
+      <c r="BA19" s="64"/>
+      <c r="BB19" s="64"/>
+      <c r="BC19" s="64"/>
+      <c r="BD19" s="65"/>
+      <c r="BE19" s="58"/>
+      <c r="BF19" s="58"/>
+      <c r="BG19" s="58"/>
+      <c r="BH19" s="58"/>
+      <c r="BI19" s="69"/>
+      <c r="BJ19" s="69"/>
+      <c r="BK19" s="58"/>
       <c r="BL19" s="23"/>
       <c r="BM19" s="24"/>
       <c r="BN19" s="25"/>
-      <c r="BO19" s="33"/>
-      <c r="BP19" s="33"/>
-      <c r="BQ19" s="33"/>
-      <c r="BR19" s="33"/>
-      <c r="BS19" s="33"/>
-      <c r="BT19" s="33"/>
-      <c r="BU19" s="33"/>
-      <c r="BV19" s="33"/>
-      <c r="BW19" s="33"/>
-      <c r="BX19" s="33"/>
-      <c r="BY19" s="33"/>
-      <c r="BZ19" s="33"/>
-      <c r="CA19" s="33"/>
-      <c r="CB19" s="69"/>
-      <c r="CC19" s="70"/>
+      <c r="BO19" s="70"/>
+      <c r="BP19" s="70"/>
+      <c r="BQ19" s="70"/>
+      <c r="BR19" s="70"/>
+      <c r="BS19" s="70"/>
+      <c r="BT19" s="70"/>
+      <c r="BU19" s="70"/>
+      <c r="BV19" s="70"/>
+      <c r="BW19" s="70"/>
+      <c r="BX19" s="70"/>
+      <c r="BY19" s="70"/>
+      <c r="BZ19" s="70"/>
+      <c r="CA19" s="70"/>
+      <c r="CB19" s="41"/>
+      <c r="CC19" s="42"/>
     </row>
     <row r="20" spans="1:82" ht="11.25" customHeight="1">
-      <c r="A20" s="40"/>
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="41"/>
-      <c r="H20" s="41"/>
-      <c r="I20" s="41"/>
-      <c r="J20" s="41"/>
-      <c r="K20" s="41"/>
-      <c r="L20" s="41"/>
-      <c r="M20" s="41"/>
-      <c r="N20" s="41"/>
-      <c r="O20" s="41"/>
-      <c r="P20" s="41"/>
-      <c r="Q20" s="41"/>
-      <c r="R20" s="41"/>
-      <c r="S20" s="41"/>
-      <c r="T20" s="41"/>
-      <c r="U20" s="41"/>
-      <c r="V20" s="41"/>
-      <c r="W20" s="41"/>
-      <c r="X20" s="41"/>
-      <c r="Y20" s="41"/>
-      <c r="Z20" s="41"/>
-      <c r="AA20" s="41"/>
-      <c r="AB20" s="41"/>
-      <c r="AC20" s="41"/>
-      <c r="AD20" s="41"/>
-      <c r="AE20" s="41"/>
-      <c r="AF20" s="41"/>
-      <c r="AG20" s="41"/>
-      <c r="AH20" s="41"/>
-      <c r="AI20" s="41"/>
-      <c r="AJ20" s="41"/>
-      <c r="AK20" s="41"/>
-      <c r="AL20" s="41"/>
-      <c r="AM20" s="41"/>
-      <c r="AN20" s="41"/>
-      <c r="AO20" s="41"/>
-      <c r="AP20" s="41"/>
-      <c r="AQ20" s="41"/>
-      <c r="AR20" s="41"/>
-      <c r="AS20" s="41"/>
-      <c r="AT20" s="41"/>
-      <c r="AU20" s="41"/>
-      <c r="AV20" s="41"/>
-      <c r="AW20" s="41"/>
-      <c r="AX20" s="42"/>
-      <c r="AY20" s="40"/>
-      <c r="AZ20" s="41"/>
-      <c r="BA20" s="41"/>
-      <c r="BB20" s="41"/>
-      <c r="BC20" s="41"/>
-      <c r="BD20" s="42"/>
-      <c r="BE20" s="53"/>
-      <c r="BF20" s="53"/>
-      <c r="BG20" s="53"/>
-      <c r="BH20" s="53"/>
-      <c r="BI20" s="54"/>
-      <c r="BJ20" s="54"/>
-      <c r="BK20" s="53"/>
+      <c r="A20" s="66"/>
+      <c r="B20" s="67"/>
+      <c r="C20" s="67"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="67"/>
+      <c r="G20" s="67"/>
+      <c r="H20" s="67"/>
+      <c r="I20" s="67"/>
+      <c r="J20" s="67"/>
+      <c r="K20" s="67"/>
+      <c r="L20" s="67"/>
+      <c r="M20" s="67"/>
+      <c r="N20" s="67"/>
+      <c r="O20" s="67"/>
+      <c r="P20" s="67"/>
+      <c r="Q20" s="67"/>
+      <c r="R20" s="67"/>
+      <c r="S20" s="67"/>
+      <c r="T20" s="67"/>
+      <c r="U20" s="67"/>
+      <c r="V20" s="67"/>
+      <c r="W20" s="67"/>
+      <c r="X20" s="67"/>
+      <c r="Y20" s="67"/>
+      <c r="Z20" s="67"/>
+      <c r="AA20" s="67"/>
+      <c r="AB20" s="67"/>
+      <c r="AC20" s="67"/>
+      <c r="AD20" s="67"/>
+      <c r="AE20" s="67"/>
+      <c r="AF20" s="67"/>
+      <c r="AG20" s="67"/>
+      <c r="AH20" s="67"/>
+      <c r="AI20" s="67"/>
+      <c r="AJ20" s="67"/>
+      <c r="AK20" s="67"/>
+      <c r="AL20" s="67"/>
+      <c r="AM20" s="67"/>
+      <c r="AN20" s="67"/>
+      <c r="AO20" s="67"/>
+      <c r="AP20" s="67"/>
+      <c r="AQ20" s="67"/>
+      <c r="AR20" s="67"/>
+      <c r="AS20" s="67"/>
+      <c r="AT20" s="67"/>
+      <c r="AU20" s="67"/>
+      <c r="AV20" s="67"/>
+      <c r="AW20" s="67"/>
+      <c r="AX20" s="68"/>
+      <c r="AY20" s="66"/>
+      <c r="AZ20" s="67"/>
+      <c r="BA20" s="67"/>
+      <c r="BB20" s="67"/>
+      <c r="BC20" s="67"/>
+      <c r="BD20" s="68"/>
+      <c r="BE20" s="59"/>
+      <c r="BF20" s="59"/>
+      <c r="BG20" s="59"/>
+      <c r="BH20" s="59"/>
+      <c r="BI20" s="69"/>
+      <c r="BJ20" s="69"/>
+      <c r="BK20" s="59"/>
       <c r="BL20" s="26"/>
       <c r="BM20" s="27"/>
       <c r="BN20" s="28"/>
-      <c r="BO20" s="33"/>
-      <c r="BP20" s="33"/>
-      <c r="BQ20" s="33"/>
-      <c r="BR20" s="33"/>
-      <c r="BS20" s="33"/>
-      <c r="BT20" s="33"/>
-      <c r="BU20" s="33"/>
-      <c r="BV20" s="33"/>
-      <c r="BW20" s="33"/>
-      <c r="BX20" s="33"/>
-      <c r="BY20" s="33"/>
-      <c r="BZ20" s="33"/>
-      <c r="CA20" s="33"/>
-      <c r="CB20" s="71"/>
-      <c r="CC20" s="72"/>
+      <c r="BO20" s="70"/>
+      <c r="BP20" s="70"/>
+      <c r="BQ20" s="70"/>
+      <c r="BR20" s="70"/>
+      <c r="BS20" s="70"/>
+      <c r="BT20" s="70"/>
+      <c r="BU20" s="70"/>
+      <c r="BV20" s="70"/>
+      <c r="BW20" s="70"/>
+      <c r="BX20" s="70"/>
+      <c r="BY20" s="70"/>
+      <c r="BZ20" s="70"/>
+      <c r="CA20" s="70"/>
+      <c r="CB20" s="43"/>
+      <c r="CC20" s="44"/>
     </row>
     <row r="21" spans="1:82" ht="11.25" customHeight="1">
       <c r="A21" s="29" t="s">
@@ -6064,25 +6046,25 @@
       <c r="E21" s="55" t="s">
         <v>221</v>
       </c>
-      <c r="F21" s="43" t="s">
+      <c r="F21" s="71" t="s">
         <v>236</v>
       </c>
-      <c r="G21" s="46" t="s">
+      <c r="G21" s="74" t="s">
         <v>237</v>
       </c>
-      <c r="H21" s="43" t="s">
+      <c r="H21" s="71" t="s">
         <v>238</v>
       </c>
-      <c r="I21" s="46" t="s">
+      <c r="I21" s="74" t="s">
         <v>239</v>
       </c>
-      <c r="J21" s="30" t="s">
+      <c r="J21" s="33" t="s">
         <v>152</v>
       </c>
-      <c r="K21" s="30" t="s">
+      <c r="K21" s="33" t="s">
         <v>214</v>
       </c>
-      <c r="L21" s="30" t="s">
+      <c r="L21" s="33" t="s">
         <v>150</v>
       </c>
       <c r="M21" s="29" t="s">
@@ -6103,7 +6085,7 @@
       <c r="R21" s="29" t="s">
         <v>147</v>
       </c>
-      <c r="S21" s="48" t="s">
+      <c r="S21" s="30" t="s">
         <v>183</v>
       </c>
       <c r="T21" s="29" t="s">
@@ -6115,125 +6097,125 @@
       <c r="V21" s="29" t="s">
         <v>172</v>
       </c>
-      <c r="W21" s="30" t="s">
+      <c r="W21" s="33" t="s">
         <v>156</v>
       </c>
-      <c r="X21" s="30" t="s">
+      <c r="X21" s="33" t="s">
         <v>215</v>
       </c>
-      <c r="Y21" s="30" t="s">
+      <c r="Y21" s="33" t="s">
         <v>166</v>
       </c>
-      <c r="Z21" s="30" t="s">
+      <c r="Z21" s="33" t="s">
         <v>216</v>
       </c>
-      <c r="AA21" s="30" t="s">
+      <c r="AA21" s="33" t="s">
         <v>165</v>
       </c>
-      <c r="AB21" s="48" t="s">
+      <c r="AB21" s="30" t="s">
         <v>173</v>
       </c>
-      <c r="AC21" s="48" t="s">
+      <c r="AC21" s="30" t="s">
         <v>174</v>
       </c>
-      <c r="AD21" s="48" t="s">
+      <c r="AD21" s="30" t="s">
         <v>167</v>
       </c>
-      <c r="AE21" s="48" t="s">
+      <c r="AE21" s="30" t="s">
         <v>168</v>
       </c>
-      <c r="AF21" s="48" t="s">
+      <c r="AF21" s="30" t="s">
         <v>177</v>
       </c>
-      <c r="AG21" s="30" t="s">
+      <c r="AG21" s="33" t="s">
         <v>160</v>
       </c>
-      <c r="AH21" s="48" t="s">
+      <c r="AH21" s="30" t="s">
         <v>163</v>
       </c>
-      <c r="AI21" s="48" t="s">
+      <c r="AI21" s="30" t="s">
         <v>224</v>
       </c>
-      <c r="AJ21" s="58" t="s">
+      <c r="AJ21" s="49" t="s">
         <v>225</v>
       </c>
-      <c r="AK21" s="56" t="s">
+      <c r="AK21" s="48" t="s">
         <v>228</v>
       </c>
-      <c r="AL21" s="61" t="s">
+      <c r="AL21" s="52" t="s">
         <v>161</v>
       </c>
-      <c r="AM21" s="48" t="s">
+      <c r="AM21" s="30" t="s">
         <v>226</v>
       </c>
-      <c r="AN21" s="58" t="s">
+      <c r="AN21" s="49" t="s">
         <v>227</v>
       </c>
-      <c r="AO21" s="56" t="s">
+      <c r="AO21" s="48" t="s">
         <v>229</v>
       </c>
-      <c r="AP21" s="61" t="s">
+      <c r="AP21" s="52" t="s">
         <v>162</v>
       </c>
-      <c r="AQ21" s="48" t="s">
+      <c r="AQ21" s="30" t="s">
         <v>233</v>
       </c>
-      <c r="AR21" s="58" t="s">
+      <c r="AR21" s="49" t="s">
         <v>230</v>
       </c>
-      <c r="AS21" s="56" t="s">
+      <c r="AS21" s="48" t="s">
         <v>231</v>
       </c>
-      <c r="AT21" s="48" t="s">
+      <c r="AT21" s="30" t="s">
         <v>164</v>
       </c>
-      <c r="AU21" s="48" t="s">
+      <c r="AU21" s="30" t="s">
         <v>232</v>
       </c>
-      <c r="AV21" s="58" t="s">
+      <c r="AV21" s="49" t="s">
         <v>234</v>
       </c>
-      <c r="AW21" s="56" t="s">
+      <c r="AW21" s="48" t="s">
         <v>235</v>
       </c>
-      <c r="AX21" s="58" t="s">
+      <c r="AX21" s="49" t="s">
         <v>178</v>
       </c>
-      <c r="AY21" s="56" t="s">
+      <c r="AY21" s="48" t="s">
         <v>242</v>
       </c>
-      <c r="AZ21" s="57" t="s">
+      <c r="AZ21" s="56" t="s">
         <v>240</v>
       </c>
-      <c r="BA21" s="56" t="s">
+      <c r="BA21" s="48" t="s">
         <v>243</v>
       </c>
-      <c r="BB21" s="56" t="s">
+      <c r="BB21" s="48" t="s">
         <v>241</v>
       </c>
-      <c r="BC21" s="56" t="s">
+      <c r="BC21" s="48" t="s">
         <v>190</v>
       </c>
-      <c r="BD21" s="56" t="s">
+      <c r="BD21" s="48" t="s">
         <v>191</v>
       </c>
-      <c r="BE21" s="73" t="s">
+      <c r="BE21" s="45" t="s">
         <v>192</v>
       </c>
-      <c r="BF21" s="48" t="s">
+      <c r="BF21" s="30" t="s">
         <v>151</v>
       </c>
-      <c r="BG21" s="48" t="s">
+      <c r="BG21" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="BH21" s="56" t="s">
-        <v>509</v>
-      </c>
-      <c r="BI21" s="56" t="s">
-        <v>510</v>
-      </c>
-      <c r="BJ21" s="56" t="s">
-        <v>511</v>
+      <c r="BH21" s="48" t="s">
+        <v>497</v>
+      </c>
+      <c r="BI21" s="48" t="s">
+        <v>498</v>
+      </c>
+      <c r="BJ21" s="48" t="s">
+        <v>499</v>
       </c>
       <c r="BK21" s="29" t="s">
         <v>188</v>
@@ -6247,53 +6229,53 @@
       <c r="BN21" s="29" t="s">
         <v>155</v>
       </c>
-      <c r="BO21" s="48" t="s">
-        <v>512</v>
-      </c>
-      <c r="BP21" s="48" t="s">
+      <c r="BO21" s="30" t="s">
+        <v>500</v>
+      </c>
+      <c r="BP21" s="30" t="s">
         <v>171</v>
       </c>
-      <c r="BQ21" s="48" t="s">
+      <c r="BQ21" s="30" t="s">
         <v>170</v>
       </c>
-      <c r="BR21" s="48" t="s">
-        <v>513</v>
-      </c>
-      <c r="BS21" s="48" t="s">
+      <c r="BR21" s="30" t="s">
+        <v>501</v>
+      </c>
+      <c r="BS21" s="30" t="s">
         <v>181</v>
       </c>
-      <c r="BT21" s="48" t="s">
+      <c r="BT21" s="30" t="s">
         <v>175</v>
       </c>
-      <c r="BU21" s="48" t="s">
+      <c r="BU21" s="30" t="s">
         <v>169</v>
       </c>
-      <c r="BV21" s="48" t="s">
+      <c r="BV21" s="30" t="s">
         <v>182</v>
       </c>
-      <c r="BW21" s="48" t="s">
+      <c r="BW21" s="30" t="s">
         <v>184</v>
       </c>
-      <c r="BX21" s="48" t="s">
+      <c r="BX21" s="30" t="s">
         <v>176</v>
       </c>
-      <c r="BY21" s="48" t="s">
+      <c r="BY21" s="30" t="s">
         <v>179</v>
       </c>
-      <c r="BZ21" s="48" t="s">
+      <c r="BZ21" s="30" t="s">
         <v>179</v>
       </c>
-      <c r="CA21" s="48" t="s">
+      <c r="CA21" s="30" t="s">
         <v>180</v>
       </c>
-      <c r="CB21" s="48" t="s">
-        <v>515</v>
-      </c>
-      <c r="CC21" s="48" t="s">
-        <v>515</v>
-      </c>
-      <c r="CD21" s="48" t="s">
-        <v>537</v>
+      <c r="CB21" s="30" t="s">
+        <v>503</v>
+      </c>
+      <c r="CC21" s="30" t="s">
+        <v>503</v>
+      </c>
+      <c r="CD21" s="30" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="22" spans="1:82">
@@ -6302,83 +6284,83 @@
       <c r="C22" s="29"/>
       <c r="D22" s="29"/>
       <c r="E22" s="55"/>
-      <c r="F22" s="44"/>
-      <c r="G22" s="46"/>
-      <c r="H22" s="44"/>
-      <c r="I22" s="46"/>
-      <c r="J22" s="31"/>
-      <c r="K22" s="31"/>
-      <c r="L22" s="31"/>
+      <c r="F22" s="72"/>
+      <c r="G22" s="74"/>
+      <c r="H22" s="72"/>
+      <c r="I22" s="74"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="34"/>
+      <c r="L22" s="34"/>
       <c r="M22" s="29"/>
       <c r="N22" s="29"/>
       <c r="O22" s="29"/>
       <c r="P22" s="29"/>
       <c r="Q22" s="29"/>
       <c r="R22" s="29"/>
-      <c r="S22" s="49"/>
+      <c r="S22" s="31"/>
       <c r="T22" s="29"/>
       <c r="U22" s="29"/>
       <c r="V22" s="29"/>
-      <c r="W22" s="31"/>
-      <c r="X22" s="31"/>
-      <c r="Y22" s="31"/>
-      <c r="Z22" s="31"/>
-      <c r="AA22" s="31"/>
-      <c r="AB22" s="49"/>
-      <c r="AC22" s="49"/>
-      <c r="AD22" s="49"/>
-      <c r="AE22" s="49"/>
-      <c r="AF22" s="49"/>
-      <c r="AG22" s="31"/>
-      <c r="AH22" s="49"/>
-      <c r="AI22" s="49"/>
-      <c r="AJ22" s="59"/>
-      <c r="AK22" s="56"/>
-      <c r="AL22" s="62"/>
-      <c r="AM22" s="49"/>
-      <c r="AN22" s="59"/>
-      <c r="AO22" s="56"/>
-      <c r="AP22" s="62"/>
-      <c r="AQ22" s="49"/>
-      <c r="AR22" s="59"/>
-      <c r="AS22" s="56"/>
-      <c r="AT22" s="49"/>
-      <c r="AU22" s="49"/>
-      <c r="AV22" s="59"/>
-      <c r="AW22" s="56"/>
-      <c r="AX22" s="59"/>
-      <c r="AY22" s="56"/>
-      <c r="AZ22" s="57"/>
-      <c r="BA22" s="56"/>
-      <c r="BB22" s="56"/>
-      <c r="BC22" s="56"/>
-      <c r="BD22" s="56"/>
-      <c r="BE22" s="74"/>
-      <c r="BF22" s="49"/>
-      <c r="BG22" s="49"/>
-      <c r="BH22" s="56"/>
-      <c r="BI22" s="56"/>
-      <c r="BJ22" s="56"/>
+      <c r="W22" s="34"/>
+      <c r="X22" s="34"/>
+      <c r="Y22" s="34"/>
+      <c r="Z22" s="34"/>
+      <c r="AA22" s="34"/>
+      <c r="AB22" s="31"/>
+      <c r="AC22" s="31"/>
+      <c r="AD22" s="31"/>
+      <c r="AE22" s="31"/>
+      <c r="AF22" s="31"/>
+      <c r="AG22" s="34"/>
+      <c r="AH22" s="31"/>
+      <c r="AI22" s="31"/>
+      <c r="AJ22" s="50"/>
+      <c r="AK22" s="48"/>
+      <c r="AL22" s="53"/>
+      <c r="AM22" s="31"/>
+      <c r="AN22" s="50"/>
+      <c r="AO22" s="48"/>
+      <c r="AP22" s="53"/>
+      <c r="AQ22" s="31"/>
+      <c r="AR22" s="50"/>
+      <c r="AS22" s="48"/>
+      <c r="AT22" s="31"/>
+      <c r="AU22" s="31"/>
+      <c r="AV22" s="50"/>
+      <c r="AW22" s="48"/>
+      <c r="AX22" s="50"/>
+      <c r="AY22" s="48"/>
+      <c r="AZ22" s="56"/>
+      <c r="BA22" s="48"/>
+      <c r="BB22" s="48"/>
+      <c r="BC22" s="48"/>
+      <c r="BD22" s="48"/>
+      <c r="BE22" s="46"/>
+      <c r="BF22" s="31"/>
+      <c r="BG22" s="31"/>
+      <c r="BH22" s="48"/>
+      <c r="BI22" s="48"/>
+      <c r="BJ22" s="48"/>
       <c r="BK22" s="29"/>
       <c r="BL22" s="29"/>
       <c r="BM22" s="29"/>
       <c r="BN22" s="29"/>
-      <c r="BO22" s="49"/>
-      <c r="BP22" s="49"/>
-      <c r="BQ22" s="49"/>
-      <c r="BR22" s="49"/>
-      <c r="BS22" s="49"/>
-      <c r="BT22" s="49"/>
-      <c r="BU22" s="49"/>
-      <c r="BV22" s="49"/>
-      <c r="BW22" s="49"/>
-      <c r="BX22" s="49"/>
-      <c r="BY22" s="49"/>
-      <c r="BZ22" s="49"/>
-      <c r="CA22" s="49"/>
-      <c r="CB22" s="49"/>
-      <c r="CC22" s="49"/>
-      <c r="CD22" s="49"/>
+      <c r="BO22" s="31"/>
+      <c r="BP22" s="31"/>
+      <c r="BQ22" s="31"/>
+      <c r="BR22" s="31"/>
+      <c r="BS22" s="31"/>
+      <c r="BT22" s="31"/>
+      <c r="BU22" s="31"/>
+      <c r="BV22" s="31"/>
+      <c r="BW22" s="31"/>
+      <c r="BX22" s="31"/>
+      <c r="BY22" s="31"/>
+      <c r="BZ22" s="31"/>
+      <c r="CA22" s="31"/>
+      <c r="CB22" s="31"/>
+      <c r="CC22" s="31"/>
+      <c r="CD22" s="31"/>
     </row>
     <row r="23" spans="1:82">
       <c r="A23" s="29"/>
@@ -6386,83 +6368,83 @@
       <c r="C23" s="29"/>
       <c r="D23" s="29"/>
       <c r="E23" s="55"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="44"/>
-      <c r="I23" s="46"/>
-      <c r="J23" s="31"/>
-      <c r="K23" s="31"/>
-      <c r="L23" s="31"/>
+      <c r="F23" s="72"/>
+      <c r="G23" s="74"/>
+      <c r="H23" s="72"/>
+      <c r="I23" s="74"/>
+      <c r="J23" s="34"/>
+      <c r="K23" s="34"/>
+      <c r="L23" s="34"/>
       <c r="M23" s="29"/>
       <c r="N23" s="29"/>
       <c r="O23" s="29"/>
       <c r="P23" s="29"/>
       <c r="Q23" s="29"/>
       <c r="R23" s="29"/>
-      <c r="S23" s="49"/>
+      <c r="S23" s="31"/>
       <c r="T23" s="29"/>
       <c r="U23" s="29"/>
       <c r="V23" s="29"/>
-      <c r="W23" s="31"/>
-      <c r="X23" s="31"/>
-      <c r="Y23" s="31"/>
-      <c r="Z23" s="31"/>
-      <c r="AA23" s="31"/>
-      <c r="AB23" s="49"/>
-      <c r="AC23" s="49"/>
-      <c r="AD23" s="49"/>
-      <c r="AE23" s="49"/>
-      <c r="AF23" s="49"/>
-      <c r="AG23" s="31"/>
-      <c r="AH23" s="49"/>
-      <c r="AI23" s="49"/>
-      <c r="AJ23" s="59"/>
-      <c r="AK23" s="56"/>
-      <c r="AL23" s="62"/>
-      <c r="AM23" s="49"/>
-      <c r="AN23" s="59"/>
-      <c r="AO23" s="56"/>
-      <c r="AP23" s="62"/>
-      <c r="AQ23" s="49"/>
-      <c r="AR23" s="59"/>
-      <c r="AS23" s="56"/>
-      <c r="AT23" s="49"/>
-      <c r="AU23" s="49"/>
-      <c r="AV23" s="59"/>
-      <c r="AW23" s="56"/>
-      <c r="AX23" s="59"/>
-      <c r="AY23" s="56"/>
-      <c r="AZ23" s="57"/>
-      <c r="BA23" s="56"/>
-      <c r="BB23" s="56"/>
-      <c r="BC23" s="56"/>
-      <c r="BD23" s="56"/>
-      <c r="BE23" s="74"/>
-      <c r="BF23" s="49"/>
-      <c r="BG23" s="49"/>
-      <c r="BH23" s="56"/>
-      <c r="BI23" s="56"/>
-      <c r="BJ23" s="56"/>
+      <c r="W23" s="34"/>
+      <c r="X23" s="34"/>
+      <c r="Y23" s="34"/>
+      <c r="Z23" s="34"/>
+      <c r="AA23" s="34"/>
+      <c r="AB23" s="31"/>
+      <c r="AC23" s="31"/>
+      <c r="AD23" s="31"/>
+      <c r="AE23" s="31"/>
+      <c r="AF23" s="31"/>
+      <c r="AG23" s="34"/>
+      <c r="AH23" s="31"/>
+      <c r="AI23" s="31"/>
+      <c r="AJ23" s="50"/>
+      <c r="AK23" s="48"/>
+      <c r="AL23" s="53"/>
+      <c r="AM23" s="31"/>
+      <c r="AN23" s="50"/>
+      <c r="AO23" s="48"/>
+      <c r="AP23" s="53"/>
+      <c r="AQ23" s="31"/>
+      <c r="AR23" s="50"/>
+      <c r="AS23" s="48"/>
+      <c r="AT23" s="31"/>
+      <c r="AU23" s="31"/>
+      <c r="AV23" s="50"/>
+      <c r="AW23" s="48"/>
+      <c r="AX23" s="50"/>
+      <c r="AY23" s="48"/>
+      <c r="AZ23" s="56"/>
+      <c r="BA23" s="48"/>
+      <c r="BB23" s="48"/>
+      <c r="BC23" s="48"/>
+      <c r="BD23" s="48"/>
+      <c r="BE23" s="46"/>
+      <c r="BF23" s="31"/>
+      <c r="BG23" s="31"/>
+      <c r="BH23" s="48"/>
+      <c r="BI23" s="48"/>
+      <c r="BJ23" s="48"/>
       <c r="BK23" s="29"/>
       <c r="BL23" s="29"/>
       <c r="BM23" s="29"/>
       <c r="BN23" s="29"/>
-      <c r="BO23" s="49"/>
-      <c r="BP23" s="49"/>
-      <c r="BQ23" s="49"/>
-      <c r="BR23" s="49"/>
-      <c r="BS23" s="49"/>
-      <c r="BT23" s="49"/>
-      <c r="BU23" s="49"/>
-      <c r="BV23" s="49"/>
-      <c r="BW23" s="49"/>
-      <c r="BX23" s="49"/>
-      <c r="BY23" s="49"/>
-      <c r="BZ23" s="49"/>
-      <c r="CA23" s="49"/>
-      <c r="CB23" s="49"/>
-      <c r="CC23" s="49"/>
-      <c r="CD23" s="49"/>
+      <c r="BO23" s="31"/>
+      <c r="BP23" s="31"/>
+      <c r="BQ23" s="31"/>
+      <c r="BR23" s="31"/>
+      <c r="BS23" s="31"/>
+      <c r="BT23" s="31"/>
+      <c r="BU23" s="31"/>
+      <c r="BV23" s="31"/>
+      <c r="BW23" s="31"/>
+      <c r="BX23" s="31"/>
+      <c r="BY23" s="31"/>
+      <c r="BZ23" s="31"/>
+      <c r="CA23" s="31"/>
+      <c r="CB23" s="31"/>
+      <c r="CC23" s="31"/>
+      <c r="CD23" s="31"/>
     </row>
     <row r="24" spans="1:82">
       <c r="A24" s="29"/>
@@ -6470,83 +6452,83 @@
       <c r="C24" s="29"/>
       <c r="D24" s="29"/>
       <c r="E24" s="55"/>
-      <c r="F24" s="44"/>
-      <c r="G24" s="46"/>
-      <c r="H24" s="44"/>
-      <c r="I24" s="46"/>
-      <c r="J24" s="31"/>
-      <c r="K24" s="31"/>
-      <c r="L24" s="31"/>
+      <c r="F24" s="72"/>
+      <c r="G24" s="74"/>
+      <c r="H24" s="72"/>
+      <c r="I24" s="74"/>
+      <c r="J24" s="34"/>
+      <c r="K24" s="34"/>
+      <c r="L24" s="34"/>
       <c r="M24" s="29"/>
       <c r="N24" s="29"/>
       <c r="O24" s="29"/>
       <c r="P24" s="29"/>
       <c r="Q24" s="29"/>
       <c r="R24" s="29"/>
-      <c r="S24" s="49"/>
+      <c r="S24" s="31"/>
       <c r="T24" s="29"/>
       <c r="U24" s="29"/>
       <c r="V24" s="29"/>
-      <c r="W24" s="31"/>
-      <c r="X24" s="31"/>
-      <c r="Y24" s="31"/>
-      <c r="Z24" s="31"/>
-      <c r="AA24" s="31"/>
-      <c r="AB24" s="49"/>
-      <c r="AC24" s="49"/>
-      <c r="AD24" s="49"/>
-      <c r="AE24" s="49"/>
-      <c r="AF24" s="49"/>
-      <c r="AG24" s="31"/>
-      <c r="AH24" s="49"/>
-      <c r="AI24" s="49"/>
-      <c r="AJ24" s="59"/>
-      <c r="AK24" s="56"/>
-      <c r="AL24" s="62"/>
-      <c r="AM24" s="49"/>
-      <c r="AN24" s="59"/>
-      <c r="AO24" s="56"/>
-      <c r="AP24" s="62"/>
-      <c r="AQ24" s="49"/>
-      <c r="AR24" s="59"/>
-      <c r="AS24" s="56"/>
-      <c r="AT24" s="49"/>
-      <c r="AU24" s="49"/>
-      <c r="AV24" s="59"/>
-      <c r="AW24" s="56"/>
-      <c r="AX24" s="59"/>
-      <c r="AY24" s="56"/>
-      <c r="AZ24" s="57"/>
-      <c r="BA24" s="56"/>
-      <c r="BB24" s="56"/>
-      <c r="BC24" s="56"/>
-      <c r="BD24" s="56"/>
-      <c r="BE24" s="74"/>
-      <c r="BF24" s="49"/>
-      <c r="BG24" s="49"/>
-      <c r="BH24" s="56"/>
-      <c r="BI24" s="56"/>
-      <c r="BJ24" s="56"/>
+      <c r="W24" s="34"/>
+      <c r="X24" s="34"/>
+      <c r="Y24" s="34"/>
+      <c r="Z24" s="34"/>
+      <c r="AA24" s="34"/>
+      <c r="AB24" s="31"/>
+      <c r="AC24" s="31"/>
+      <c r="AD24" s="31"/>
+      <c r="AE24" s="31"/>
+      <c r="AF24" s="31"/>
+      <c r="AG24" s="34"/>
+      <c r="AH24" s="31"/>
+      <c r="AI24" s="31"/>
+      <c r="AJ24" s="50"/>
+      <c r="AK24" s="48"/>
+      <c r="AL24" s="53"/>
+      <c r="AM24" s="31"/>
+      <c r="AN24" s="50"/>
+      <c r="AO24" s="48"/>
+      <c r="AP24" s="53"/>
+      <c r="AQ24" s="31"/>
+      <c r="AR24" s="50"/>
+      <c r="AS24" s="48"/>
+      <c r="AT24" s="31"/>
+      <c r="AU24" s="31"/>
+      <c r="AV24" s="50"/>
+      <c r="AW24" s="48"/>
+      <c r="AX24" s="50"/>
+      <c r="AY24" s="48"/>
+      <c r="AZ24" s="56"/>
+      <c r="BA24" s="48"/>
+      <c r="BB24" s="48"/>
+      <c r="BC24" s="48"/>
+      <c r="BD24" s="48"/>
+      <c r="BE24" s="46"/>
+      <c r="BF24" s="31"/>
+      <c r="BG24" s="31"/>
+      <c r="BH24" s="48"/>
+      <c r="BI24" s="48"/>
+      <c r="BJ24" s="48"/>
       <c r="BK24" s="29"/>
       <c r="BL24" s="29"/>
       <c r="BM24" s="29"/>
       <c r="BN24" s="29"/>
-      <c r="BO24" s="49"/>
-      <c r="BP24" s="49"/>
-      <c r="BQ24" s="49"/>
-      <c r="BR24" s="49"/>
-      <c r="BS24" s="49"/>
-      <c r="BT24" s="49"/>
-      <c r="BU24" s="49"/>
-      <c r="BV24" s="49"/>
-      <c r="BW24" s="49"/>
-      <c r="BX24" s="49"/>
-      <c r="BY24" s="49"/>
-      <c r="BZ24" s="49"/>
-      <c r="CA24" s="49"/>
-      <c r="CB24" s="49"/>
-      <c r="CC24" s="49"/>
-      <c r="CD24" s="49"/>
+      <c r="BO24" s="31"/>
+      <c r="BP24" s="31"/>
+      <c r="BQ24" s="31"/>
+      <c r="BR24" s="31"/>
+      <c r="BS24" s="31"/>
+      <c r="BT24" s="31"/>
+      <c r="BU24" s="31"/>
+      <c r="BV24" s="31"/>
+      <c r="BW24" s="31"/>
+      <c r="BX24" s="31"/>
+      <c r="BY24" s="31"/>
+      <c r="BZ24" s="31"/>
+      <c r="CA24" s="31"/>
+      <c r="CB24" s="31"/>
+      <c r="CC24" s="31"/>
+      <c r="CD24" s="31"/>
     </row>
     <row r="25" spans="1:82">
       <c r="A25" s="29"/>
@@ -6554,83 +6536,83 @@
       <c r="C25" s="29"/>
       <c r="D25" s="29"/>
       <c r="E25" s="55"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="46"/>
-      <c r="H25" s="44"/>
-      <c r="I25" s="46"/>
-      <c r="J25" s="31"/>
-      <c r="K25" s="31"/>
-      <c r="L25" s="31"/>
+      <c r="F25" s="72"/>
+      <c r="G25" s="74"/>
+      <c r="H25" s="72"/>
+      <c r="I25" s="74"/>
+      <c r="J25" s="34"/>
+      <c r="K25" s="34"/>
+      <c r="L25" s="34"/>
       <c r="M25" s="29"/>
       <c r="N25" s="29"/>
       <c r="O25" s="29"/>
       <c r="P25" s="29"/>
       <c r="Q25" s="29"/>
       <c r="R25" s="29"/>
-      <c r="S25" s="49"/>
+      <c r="S25" s="31"/>
       <c r="T25" s="29"/>
       <c r="U25" s="29"/>
       <c r="V25" s="29"/>
-      <c r="W25" s="31"/>
-      <c r="X25" s="31"/>
-      <c r="Y25" s="31"/>
-      <c r="Z25" s="31"/>
-      <c r="AA25" s="31"/>
-      <c r="AB25" s="49"/>
-      <c r="AC25" s="49"/>
-      <c r="AD25" s="49"/>
-      <c r="AE25" s="49"/>
-      <c r="AF25" s="49"/>
-      <c r="AG25" s="31"/>
-      <c r="AH25" s="49"/>
-      <c r="AI25" s="49"/>
-      <c r="AJ25" s="59"/>
-      <c r="AK25" s="56"/>
-      <c r="AL25" s="62"/>
-      <c r="AM25" s="49"/>
-      <c r="AN25" s="59"/>
-      <c r="AO25" s="56"/>
-      <c r="AP25" s="62"/>
-      <c r="AQ25" s="49"/>
-      <c r="AR25" s="59"/>
-      <c r="AS25" s="56"/>
-      <c r="AT25" s="49"/>
-      <c r="AU25" s="49"/>
-      <c r="AV25" s="59"/>
-      <c r="AW25" s="56"/>
-      <c r="AX25" s="59"/>
-      <c r="AY25" s="56"/>
-      <c r="AZ25" s="57"/>
-      <c r="BA25" s="56"/>
-      <c r="BB25" s="56"/>
-      <c r="BC25" s="56"/>
-      <c r="BD25" s="56"/>
-      <c r="BE25" s="74"/>
-      <c r="BF25" s="49"/>
-      <c r="BG25" s="49"/>
-      <c r="BH25" s="56"/>
-      <c r="BI25" s="56"/>
-      <c r="BJ25" s="56"/>
+      <c r="W25" s="34"/>
+      <c r="X25" s="34"/>
+      <c r="Y25" s="34"/>
+      <c r="Z25" s="34"/>
+      <c r="AA25" s="34"/>
+      <c r="AB25" s="31"/>
+      <c r="AC25" s="31"/>
+      <c r="AD25" s="31"/>
+      <c r="AE25" s="31"/>
+      <c r="AF25" s="31"/>
+      <c r="AG25" s="34"/>
+      <c r="AH25" s="31"/>
+      <c r="AI25" s="31"/>
+      <c r="AJ25" s="50"/>
+      <c r="AK25" s="48"/>
+      <c r="AL25" s="53"/>
+      <c r="AM25" s="31"/>
+      <c r="AN25" s="50"/>
+      <c r="AO25" s="48"/>
+      <c r="AP25" s="53"/>
+      <c r="AQ25" s="31"/>
+      <c r="AR25" s="50"/>
+      <c r="AS25" s="48"/>
+      <c r="AT25" s="31"/>
+      <c r="AU25" s="31"/>
+      <c r="AV25" s="50"/>
+      <c r="AW25" s="48"/>
+      <c r="AX25" s="50"/>
+      <c r="AY25" s="48"/>
+      <c r="AZ25" s="56"/>
+      <c r="BA25" s="48"/>
+      <c r="BB25" s="48"/>
+      <c r="BC25" s="48"/>
+      <c r="BD25" s="48"/>
+      <c r="BE25" s="46"/>
+      <c r="BF25" s="31"/>
+      <c r="BG25" s="31"/>
+      <c r="BH25" s="48"/>
+      <c r="BI25" s="48"/>
+      <c r="BJ25" s="48"/>
       <c r="BK25" s="29"/>
       <c r="BL25" s="29"/>
       <c r="BM25" s="29"/>
       <c r="BN25" s="29"/>
-      <c r="BO25" s="49"/>
-      <c r="BP25" s="49"/>
-      <c r="BQ25" s="49"/>
-      <c r="BR25" s="49"/>
-      <c r="BS25" s="49"/>
-      <c r="BT25" s="49"/>
-      <c r="BU25" s="49"/>
-      <c r="BV25" s="49"/>
-      <c r="BW25" s="49"/>
-      <c r="BX25" s="49"/>
-      <c r="BY25" s="49"/>
-      <c r="BZ25" s="49"/>
-      <c r="CA25" s="49"/>
-      <c r="CB25" s="49"/>
-      <c r="CC25" s="49"/>
-      <c r="CD25" s="49"/>
+      <c r="BO25" s="31"/>
+      <c r="BP25" s="31"/>
+      <c r="BQ25" s="31"/>
+      <c r="BR25" s="31"/>
+      <c r="BS25" s="31"/>
+      <c r="BT25" s="31"/>
+      <c r="BU25" s="31"/>
+      <c r="BV25" s="31"/>
+      <c r="BW25" s="31"/>
+      <c r="BX25" s="31"/>
+      <c r="BY25" s="31"/>
+      <c r="BZ25" s="31"/>
+      <c r="CA25" s="31"/>
+      <c r="CB25" s="31"/>
+      <c r="CC25" s="31"/>
+      <c r="CD25" s="31"/>
     </row>
     <row r="26" spans="1:82">
       <c r="A26" s="29"/>
@@ -6638,99 +6620,99 @@
       <c r="C26" s="29"/>
       <c r="D26" s="29"/>
       <c r="E26" s="55"/>
-      <c r="F26" s="44"/>
-      <c r="G26" s="46"/>
-      <c r="H26" s="44"/>
-      <c r="I26" s="46"/>
-      <c r="J26" s="32"/>
-      <c r="K26" s="32"/>
-      <c r="L26" s="32"/>
+      <c r="F26" s="72"/>
+      <c r="G26" s="74"/>
+      <c r="H26" s="72"/>
+      <c r="I26" s="74"/>
+      <c r="J26" s="35"/>
+      <c r="K26" s="35"/>
+      <c r="L26" s="35"/>
       <c r="M26" s="29"/>
       <c r="N26" s="29"/>
       <c r="O26" s="29"/>
       <c r="P26" s="29"/>
       <c r="Q26" s="29"/>
       <c r="R26" s="29"/>
-      <c r="S26" s="50"/>
+      <c r="S26" s="32"/>
       <c r="T26" s="29"/>
       <c r="U26" s="29"/>
       <c r="V26" s="29"/>
-      <c r="W26" s="32"/>
-      <c r="X26" s="32"/>
-      <c r="Y26" s="32"/>
-      <c r="Z26" s="32"/>
-      <c r="AA26" s="32"/>
-      <c r="AB26" s="50"/>
-      <c r="AC26" s="50"/>
-      <c r="AD26" s="50"/>
-      <c r="AE26" s="50"/>
-      <c r="AF26" s="50"/>
-      <c r="AG26" s="32"/>
-      <c r="AH26" s="50"/>
-      <c r="AI26" s="50"/>
-      <c r="AJ26" s="60"/>
-      <c r="AK26" s="56"/>
-      <c r="AL26" s="63"/>
-      <c r="AM26" s="50"/>
-      <c r="AN26" s="60"/>
-      <c r="AO26" s="56"/>
-      <c r="AP26" s="63"/>
-      <c r="AQ26" s="50"/>
-      <c r="AR26" s="60"/>
-      <c r="AS26" s="56"/>
-      <c r="AT26" s="50"/>
-      <c r="AU26" s="50"/>
-      <c r="AV26" s="60"/>
-      <c r="AW26" s="56"/>
-      <c r="AX26" s="60"/>
-      <c r="AY26" s="56"/>
-      <c r="AZ26" s="57"/>
-      <c r="BA26" s="56"/>
-      <c r="BB26" s="56"/>
-      <c r="BC26" s="56"/>
-      <c r="BD26" s="56"/>
-      <c r="BE26" s="75"/>
-      <c r="BF26" s="50"/>
-      <c r="BG26" s="50"/>
-      <c r="BH26" s="56"/>
-      <c r="BI26" s="56"/>
-      <c r="BJ26" s="56"/>
+      <c r="W26" s="35"/>
+      <c r="X26" s="35"/>
+      <c r="Y26" s="35"/>
+      <c r="Z26" s="35"/>
+      <c r="AA26" s="35"/>
+      <c r="AB26" s="32"/>
+      <c r="AC26" s="32"/>
+      <c r="AD26" s="32"/>
+      <c r="AE26" s="32"/>
+      <c r="AF26" s="32"/>
+      <c r="AG26" s="35"/>
+      <c r="AH26" s="32"/>
+      <c r="AI26" s="32"/>
+      <c r="AJ26" s="51"/>
+      <c r="AK26" s="48"/>
+      <c r="AL26" s="54"/>
+      <c r="AM26" s="32"/>
+      <c r="AN26" s="51"/>
+      <c r="AO26" s="48"/>
+      <c r="AP26" s="54"/>
+      <c r="AQ26" s="32"/>
+      <c r="AR26" s="51"/>
+      <c r="AS26" s="48"/>
+      <c r="AT26" s="32"/>
+      <c r="AU26" s="32"/>
+      <c r="AV26" s="51"/>
+      <c r="AW26" s="48"/>
+      <c r="AX26" s="51"/>
+      <c r="AY26" s="48"/>
+      <c r="AZ26" s="56"/>
+      <c r="BA26" s="48"/>
+      <c r="BB26" s="48"/>
+      <c r="BC26" s="48"/>
+      <c r="BD26" s="48"/>
+      <c r="BE26" s="47"/>
+      <c r="BF26" s="32"/>
+      <c r="BG26" s="32"/>
+      <c r="BH26" s="48"/>
+      <c r="BI26" s="48"/>
+      <c r="BJ26" s="48"/>
       <c r="BK26" s="29"/>
       <c r="BL26" s="29"/>
       <c r="BM26" s="29"/>
       <c r="BN26" s="29"/>
-      <c r="BO26" s="50"/>
-      <c r="BP26" s="50"/>
-      <c r="BQ26" s="50"/>
-      <c r="BR26" s="50"/>
-      <c r="BS26" s="50"/>
-      <c r="BT26" s="50"/>
-      <c r="BU26" s="50"/>
-      <c r="BV26" s="50"/>
-      <c r="BW26" s="50"/>
-      <c r="BX26" s="50"/>
-      <c r="BY26" s="50"/>
-      <c r="BZ26" s="50"/>
-      <c r="CA26" s="50"/>
-      <c r="CB26" s="50"/>
-      <c r="CC26" s="50"/>
-      <c r="CD26" s="50"/>
+      <c r="BO26" s="32"/>
+      <c r="BP26" s="32"/>
+      <c r="BQ26" s="32"/>
+      <c r="BR26" s="32"/>
+      <c r="BS26" s="32"/>
+      <c r="BT26" s="32"/>
+      <c r="BU26" s="32"/>
+      <c r="BV26" s="32"/>
+      <c r="BW26" s="32"/>
+      <c r="BX26" s="32"/>
+      <c r="BY26" s="32"/>
+      <c r="BZ26" s="32"/>
+      <c r="CA26" s="32"/>
+      <c r="CB26" s="32"/>
+      <c r="CC26" s="32"/>
+      <c r="CD26" s="32"/>
     </row>
     <row r="27" spans="1:82" ht="11.25" customHeight="1">
-      <c r="F27" s="44"/>
-      <c r="G27" s="46"/>
-      <c r="H27" s="44"/>
-      <c r="I27" s="46"/>
-      <c r="AK27" s="56"/>
-      <c r="AO27" s="56"/>
-      <c r="AS27" s="56"/>
-      <c r="AW27" s="56"/>
-      <c r="AY27" s="56"/>
-      <c r="AZ27" s="57"/>
-      <c r="BA27" s="56"/>
-      <c r="BB27" s="56"/>
-      <c r="BC27" s="56"/>
-      <c r="BD27" s="56"/>
+      <c r="F27" s="72"/>
+      <c r="G27" s="74"/>
+      <c r="H27" s="72"/>
+      <c r="I27" s="74"/>
+      <c r="AK27" s="48"/>
+      <c r="AO27" s="48"/>
+      <c r="AS27" s="48"/>
+      <c r="AW27" s="48"/>
+      <c r="AY27" s="48"/>
+      <c r="AZ27" s="56"/>
+      <c r="BA27" s="48"/>
+      <c r="BB27" s="48"/>
+      <c r="BC27" s="48"/>
+      <c r="BD27" s="48"/>
     </row>
     <row r="28" spans="1:82" ht="11.25" customHeight="1">
       <c r="B28" s="7" t="s">
@@ -6739,227 +6721,227 @@
       <c r="C28" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F28" s="44"/>
-      <c r="G28" s="46"/>
-      <c r="H28" s="44"/>
-      <c r="I28" s="47"/>
+      <c r="F28" s="72"/>
+      <c r="G28" s="74"/>
+      <c r="H28" s="72"/>
+      <c r="I28" s="75"/>
       <c r="J28" s="29" t="s">
         <v>219</v>
       </c>
       <c r="V28" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="AE28" s="48" t="s">
+      <c r="AE28" s="30" t="s">
         <v>222</v>
       </c>
-      <c r="AK28" s="56"/>
-      <c r="AO28" s="56"/>
-      <c r="AS28" s="56"/>
-      <c r="AW28" s="56"/>
-      <c r="AY28" s="56"/>
-      <c r="AZ28" s="57"/>
-      <c r="BA28" s="56"/>
-      <c r="BB28" s="56"/>
-      <c r="BC28" s="56"/>
-      <c r="BD28" s="56"/>
-      <c r="BJ28" s="48" t="s">
+      <c r="AK28" s="48"/>
+      <c r="AO28" s="48"/>
+      <c r="AS28" s="48"/>
+      <c r="AW28" s="48"/>
+      <c r="AY28" s="48"/>
+      <c r="AZ28" s="56"/>
+      <c r="BA28" s="48"/>
+      <c r="BB28" s="48"/>
+      <c r="BC28" s="48"/>
+      <c r="BD28" s="48"/>
+      <c r="BJ28" s="30" t="s">
         <v>253</v>
       </c>
       <c r="BK28" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="CB28" s="30" t="s">
-        <v>516</v>
-      </c>
-      <c r="CC28" s="30" t="s">
-        <v>516</v>
+      <c r="CB28" s="33" t="s">
+        <v>504</v>
+      </c>
+      <c r="CC28" s="33" t="s">
+        <v>504</v>
       </c>
     </row>
     <row r="29" spans="1:82">
-      <c r="B29" s="64" t="s">
+      <c r="B29" s="36" t="s">
         <v>189</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>517</v>
-      </c>
-      <c r="F29" s="45"/>
-      <c r="G29" s="46"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="47"/>
+        <v>505</v>
+      </c>
+      <c r="F29" s="73"/>
+      <c r="G29" s="74"/>
+      <c r="H29" s="73"/>
+      <c r="I29" s="75"/>
       <c r="J29" s="29"/>
       <c r="V29" s="15" t="s">
-        <v>525</v>
-      </c>
-      <c r="AE29" s="49"/>
-      <c r="BJ29" s="49"/>
+        <v>513</v>
+      </c>
+      <c r="AE29" s="31"/>
+      <c r="BJ29" s="31"/>
       <c r="BK29" s="14" t="s">
-        <v>532</v>
-      </c>
-      <c r="CB29" s="31"/>
-      <c r="CC29" s="31"/>
+        <v>520</v>
+      </c>
+      <c r="CB29" s="34"/>
+      <c r="CC29" s="34"/>
     </row>
     <row r="30" spans="1:82" ht="11.25" customHeight="1">
-      <c r="B30" s="65"/>
+      <c r="B30" s="37"/>
       <c r="C30" s="5" t="s">
-        <v>518</v>
+        <v>506</v>
       </c>
       <c r="J30" s="29"/>
       <c r="V30" s="17" t="s">
-        <v>526</v>
-      </c>
-      <c r="AE30" s="49"/>
-      <c r="BJ30" s="49"/>
+        <v>514</v>
+      </c>
+      <c r="AE30" s="31"/>
+      <c r="BJ30" s="31"/>
       <c r="BK30" s="6" t="s">
-        <v>533</v>
-      </c>
-      <c r="CB30" s="31"/>
-      <c r="CC30" s="31"/>
+        <v>521</v>
+      </c>
+      <c r="CB30" s="34"/>
+      <c r="CC30" s="34"/>
     </row>
     <row r="31" spans="1:82" ht="11.25" customHeight="1">
-      <c r="B31" s="65"/>
+      <c r="B31" s="37"/>
       <c r="C31" s="5" t="s">
-        <v>519</v>
+        <v>507</v>
       </c>
       <c r="J31" s="29"/>
       <c r="V31" s="17" t="s">
-        <v>527</v>
-      </c>
-      <c r="AE31" s="49"/>
-      <c r="BJ31" s="49"/>
-      <c r="CB31" s="31"/>
-      <c r="CC31" s="31"/>
+        <v>515</v>
+      </c>
+      <c r="AE31" s="31"/>
+      <c r="BJ31" s="31"/>
+      <c r="CB31" s="34"/>
+      <c r="CC31" s="34"/>
     </row>
     <row r="32" spans="1:82" ht="11.25" customHeight="1">
-      <c r="B32" s="65"/>
+      <c r="B32" s="37"/>
       <c r="C32" s="5" t="s">
-        <v>520</v>
+        <v>508</v>
       </c>
       <c r="J32" s="29"/>
       <c r="V32" s="17" t="s">
-        <v>528</v>
-      </c>
-      <c r="AE32" s="49"/>
-      <c r="BJ32" s="49"/>
-      <c r="CB32" s="31"/>
-      <c r="CC32" s="31"/>
+        <v>516</v>
+      </c>
+      <c r="AE32" s="31"/>
+      <c r="BJ32" s="31"/>
+      <c r="CB32" s="34"/>
+      <c r="CC32" s="34"/>
     </row>
     <row r="33" spans="2:81" ht="11.25" customHeight="1">
-      <c r="B33" s="65"/>
+      <c r="B33" s="37"/>
       <c r="C33" s="5" t="s">
-        <v>521</v>
+        <v>509</v>
       </c>
       <c r="J33" s="29"/>
       <c r="V33" s="17" t="s">
-        <v>529</v>
-      </c>
-      <c r="AE33" s="49"/>
-      <c r="BJ33" s="49"/>
-      <c r="CB33" s="32"/>
-      <c r="CC33" s="32"/>
+        <v>517</v>
+      </c>
+      <c r="AE33" s="31"/>
+      <c r="BJ33" s="31"/>
+      <c r="CB33" s="35"/>
+      <c r="CC33" s="35"/>
     </row>
     <row r="34" spans="2:81" ht="11.25" customHeight="1">
-      <c r="B34" s="65"/>
+      <c r="B34" s="37"/>
       <c r="C34" s="5" t="s">
-        <v>522</v>
+        <v>510</v>
       </c>
       <c r="J34" s="29"/>
       <c r="V34" s="17" t="s">
-        <v>530</v>
-      </c>
-      <c r="AE34" s="49"/>
-      <c r="BJ34" s="50"/>
+        <v>518</v>
+      </c>
+      <c r="AE34" s="31"/>
+      <c r="BJ34" s="32"/>
       <c r="CC34" s="8"/>
     </row>
     <row r="35" spans="2:81" ht="11.25" customHeight="1">
-      <c r="B35" s="66"/>
+      <c r="B35" s="38"/>
       <c r="C35" s="5" t="s">
-        <v>523</v>
+        <v>511</v>
       </c>
       <c r="J35" s="29"/>
       <c r="V35" s="16" t="s">
-        <v>531</v>
-      </c>
-      <c r="AE35" s="49"/>
-      <c r="CB35" s="48" t="s">
-        <v>534</v>
-      </c>
-      <c r="CC35" s="48" t="s">
-        <v>534</v>
+        <v>519</v>
+      </c>
+      <c r="AE35" s="31"/>
+      <c r="CB35" s="30" t="s">
+        <v>522</v>
+      </c>
+      <c r="CC35" s="30" t="s">
+        <v>522</v>
       </c>
     </row>
     <row r="36" spans="2:81">
       <c r="C36" s="5" t="s">
-        <v>524</v>
+        <v>512</v>
       </c>
       <c r="J36" s="29"/>
-      <c r="AE36" s="49"/>
-      <c r="CB36" s="49"/>
-      <c r="CC36" s="49"/>
+      <c r="AE36" s="31"/>
+      <c r="CB36" s="31"/>
+      <c r="CC36" s="31"/>
     </row>
     <row r="37" spans="2:81">
       <c r="C37" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="AE37" s="50"/>
-      <c r="CB37" s="49"/>
-      <c r="CC37" s="49"/>
+      <c r="AE37" s="32"/>
+      <c r="CB37" s="31"/>
+      <c r="CC37" s="31"/>
     </row>
     <row r="38" spans="2:81">
       <c r="C38" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="CB38" s="49"/>
-      <c r="CC38" s="49"/>
+      <c r="CB38" s="31"/>
+      <c r="CC38" s="31"/>
     </row>
     <row r="39" spans="2:81">
       <c r="C39" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="AE39" s="30" t="s">
+      <c r="AE39" s="33" t="s">
         <v>223</v>
       </c>
-      <c r="CB39" s="49"/>
-      <c r="CC39" s="49"/>
+      <c r="CB39" s="31"/>
+      <c r="CC39" s="31"/>
     </row>
     <row r="40" spans="2:81">
       <c r="C40" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="AE40" s="31"/>
-      <c r="CB40" s="49"/>
-      <c r="CC40" s="49"/>
+      <c r="AE40" s="34"/>
+      <c r="CB40" s="31"/>
+      <c r="CC40" s="31"/>
     </row>
     <row r="41" spans="2:81">
       <c r="C41" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="AE41" s="31"/>
-      <c r="CB41" s="49"/>
-      <c r="CC41" s="49"/>
+      <c r="AE41" s="34"/>
+      <c r="CB41" s="31"/>
+      <c r="CC41" s="31"/>
     </row>
     <row r="42" spans="2:81">
       <c r="C42" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="AE42" s="31"/>
-      <c r="CB42" s="49"/>
-      <c r="CC42" s="49"/>
+      <c r="AE42" s="34"/>
+      <c r="CB42" s="31"/>
+      <c r="CC42" s="31"/>
     </row>
     <row r="43" spans="2:81">
       <c r="C43" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="AE43" s="31"/>
-      <c r="CB43" s="49"/>
-      <c r="CC43" s="49"/>
+      <c r="AE43" s="34"/>
+      <c r="CB43" s="31"/>
+      <c r="CC43" s="31"/>
     </row>
     <row r="44" spans="2:81">
       <c r="C44" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="AE44" s="32"/>
-      <c r="CB44" s="49"/>
-      <c r="CC44" s="49"/>
+      <c r="AE44" s="35"/>
+      <c r="CB44" s="31"/>
+      <c r="CC44" s="31"/>
     </row>
     <row r="45" spans="2:81">
       <c r="C45" s="5" t="s">
@@ -6968,24 +6950,24 @@
       <c r="BJ45" s="29" t="s">
         <v>187</v>
       </c>
-      <c r="CB45" s="49"/>
-      <c r="CC45" s="49"/>
+      <c r="CB45" s="31"/>
+      <c r="CC45" s="31"/>
     </row>
     <row r="46" spans="2:81">
       <c r="C46" s="5" t="s">
         <v>107</v>
       </c>
       <c r="BJ46" s="29"/>
-      <c r="CB46" s="49"/>
-      <c r="CC46" s="49"/>
+      <c r="CB46" s="31"/>
+      <c r="CC46" s="31"/>
     </row>
     <row r="47" spans="2:81">
       <c r="C47" s="5" t="s">
         <v>108</v>
       </c>
       <c r="BJ47" s="29"/>
-      <c r="CB47" s="50"/>
-      <c r="CC47" s="50"/>
+      <c r="CB47" s="32"/>
+      <c r="CC47" s="32"/>
     </row>
     <row r="48" spans="2:81">
       <c r="C48" s="5" t="s">
@@ -6997,33 +6979,33 @@
       <c r="C49" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="CB49" s="30" t="s">
-        <v>535</v>
-      </c>
-      <c r="CC49" s="30" t="s">
-        <v>536</v>
+      <c r="CB49" s="33" t="s">
+        <v>523</v>
+      </c>
+      <c r="CC49" s="33" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="50" spans="3:81">
       <c r="C50" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="CB50" s="31"/>
-      <c r="CC50" s="31"/>
+      <c r="CB50" s="34"/>
+      <c r="CC50" s="34"/>
     </row>
     <row r="51" spans="3:81">
       <c r="C51" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="CB51" s="31"/>
-      <c r="CC51" s="31"/>
+      <c r="CB51" s="34"/>
+      <c r="CC51" s="34"/>
     </row>
     <row r="52" spans="3:81">
       <c r="C52" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="CB52" s="32"/>
-      <c r="CC52" s="32"/>
+      <c r="CB52" s="35"/>
+      <c r="CC52" s="35"/>
     </row>
     <row r="53" spans="3:81">
       <c r="C53" s="5" t="s">
@@ -7167,6 +7149,89 @@
     </row>
   </sheetData>
   <mergeCells count="107">
+    <mergeCell ref="A21:A26"/>
+    <mergeCell ref="B21:B26"/>
+    <mergeCell ref="C21:C26"/>
+    <mergeCell ref="L21:L26"/>
+    <mergeCell ref="BO18:CA20"/>
+    <mergeCell ref="A18:AX20"/>
+    <mergeCell ref="AE39:AE44"/>
+    <mergeCell ref="F21:F29"/>
+    <mergeCell ref="G21:G29"/>
+    <mergeCell ref="H21:H29"/>
+    <mergeCell ref="I21:I29"/>
+    <mergeCell ref="T21:T26"/>
+    <mergeCell ref="M21:M26"/>
+    <mergeCell ref="N21:N26"/>
+    <mergeCell ref="O21:O26"/>
+    <mergeCell ref="P21:P26"/>
+    <mergeCell ref="Q21:Q26"/>
+    <mergeCell ref="R21:R26"/>
+    <mergeCell ref="BO21:BO26"/>
+    <mergeCell ref="AA21:AA26"/>
+    <mergeCell ref="BL18:BN20"/>
+    <mergeCell ref="K21:K26"/>
+    <mergeCell ref="J21:J26"/>
+    <mergeCell ref="D21:D26"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="BE18:BE20"/>
+    <mergeCell ref="AY18:BD20"/>
+    <mergeCell ref="BF18:BF20"/>
+    <mergeCell ref="BG18:BG20"/>
+    <mergeCell ref="BH18:BH20"/>
+    <mergeCell ref="BI18:BJ20"/>
+    <mergeCell ref="BK18:BK20"/>
+    <mergeCell ref="E21:E26"/>
+    <mergeCell ref="BY21:BY26"/>
+    <mergeCell ref="U21:U26"/>
+    <mergeCell ref="V21:V26"/>
+    <mergeCell ref="W21:W26"/>
+    <mergeCell ref="X21:X26"/>
+    <mergeCell ref="Y21:Y26"/>
+    <mergeCell ref="Z21:Z26"/>
+    <mergeCell ref="AK21:AK28"/>
+    <mergeCell ref="AO21:AO28"/>
+    <mergeCell ref="AS21:AS28"/>
+    <mergeCell ref="AW21:AW28"/>
+    <mergeCell ref="AZ21:AZ28"/>
+    <mergeCell ref="AM21:AM26"/>
+    <mergeCell ref="AN21:AN26"/>
+    <mergeCell ref="AP21:AP26"/>
+    <mergeCell ref="S21:S26"/>
+    <mergeCell ref="AE28:AE37"/>
+    <mergeCell ref="AB21:AB26"/>
+    <mergeCell ref="AC21:AC26"/>
+    <mergeCell ref="AD21:AD26"/>
+    <mergeCell ref="AE21:AE26"/>
+    <mergeCell ref="AQ21:AQ26"/>
+    <mergeCell ref="AF21:AF26"/>
+    <mergeCell ref="AG21:AG26"/>
+    <mergeCell ref="AH21:AH26"/>
+    <mergeCell ref="AI21:AI26"/>
+    <mergeCell ref="AJ21:AJ26"/>
+    <mergeCell ref="AL21:AL26"/>
+    <mergeCell ref="AX21:AX26"/>
+    <mergeCell ref="AR21:AR26"/>
+    <mergeCell ref="BJ45:BJ48"/>
+    <mergeCell ref="BQ21:BQ26"/>
+    <mergeCell ref="AU21:AU26"/>
+    <mergeCell ref="AV21:AV26"/>
+    <mergeCell ref="AT21:AT26"/>
+    <mergeCell ref="AY21:AY28"/>
+    <mergeCell ref="BA21:BA28"/>
+    <mergeCell ref="BR21:BR26"/>
+    <mergeCell ref="BS21:BS26"/>
+    <mergeCell ref="BB21:BB28"/>
+    <mergeCell ref="BT21:BT26"/>
+    <mergeCell ref="BJ21:BJ26"/>
+    <mergeCell ref="BK21:BK26"/>
+    <mergeCell ref="BL21:BL26"/>
+    <mergeCell ref="BM21:BM26"/>
+    <mergeCell ref="BN21:BN26"/>
+    <mergeCell ref="BP21:BP26"/>
+    <mergeCell ref="BD21:BD28"/>
+    <mergeCell ref="BC21:BC28"/>
     <mergeCell ref="CD21:CD26"/>
     <mergeCell ref="CB35:CB47"/>
     <mergeCell ref="CB49:CB52"/>
@@ -7191,89 +7256,6 @@
     <mergeCell ref="BG21:BG26"/>
     <mergeCell ref="BH21:BH26"/>
     <mergeCell ref="BI21:BI26"/>
-    <mergeCell ref="BR21:BR26"/>
-    <mergeCell ref="BS21:BS26"/>
-    <mergeCell ref="BB21:BB28"/>
-    <mergeCell ref="BT21:BT26"/>
-    <mergeCell ref="BJ21:BJ26"/>
-    <mergeCell ref="BK21:BK26"/>
-    <mergeCell ref="BL21:BL26"/>
-    <mergeCell ref="BM21:BM26"/>
-    <mergeCell ref="BN21:BN26"/>
-    <mergeCell ref="BP21:BP26"/>
-    <mergeCell ref="BD21:BD28"/>
-    <mergeCell ref="BC21:BC28"/>
-    <mergeCell ref="AG21:AG26"/>
-    <mergeCell ref="AH21:AH26"/>
-    <mergeCell ref="AI21:AI26"/>
-    <mergeCell ref="AJ21:AJ26"/>
-    <mergeCell ref="AL21:AL26"/>
-    <mergeCell ref="AX21:AX26"/>
-    <mergeCell ref="AR21:AR26"/>
-    <mergeCell ref="BJ45:BJ48"/>
-    <mergeCell ref="BQ21:BQ26"/>
-    <mergeCell ref="AU21:AU26"/>
-    <mergeCell ref="AV21:AV26"/>
-    <mergeCell ref="AT21:AT26"/>
-    <mergeCell ref="AY21:AY28"/>
-    <mergeCell ref="BA21:BA28"/>
-    <mergeCell ref="E21:E26"/>
-    <mergeCell ref="BY21:BY26"/>
-    <mergeCell ref="U21:U26"/>
-    <mergeCell ref="V21:V26"/>
-    <mergeCell ref="W21:W26"/>
-    <mergeCell ref="X21:X26"/>
-    <mergeCell ref="Y21:Y26"/>
-    <mergeCell ref="Z21:Z26"/>
-    <mergeCell ref="AK21:AK28"/>
-    <mergeCell ref="AO21:AO28"/>
-    <mergeCell ref="AS21:AS28"/>
-    <mergeCell ref="AW21:AW28"/>
-    <mergeCell ref="AZ21:AZ28"/>
-    <mergeCell ref="AM21:AM26"/>
-    <mergeCell ref="AN21:AN26"/>
-    <mergeCell ref="AP21:AP26"/>
-    <mergeCell ref="S21:S26"/>
-    <mergeCell ref="AE28:AE37"/>
-    <mergeCell ref="AB21:AB26"/>
-    <mergeCell ref="AC21:AC26"/>
-    <mergeCell ref="AD21:AD26"/>
-    <mergeCell ref="AE21:AE26"/>
-    <mergeCell ref="AQ21:AQ26"/>
-    <mergeCell ref="AF21:AF26"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="BE18:BE20"/>
-    <mergeCell ref="AY18:BD20"/>
-    <mergeCell ref="BF18:BF20"/>
-    <mergeCell ref="BG18:BG20"/>
-    <mergeCell ref="BH18:BH20"/>
-    <mergeCell ref="BI18:BJ20"/>
-    <mergeCell ref="BK18:BK20"/>
-    <mergeCell ref="A21:A26"/>
-    <mergeCell ref="B21:B26"/>
-    <mergeCell ref="C21:C26"/>
-    <mergeCell ref="L21:L26"/>
-    <mergeCell ref="BO18:CA20"/>
-    <mergeCell ref="A18:AX20"/>
-    <mergeCell ref="AE39:AE44"/>
-    <mergeCell ref="F21:F29"/>
-    <mergeCell ref="G21:G29"/>
-    <mergeCell ref="H21:H29"/>
-    <mergeCell ref="I21:I29"/>
-    <mergeCell ref="T21:T26"/>
-    <mergeCell ref="M21:M26"/>
-    <mergeCell ref="N21:N26"/>
-    <mergeCell ref="O21:O26"/>
-    <mergeCell ref="P21:P26"/>
-    <mergeCell ref="Q21:Q26"/>
-    <mergeCell ref="R21:R26"/>
-    <mergeCell ref="BO21:BO26"/>
-    <mergeCell ref="AA21:AA26"/>
-    <mergeCell ref="BL18:BN20"/>
-    <mergeCell ref="K21:K26"/>
-    <mergeCell ref="J21:J26"/>
-    <mergeCell ref="D21:D26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -7284,8 +7266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B3:L84"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L3" sqref="L3:L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7325,7 +7307,7 @@
         <v>CD_SITUACAO_NF,</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="L4" t="str">
         <f t="shared" ref="L4:L12" si="1">CONCATENATE("'",K4,"',")</f>
@@ -7363,7 +7345,7 @@
         <v>NR_REFERENCIA_FISCAL_FATURA,</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
       <c r="L6" t="str">
         <f t="shared" si="1"/>
@@ -7382,7 +7364,7 @@
         <v>NR_ITEM_NF_FATURA,</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" si="1"/>
@@ -7401,7 +7383,7 @@
         <v>NR_NF_FATURA,</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" si="1"/>
@@ -7420,7 +7402,7 @@
         <v>NR_SERIE_NF_FATURA,</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>426</v>
+        <v>417</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" si="1"/>
@@ -7439,7 +7421,7 @@
         <v>NR_NF_REMESSA,</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>447</v>
+        <v>437</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" si="1"/>
@@ -7458,7 +7440,7 @@
         <v>NR_SERIE_NF_REMESSA,</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>463</v>
+        <v>452</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" si="1"/>
@@ -7477,7 +7459,7 @@
         <v>NR_ORDEM,</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>489</v>
+        <v>478</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Revert "Views WMS Nike"
This reverts commit 9a5996c4e80a009fb93fc2c3617e272c67cf9c4e.
</commit_message>
<xml_diff>
--- a/Documentação/Planilhas/Conferencia_FAT.xlsx
+++ b/Documentação/Planilhas/Conferencia_FAT.xlsx
@@ -654,6 +654,9 @@
     <t>Sessão cislil504m00l (Nota Fiscal)</t>
   </si>
   <si>
+    <t>Fazer o detalhamento da Referência Fiscal desejada. Na aba superior "Geral", seção "Datas", pegar a informação da coluna "Data da Geração"</t>
+  </si>
+  <si>
     <t>Fazer o detalhamento da Referência Fiscal desejada. Na aba inferior Linhas - Nota Fiscal, pegar a informação da coluna "Quantidade" do item desejado</t>
   </si>
   <si>
@@ -1445,9 +1448,6 @@
   </si>
   <si>
     <t>Pegar a informação da coluna "Tipo Doc. Fiscal" . Se for "Fatura Op. Triangular", pedir o detalhamento da Referência Fiscal e na aba inferior "Linhas Nota Fiscal", pegar a informação da coluna "Linha" da Referência Fiscal Relativa, referente ao item vendido</t>
-  </si>
-  <si>
-    <t>Fazer o detalhamento da Referência Fiscal desejada. Na aba superior "Geral", seção "Datas", pegar a informação da coluna "Data da Emissão"</t>
   </si>
 </sst>
 </file>
@@ -1811,114 +1811,6 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1949,6 +1841,24 @@
     <xf numFmtId="49" fontId="4" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="4" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1960,6 +1870,96 @@
     </xf>
     <xf numFmtId="49" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2420,16 +2420,16 @@
         <v>198</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C7" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>256</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>255</v>
-      </c>
       <c r="E7" s="8" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>26</v>
@@ -2440,16 +2440,16 @@
         <v>198</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C8" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>259</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>258</v>
-      </c>
       <c r="E8" s="8" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="F8" s="8" t="s">
         <v>26</v>
@@ -2460,16 +2460,16 @@
         <v>198</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C9" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>253</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>252</v>
-      </c>
       <c r="E9" s="8" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>26</v>
@@ -2480,16 +2480,16 @@
         <v>198</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C10" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>249</v>
-      </c>
       <c r="E10" s="8" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="F10" s="8" t="s">
         <v>26</v>
@@ -2500,16 +2500,16 @@
         <v>199</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>26</v>
@@ -2520,16 +2520,16 @@
         <v>199</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C12" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>264</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>265</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>263</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>26</v>
@@ -2540,16 +2540,16 @@
         <v>199</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C13" s="11" t="s">
+        <v>257</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>256</v>
       </c>
-      <c r="D13" s="8" t="s">
-        <v>255</v>
-      </c>
       <c r="E13" s="8" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="F13" s="8" t="s">
         <v>26</v>
@@ -2560,16 +2560,16 @@
         <v>199</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="F14" s="8" t="s">
         <v>0</v>
@@ -2577,19 +2577,19 @@
     </row>
     <row r="15" spans="1:62">
       <c r="A15" s="8" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>26</v>
@@ -2597,19 +2597,19 @@
     </row>
     <row r="16" spans="1:62">
       <c r="A16" s="8" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="F16" s="8" t="s">
         <v>26</v>
@@ -2617,19 +2617,19 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="8" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>0</v>
@@ -2637,7 +2637,7 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="22" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B19" s="23"/>
       <c r="C19" s="23"/>
@@ -2729,8 +2729,8 @@
   </sheetPr>
   <dimension ref="A1:CD80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="BD1" workbookViewId="0">
+      <selection activeCell="BF6" sqref="BF6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -2857,10 +2857,10 @@
         <v>7</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>18</v>
@@ -3096,22 +3096,22 @@
     </row>
     <row r="7" spans="1:82" s="9" customFormat="1">
       <c r="A7" s="13" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>87</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="G7" s="13" t="s">
         <v>0</v>
@@ -3123,46 +3123,46 @@
         <v>86</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="K7" s="13" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="M7" s="13" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="N7" s="13" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="O7" s="13" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="P7" s="13" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="Q7" s="13" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="R7" s="13" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="S7" s="13" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="T7" s="13" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="U7" s="13" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="V7" s="13" t="s">
         <v>91</v>
       </c>
       <c r="W7" s="13" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="X7" s="13" t="s">
         <v>25</v>
@@ -3177,10 +3177,10 @@
         <v>88</v>
       </c>
       <c r="AB7" s="13" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="AC7" s="13" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AD7" s="13" t="s">
         <v>88</v>
@@ -3249,31 +3249,31 @@
         <v>93</v>
       </c>
       <c r="AZ7" s="13" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="BA7" s="13" t="s">
         <v>93</v>
       </c>
       <c r="BB7" s="13" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="BC7" s="13" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="BD7" s="13" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="BE7" s="13" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="BF7" s="13" t="s">
         <v>26</v>
       </c>
       <c r="BG7" s="13" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="BH7" s="13" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="BI7" s="13" t="s">
         <v>92</v>
@@ -3285,13 +3285,13 @@
         <v>0</v>
       </c>
       <c r="BL7" s="13" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="BM7" s="13" t="s">
         <v>0</v>
       </c>
       <c r="BN7" s="13" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="BO7" s="13" t="s">
         <v>0</v>
@@ -3300,25 +3300,25 @@
         <v>87</v>
       </c>
       <c r="BQ7" s="13" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="BR7" s="13" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="BS7" s="13" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="BT7" s="13" t="s">
         <v>85</v>
       </c>
       <c r="BU7" s="13" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="BV7" s="13" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="BW7" s="13" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="BX7" s="13" t="s">
         <v>0</v>
@@ -3333,7 +3333,7 @@
         <v>88</v>
       </c>
       <c r="CB7" s="13" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="CC7" s="13" t="s">
         <v>0</v>
@@ -3344,22 +3344,22 @@
     </row>
     <row r="8" spans="1:82" s="9" customFormat="1">
       <c r="A8" s="8" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>87</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>0</v>
@@ -3371,46 +3371,46 @@
         <v>86</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="N8" s="8" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="O8" s="8" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="P8" s="8" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="Q8" s="8" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="R8" s="8" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="S8" s="8" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="T8" s="8" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="U8" s="8" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="V8" s="8" t="s">
         <v>91</v>
       </c>
       <c r="W8" s="8" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="X8" s="8" t="s">
         <v>25</v>
@@ -3425,10 +3425,10 @@
         <v>88</v>
       </c>
       <c r="AB8" s="8" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="AC8" s="8" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AD8" s="8" t="s">
         <v>88</v>
@@ -3497,31 +3497,31 @@
         <v>93</v>
       </c>
       <c r="AZ8" s="8" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="BA8" s="8" t="s">
         <v>93</v>
       </c>
       <c r="BB8" s="8" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="BC8" s="8" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="BD8" s="8" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="BE8" s="8" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="BF8" s="8" t="s">
         <v>26</v>
       </c>
       <c r="BG8" s="8" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="BH8" s="8" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="BI8" s="8" t="s">
         <v>25</v>
@@ -3533,13 +3533,13 @@
         <v>0</v>
       </c>
       <c r="BL8" s="8" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="BM8" s="8" t="s">
         <v>0</v>
       </c>
       <c r="BN8" s="8" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="BO8" s="8" t="s">
         <v>0</v>
@@ -3548,25 +3548,25 @@
         <v>87</v>
       </c>
       <c r="BQ8" s="8" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="BR8" s="8" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="BS8" s="8" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="BT8" s="8" t="s">
         <v>85</v>
       </c>
       <c r="BU8" s="8" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="BV8" s="8" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="BW8" s="8" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="BX8" s="8" t="s">
         <v>0</v>
@@ -3581,7 +3581,7 @@
         <v>88</v>
       </c>
       <c r="CB8" s="8" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="CC8" s="8" t="s">
         <v>0</v>
@@ -3592,19 +3592,19 @@
     </row>
     <row r="9" spans="1:82" s="9" customFormat="1">
       <c r="A9" s="8" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>87</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="F9" s="8" t="s">
         <v>85</v>
@@ -3613,22 +3613,22 @@
         <v>86</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="J9" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>364</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>365</v>
+      </c>
+      <c r="M9" s="8" t="s">
         <v>323</v>
-      </c>
-      <c r="K9" s="8" t="s">
-        <v>363</v>
-      </c>
-      <c r="L9" s="8" t="s">
-        <v>364</v>
-      </c>
-      <c r="M9" s="8" t="s">
-        <v>322</v>
       </c>
       <c r="N9" s="8" t="s">
         <v>0</v>
@@ -3640,10 +3640,10 @@
         <v>158</v>
       </c>
       <c r="Q9" s="8" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="R9" s="8" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="S9" s="8" t="s">
         <v>86</v>
@@ -3658,16 +3658,16 @@
         <v>91</v>
       </c>
       <c r="W9" s="8" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="X9" s="8" t="s">
         <v>25</v>
       </c>
       <c r="Y9" s="8" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="Z9" s="8" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="AA9" s="8" t="s">
         <v>88</v>
@@ -3685,43 +3685,43 @@
         <v>88</v>
       </c>
       <c r="AF9" s="8" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="AG9" s="8" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="AH9" s="8" t="s">
         <v>85</v>
       </c>
       <c r="AI9" s="8" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="AJ9" s="8" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="AK9" s="8" t="s">
         <v>88</v>
       </c>
       <c r="AL9" s="8" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="AM9" s="8" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="AN9" s="8" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="AO9" s="8" t="s">
         <v>88</v>
       </c>
       <c r="AP9" s="8" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="AQ9" s="8" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="AR9" s="8" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="AS9" s="8" t="s">
         <v>88</v>
@@ -3742,34 +3742,34 @@
         <v>85</v>
       </c>
       <c r="AY9" s="8" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="AZ9" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="BA9" s="8" t="s">
         <v>379</v>
       </c>
-      <c r="BA9" s="8" t="s">
-        <v>378</v>
-      </c>
       <c r="BB9" s="8" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="BC9" s="8" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="BD9" s="8" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="BE9" s="8" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="BF9" s="8" t="s">
         <v>26</v>
       </c>
       <c r="BG9" s="8" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="BH9" s="8" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="BI9" s="8" t="s">
         <v>92</v>
@@ -3781,13 +3781,13 @@
         <v>0</v>
       </c>
       <c r="BL9" s="8" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="BM9" s="8" t="s">
         <v>0</v>
       </c>
       <c r="BN9" s="8" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="BO9" s="8" t="s">
         <v>0</v>
@@ -3796,25 +3796,25 @@
         <v>87</v>
       </c>
       <c r="BQ9" s="8" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="BR9" s="8" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="BS9" s="8" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="BT9" s="8" t="s">
         <v>85</v>
       </c>
       <c r="BU9" s="8" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="BV9" s="8" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="BW9" s="8" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="BX9" s="8" t="s">
         <v>0</v>
@@ -3829,7 +3829,7 @@
         <v>88</v>
       </c>
       <c r="CB9" s="8" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="CC9" s="8" t="s">
         <v>0</v>
@@ -3840,22 +3840,22 @@
     </row>
     <row r="10" spans="1:82" s="9" customFormat="1">
       <c r="A10" s="8" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>87</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>0</v>
@@ -3867,46 +3867,46 @@
         <v>86</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="M10" s="8" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="N10" s="8" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="O10" s="8" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="P10" s="8" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="Q10" s="8" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="R10" s="8" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="S10" s="8" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="T10" s="8" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="U10" s="8" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="V10" s="8" t="s">
         <v>91</v>
       </c>
       <c r="W10" s="8" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="X10" s="8" t="s">
         <v>25</v>
@@ -3921,10 +3921,10 @@
         <v>88</v>
       </c>
       <c r="AB10" s="8" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="AC10" s="8" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AD10" s="8" t="s">
         <v>88</v>
@@ -3993,31 +3993,31 @@
         <v>93</v>
       </c>
       <c r="AZ10" s="8" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="BA10" s="8" t="s">
         <v>93</v>
       </c>
       <c r="BB10" s="8" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="BC10" s="8" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="BD10" s="8" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="BE10" s="8" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="BF10" s="8" t="s">
         <v>26</v>
       </c>
       <c r="BG10" s="8" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="BH10" s="8" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="BI10" s="8" t="s">
         <v>92</v>
@@ -4029,13 +4029,13 @@
         <v>0</v>
       </c>
       <c r="BL10" s="8" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="BM10" s="8" t="s">
         <v>0</v>
       </c>
       <c r="BN10" s="8" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="BO10" s="8" t="s">
         <v>0</v>
@@ -4044,25 +4044,25 @@
         <v>87</v>
       </c>
       <c r="BQ10" s="8" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="BR10" s="8" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="BS10" s="8" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="BT10" s="8" t="s">
         <v>85</v>
       </c>
       <c r="BU10" s="8" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="BV10" s="8" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="BW10" s="8" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="BX10" s="8" t="s">
         <v>0</v>
@@ -4077,7 +4077,7 @@
         <v>88</v>
       </c>
       <c r="CB10" s="8" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="CC10" s="8" t="s">
         <v>0</v>
@@ -4088,19 +4088,19 @@
     </row>
     <row r="11" spans="1:82" s="9" customFormat="1">
       <c r="A11" s="8" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>87</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="F11" s="8" t="s">
         <v>85</v>
@@ -4109,22 +4109,22 @@
         <v>86</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="J11" s="8" t="s">
+        <v>386</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>393</v>
+      </c>
+      <c r="M11" s="8" t="s">
         <v>385</v>
-      </c>
-      <c r="K11" s="8" t="s">
-        <v>391</v>
-      </c>
-      <c r="L11" s="8" t="s">
-        <v>392</v>
-      </c>
-      <c r="M11" s="8" t="s">
-        <v>384</v>
       </c>
       <c r="N11" s="8" t="s">
         <v>0</v>
@@ -4136,10 +4136,10 @@
         <v>158</v>
       </c>
       <c r="Q11" s="8" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="R11" s="8" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="S11" s="8" t="s">
         <v>86</v>
@@ -4154,16 +4154,16 @@
         <v>91</v>
       </c>
       <c r="W11" s="8" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="X11" s="8" t="s">
         <v>25</v>
       </c>
       <c r="Y11" s="8" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="Z11" s="8" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="AA11" s="8" t="s">
         <v>88</v>
@@ -4181,43 +4181,43 @@
         <v>88</v>
       </c>
       <c r="AF11" s="8" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="AG11" s="8" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="AH11" s="8" t="s">
         <v>85</v>
       </c>
       <c r="AI11" s="8" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="AJ11" s="8" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="AK11" s="8" t="s">
         <v>88</v>
       </c>
       <c r="AL11" s="8" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="AM11" s="8" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="AN11" s="8" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="AO11" s="8" t="s">
         <v>88</v>
       </c>
       <c r="AP11" s="8" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="AQ11" s="8" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="AR11" s="8" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="AS11" s="8" t="s">
         <v>88</v>
@@ -4238,34 +4238,34 @@
         <v>85</v>
       </c>
       <c r="AY11" s="8" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="AZ11" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="BA11" s="8" t="s">
         <v>379</v>
       </c>
-      <c r="BA11" s="8" t="s">
-        <v>378</v>
-      </c>
       <c r="BB11" s="8" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="BC11" s="8" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="BD11" s="8" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="BE11" s="8" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="BF11" s="8" t="s">
         <v>26</v>
       </c>
       <c r="BG11" s="8" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="BH11" s="8" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="BI11" s="8" t="s">
         <v>92</v>
@@ -4277,13 +4277,13 @@
         <v>0</v>
       </c>
       <c r="BL11" s="8" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="BM11" s="8" t="s">
         <v>0</v>
       </c>
       <c r="BN11" s="8" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="BO11" s="8" t="s">
         <v>0</v>
@@ -4292,25 +4292,25 @@
         <v>87</v>
       </c>
       <c r="BQ11" s="8" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="BR11" s="8" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="BS11" s="8" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="BT11" s="8" t="s">
         <v>85</v>
       </c>
       <c r="BU11" s="8" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="BV11" s="8" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="BW11" s="8" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="BX11" s="8" t="s">
         <v>0</v>
@@ -4325,7 +4325,7 @@
         <v>88</v>
       </c>
       <c r="CB11" s="8" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="CC11" s="8" t="s">
         <v>0</v>
@@ -4336,19 +4336,19 @@
     </row>
     <row r="12" spans="1:82" s="9" customFormat="1">
       <c r="A12" s="8" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>87</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="F12" s="8" t="s">
         <v>85</v>
@@ -4363,46 +4363,46 @@
         <v>86</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="M12" s="8" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="N12" s="8" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="O12" s="8" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="P12" s="8" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="Q12" s="8" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="R12" s="8" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="S12" s="8" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="T12" s="8" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="U12" s="8" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="V12" s="8" t="s">
         <v>91</v>
       </c>
       <c r="W12" s="8" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="X12" s="8" t="s">
         <v>25</v>
@@ -4417,10 +4417,10 @@
         <v>88</v>
       </c>
       <c r="AB12" s="8" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="AC12" s="8" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AD12" s="8" t="s">
         <v>88</v>
@@ -4489,31 +4489,31 @@
         <v>93</v>
       </c>
       <c r="AZ12" s="8" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="BA12" s="8" t="s">
         <v>93</v>
       </c>
       <c r="BB12" s="8" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="BC12" s="8" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="BD12" s="8" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="BE12" s="8" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="BF12" s="8" t="s">
         <v>26</v>
       </c>
       <c r="BG12" s="8" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="BH12" s="8" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="BI12" s="8" t="s">
         <v>92</v>
@@ -4525,13 +4525,13 @@
         <v>0</v>
       </c>
       <c r="BL12" s="8" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="BM12" s="8" t="s">
         <v>0</v>
       </c>
       <c r="BN12" s="8" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="BO12" s="8" t="s">
         <v>0</v>
@@ -4540,25 +4540,25 @@
         <v>87</v>
       </c>
       <c r="BQ12" s="8" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="BR12" s="8" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="BS12" s="8" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="BT12" s="8" t="s">
         <v>85</v>
       </c>
       <c r="BU12" s="8" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="BV12" s="8" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="BW12" s="8" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="BX12" s="8" t="s">
         <v>0</v>
@@ -4584,22 +4584,22 @@
     </row>
     <row r="13" spans="1:82" s="9" customFormat="1">
       <c r="A13" s="8" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>87</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>0</v>
@@ -4611,46 +4611,46 @@
         <v>86</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="M13" s="8" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="N13" s="8" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="O13" s="8" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="P13" s="8" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="Q13" s="8" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="R13" s="8" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="S13" s="8" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="T13" s="8" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="U13" s="8" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="V13" s="8" t="s">
         <v>91</v>
       </c>
       <c r="W13" s="8" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="X13" s="8" t="s">
         <v>25</v>
@@ -4665,10 +4665,10 @@
         <v>88</v>
       </c>
       <c r="AB13" s="8" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="AC13" s="8" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AD13" s="8" t="s">
         <v>88</v>
@@ -4737,31 +4737,31 @@
         <v>93</v>
       </c>
       <c r="AZ13" s="8" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="BA13" s="8" t="s">
         <v>93</v>
       </c>
       <c r="BB13" s="8" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="BC13" s="8" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="BD13" s="8" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="BE13" s="8" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="BF13" s="8" t="s">
         <v>26</v>
       </c>
       <c r="BG13" s="8" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="BH13" s="8" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="BI13" s="8" t="s">
         <v>92</v>
@@ -4773,13 +4773,13 @@
         <v>0</v>
       </c>
       <c r="BL13" s="8" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="BM13" s="8" t="s">
         <v>0</v>
       </c>
       <c r="BN13" s="8" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="BO13" s="8" t="s">
         <v>0</v>
@@ -4788,25 +4788,25 @@
         <v>91</v>
       </c>
       <c r="BQ13" s="8" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="BR13" s="8" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="BS13" s="8" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="BT13" s="8" t="s">
         <v>85</v>
       </c>
       <c r="BU13" s="8" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="BV13" s="8" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="BW13" s="8" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="BX13" s="8" t="s">
         <v>0</v>
@@ -4821,7 +4821,7 @@
         <v>88</v>
       </c>
       <c r="CB13" s="8" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="CC13" s="8" t="s">
         <v>0</v>
@@ -4832,22 +4832,22 @@
     </row>
     <row r="14" spans="1:82" s="9" customFormat="1">
       <c r="A14" s="8" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>87</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="G14" s="8" t="s">
         <v>0</v>
@@ -4859,34 +4859,34 @@
         <v>86</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="M14" s="8" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="N14" s="8" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="O14" s="8" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="P14" s="8" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="Q14" s="8" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="R14" s="8" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="S14" s="8" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="T14" s="8" t="s">
         <v>25</v>
@@ -4898,7 +4898,7 @@
         <v>91</v>
       </c>
       <c r="W14" s="8" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="X14" s="8" t="s">
         <v>25</v>
@@ -4913,10 +4913,10 @@
         <v>88</v>
       </c>
       <c r="AB14" s="8" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="AC14" s="8" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="AD14" s="8" t="s">
         <v>88</v>
@@ -4985,13 +4985,13 @@
         <v>93</v>
       </c>
       <c r="AZ14" s="8" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="BA14" s="8" t="s">
         <v>93</v>
       </c>
       <c r="BB14" s="8" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="BC14" s="8" t="s">
         <v>90</v>
@@ -5000,16 +5000,16 @@
         <v>90</v>
       </c>
       <c r="BE14" s="8" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="BF14" s="8" t="s">
         <v>26</v>
       </c>
       <c r="BG14" s="8" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="BH14" s="8" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="BI14" s="8" t="s">
         <v>92</v>
@@ -5021,13 +5021,13 @@
         <v>0</v>
       </c>
       <c r="BL14" s="8" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="BM14" s="8" t="s">
         <v>0</v>
       </c>
       <c r="BN14" s="8" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="BO14" s="8" t="s">
         <v>0</v>
@@ -5039,7 +5039,7 @@
         <v>89</v>
       </c>
       <c r="BR14" s="8" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="BS14" s="8" t="s">
         <v>85</v>
@@ -5048,13 +5048,13 @@
         <v>85</v>
       </c>
       <c r="BU14" s="8" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="BV14" s="8" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="BW14" s="8" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="BX14" s="8" t="s">
         <v>0</v>
@@ -5080,19 +5080,19 @@
     </row>
     <row r="15" spans="1:82" s="9" customFormat="1">
       <c r="A15" s="8" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>87</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="F15" s="8" t="s">
         <v>85</v>
@@ -5101,22 +5101,22 @@
         <v>86</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="J15" s="8" t="s">
+        <v>422</v>
+      </c>
+      <c r="K15" s="8" t="s">
+        <v>438</v>
+      </c>
+      <c r="L15" s="8" t="s">
+        <v>439</v>
+      </c>
+      <c r="M15" s="8" t="s">
         <v>421</v>
-      </c>
-      <c r="K15" s="8" t="s">
-        <v>437</v>
-      </c>
-      <c r="L15" s="8" t="s">
-        <v>438</v>
-      </c>
-      <c r="M15" s="8" t="s">
-        <v>420</v>
       </c>
       <c r="N15" s="8" t="s">
         <v>0</v>
@@ -5128,10 +5128,10 @@
         <v>158</v>
       </c>
       <c r="Q15" s="8" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="R15" s="8" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="S15" s="8" t="s">
         <v>86</v>
@@ -5146,16 +5146,16 @@
         <v>91</v>
       </c>
       <c r="W15" s="8" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="X15" s="8" t="s">
         <v>25</v>
       </c>
       <c r="Y15" s="8" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="Z15" s="8" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="AA15" s="8" t="s">
         <v>88</v>
@@ -5191,28 +5191,28 @@
         <v>88</v>
       </c>
       <c r="AL15" s="8" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="AM15" s="8" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="AN15" s="8" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="AO15" s="8" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="AP15" s="8" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="AQ15" s="8" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="AR15" s="8" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="AS15" s="8" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="AT15" s="8" t="s">
         <v>88</v>
@@ -5233,13 +5233,13 @@
         <v>93</v>
       </c>
       <c r="AZ15" s="8" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="BA15" s="8" t="s">
         <v>93</v>
       </c>
       <c r="BB15" s="8" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="BC15" s="8" t="s">
         <v>90</v>
@@ -5248,16 +5248,16 @@
         <v>90</v>
       </c>
       <c r="BE15" s="8" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="BF15" s="8" t="s">
         <v>26</v>
       </c>
       <c r="BG15" s="8" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="BH15" s="8" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="BI15" s="8" t="s">
         <v>92</v>
@@ -5269,13 +5269,13 @@
         <v>0</v>
       </c>
       <c r="BL15" s="8" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="BM15" s="8" t="s">
         <v>0</v>
       </c>
       <c r="BN15" s="8" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="BO15" s="8" t="s">
         <v>0</v>
@@ -5287,7 +5287,7 @@
         <v>89</v>
       </c>
       <c r="BR15" s="8" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="BS15" s="8" t="s">
         <v>85</v>
@@ -5296,13 +5296,13 @@
         <v>85</v>
       </c>
       <c r="BU15" s="8" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="BV15" s="8" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="BW15" s="8" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="BX15" s="8" t="s">
         <v>0</v>
@@ -5328,22 +5328,22 @@
     </row>
     <row r="16" spans="1:82" s="9" customFormat="1">
       <c r="A16" s="8" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>91</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="G16" s="8" t="s">
         <v>0</v>
@@ -5355,46 +5355,46 @@
         <v>86</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="K16" s="8" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="L16" s="8" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="M16" s="8" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="N16" s="8" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="O16" s="8" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="P16" s="8" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="Q16" s="8" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="R16" s="8" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="S16" s="8" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="T16" s="8" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="U16" s="8" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="V16" s="8" t="s">
         <v>26</v>
       </c>
       <c r="W16" s="8" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="X16" s="8" t="s">
         <v>25</v>
@@ -5409,10 +5409,10 @@
         <v>88</v>
       </c>
       <c r="AB16" s="8" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="AC16" s="8" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AD16" s="8" t="s">
         <v>88</v>
@@ -5481,31 +5481,31 @@
         <v>93</v>
       </c>
       <c r="AZ16" s="8" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="BA16" s="8" t="s">
         <v>93</v>
       </c>
       <c r="BB16" s="8" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="BC16" s="8" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="BD16" s="8" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="BE16" s="8" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="BF16" s="8" t="s">
         <v>26</v>
       </c>
       <c r="BG16" s="8" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="BH16" s="8" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="BI16" s="8" t="s">
         <v>92</v>
@@ -5517,13 +5517,13 @@
         <v>0</v>
       </c>
       <c r="BL16" s="8" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="BM16" s="8" t="s">
         <v>0</v>
       </c>
       <c r="BN16" s="8" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="BO16" s="8" t="s">
         <v>0</v>
@@ -5532,25 +5532,25 @@
         <v>87</v>
       </c>
       <c r="BQ16" s="8" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="BR16" s="8" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="BS16" s="8" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="BT16" s="8" t="s">
         <v>85</v>
       </c>
       <c r="BU16" s="8" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="BV16" s="8" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="BW16" s="8" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="BX16" s="8" t="s">
         <v>0</v>
@@ -5565,7 +5565,7 @@
         <v>88</v>
       </c>
       <c r="CB16" s="8" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="CC16" s="8" t="s">
         <v>0</v>
@@ -5575,275 +5575,275 @@
       </c>
     </row>
     <row r="18" spans="1:82" ht="15" customHeight="1">
-      <c r="A18" s="69" t="s">
+      <c r="A18" s="33" t="s">
         <v>209</v>
       </c>
-      <c r="B18" s="70"/>
-      <c r="C18" s="70"/>
-      <c r="D18" s="70"/>
-      <c r="E18" s="70"/>
-      <c r="F18" s="70"/>
-      <c r="G18" s="70"/>
-      <c r="H18" s="70"/>
-      <c r="I18" s="70"/>
-      <c r="J18" s="70"/>
-      <c r="K18" s="70"/>
-      <c r="L18" s="70"/>
-      <c r="M18" s="70"/>
-      <c r="N18" s="70"/>
-      <c r="O18" s="70"/>
-      <c r="P18" s="70"/>
-      <c r="Q18" s="70"/>
-      <c r="R18" s="70"/>
-      <c r="S18" s="70"/>
-      <c r="T18" s="70"/>
-      <c r="U18" s="70"/>
-      <c r="V18" s="70"/>
-      <c r="W18" s="70"/>
-      <c r="X18" s="70"/>
-      <c r="Y18" s="70"/>
-      <c r="Z18" s="70"/>
-      <c r="AA18" s="70"/>
-      <c r="AB18" s="70"/>
-      <c r="AC18" s="70"/>
-      <c r="AD18" s="70"/>
-      <c r="AE18" s="70"/>
-      <c r="AF18" s="70"/>
-      <c r="AG18" s="70"/>
-      <c r="AH18" s="70"/>
-      <c r="AI18" s="70"/>
-      <c r="AJ18" s="70"/>
-      <c r="AK18" s="70"/>
-      <c r="AL18" s="70"/>
-      <c r="AM18" s="70"/>
-      <c r="AN18" s="70"/>
-      <c r="AO18" s="70"/>
-      <c r="AP18" s="70"/>
-      <c r="AQ18" s="70"/>
-      <c r="AR18" s="70"/>
-      <c r="AS18" s="70"/>
-      <c r="AT18" s="70"/>
-      <c r="AU18" s="70"/>
-      <c r="AV18" s="70"/>
-      <c r="AW18" s="70"/>
-      <c r="AX18" s="71"/>
-      <c r="AY18" s="69" t="s">
-        <v>237</v>
-      </c>
-      <c r="AZ18" s="70"/>
-      <c r="BA18" s="70"/>
-      <c r="BB18" s="70"/>
-      <c r="BC18" s="70"/>
-      <c r="BD18" s="71"/>
-      <c r="BE18" s="78" t="s">
-        <v>240</v>
-      </c>
-      <c r="BF18" s="78" t="s">
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="34"/>
+      <c r="L18" s="34"/>
+      <c r="M18" s="34"/>
+      <c r="N18" s="34"/>
+      <c r="O18" s="34"/>
+      <c r="P18" s="34"/>
+      <c r="Q18" s="34"/>
+      <c r="R18" s="34"/>
+      <c r="S18" s="34"/>
+      <c r="T18" s="34"/>
+      <c r="U18" s="34"/>
+      <c r="V18" s="34"/>
+      <c r="W18" s="34"/>
+      <c r="X18" s="34"/>
+      <c r="Y18" s="34"/>
+      <c r="Z18" s="34"/>
+      <c r="AA18" s="34"/>
+      <c r="AB18" s="34"/>
+      <c r="AC18" s="34"/>
+      <c r="AD18" s="34"/>
+      <c r="AE18" s="34"/>
+      <c r="AF18" s="34"/>
+      <c r="AG18" s="34"/>
+      <c r="AH18" s="34"/>
+      <c r="AI18" s="34"/>
+      <c r="AJ18" s="34"/>
+      <c r="AK18" s="34"/>
+      <c r="AL18" s="34"/>
+      <c r="AM18" s="34"/>
+      <c r="AN18" s="34"/>
+      <c r="AO18" s="34"/>
+      <c r="AP18" s="34"/>
+      <c r="AQ18" s="34"/>
+      <c r="AR18" s="34"/>
+      <c r="AS18" s="34"/>
+      <c r="AT18" s="34"/>
+      <c r="AU18" s="34"/>
+      <c r="AV18" s="34"/>
+      <c r="AW18" s="34"/>
+      <c r="AX18" s="35"/>
+      <c r="AY18" s="33" t="s">
+        <v>238</v>
+      </c>
+      <c r="AZ18" s="34"/>
+      <c r="BA18" s="34"/>
+      <c r="BB18" s="34"/>
+      <c r="BC18" s="34"/>
+      <c r="BD18" s="35"/>
+      <c r="BE18" s="48" t="s">
         <v>241</v>
       </c>
-      <c r="BG18" s="78" t="s">
-        <v>238</v>
-      </c>
-      <c r="BH18" s="78" t="s">
-        <v>247</v>
-      </c>
-      <c r="BI18" s="81" t="s">
+      <c r="BF18" s="48" t="s">
         <v>242</v>
       </c>
-      <c r="BJ18" s="81"/>
-      <c r="BK18" s="78" t="s">
+      <c r="BG18" s="48" t="s">
+        <v>239</v>
+      </c>
+      <c r="BH18" s="48" t="s">
+        <v>248</v>
+      </c>
+      <c r="BI18" s="51" t="s">
         <v>243</v>
       </c>
+      <c r="BJ18" s="51"/>
+      <c r="BK18" s="48" t="s">
+        <v>244</v>
+      </c>
       <c r="BL18" s="22" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="BM18" s="23"/>
       <c r="BN18" s="24"/>
-      <c r="BO18" s="68" t="s">
-        <v>245</v>
-      </c>
-      <c r="BP18" s="68"/>
-      <c r="BQ18" s="68"/>
-      <c r="BR18" s="68"/>
-      <c r="BS18" s="68"/>
-      <c r="BT18" s="68"/>
-      <c r="BU18" s="68"/>
-      <c r="BV18" s="68"/>
-      <c r="BW18" s="68"/>
-      <c r="BX18" s="68"/>
-      <c r="BY18" s="68"/>
-      <c r="BZ18" s="68"/>
-      <c r="CA18" s="68"/>
-      <c r="CB18" s="38" t="s">
-        <v>294</v>
-      </c>
-      <c r="CC18" s="39"/>
+      <c r="BO18" s="32" t="s">
+        <v>246</v>
+      </c>
+      <c r="BP18" s="32"/>
+      <c r="BQ18" s="32"/>
+      <c r="BR18" s="32"/>
+      <c r="BS18" s="32"/>
+      <c r="BT18" s="32"/>
+      <c r="BU18" s="32"/>
+      <c r="BV18" s="32"/>
+      <c r="BW18" s="32"/>
+      <c r="BX18" s="32"/>
+      <c r="BY18" s="32"/>
+      <c r="BZ18" s="32"/>
+      <c r="CA18" s="32"/>
+      <c r="CB18" s="64" t="s">
+        <v>295</v>
+      </c>
+      <c r="CC18" s="65"/>
     </row>
     <row r="19" spans="1:82" ht="11.25" customHeight="1">
-      <c r="A19" s="72"/>
-      <c r="B19" s="73"/>
-      <c r="C19" s="73"/>
-      <c r="D19" s="73"/>
-      <c r="E19" s="73"/>
-      <c r="F19" s="73"/>
-      <c r="G19" s="73"/>
-      <c r="H19" s="73"/>
-      <c r="I19" s="73"/>
-      <c r="J19" s="73"/>
-      <c r="K19" s="73"/>
-      <c r="L19" s="73"/>
-      <c r="M19" s="73"/>
-      <c r="N19" s="73"/>
-      <c r="O19" s="73"/>
-      <c r="P19" s="73"/>
-      <c r="Q19" s="73"/>
-      <c r="R19" s="73"/>
-      <c r="S19" s="73"/>
-      <c r="T19" s="73"/>
-      <c r="U19" s="73"/>
-      <c r="V19" s="73"/>
-      <c r="W19" s="73"/>
-      <c r="X19" s="73"/>
-      <c r="Y19" s="73"/>
-      <c r="Z19" s="73"/>
-      <c r="AA19" s="73"/>
-      <c r="AB19" s="73"/>
-      <c r="AC19" s="73"/>
-      <c r="AD19" s="73"/>
-      <c r="AE19" s="73"/>
-      <c r="AF19" s="73"/>
-      <c r="AG19" s="73"/>
-      <c r="AH19" s="73"/>
-      <c r="AI19" s="73"/>
-      <c r="AJ19" s="73"/>
-      <c r="AK19" s="73"/>
-      <c r="AL19" s="73"/>
-      <c r="AM19" s="73"/>
-      <c r="AN19" s="73"/>
-      <c r="AO19" s="73"/>
-      <c r="AP19" s="73"/>
-      <c r="AQ19" s="73"/>
-      <c r="AR19" s="73"/>
-      <c r="AS19" s="73"/>
-      <c r="AT19" s="73"/>
-      <c r="AU19" s="73"/>
-      <c r="AV19" s="73"/>
-      <c r="AW19" s="73"/>
-      <c r="AX19" s="74"/>
-      <c r="AY19" s="72"/>
-      <c r="AZ19" s="73"/>
-      <c r="BA19" s="73"/>
-      <c r="BB19" s="73"/>
-      <c r="BC19" s="73"/>
-      <c r="BD19" s="74"/>
-      <c r="BE19" s="79"/>
-      <c r="BF19" s="79"/>
-      <c r="BG19" s="79"/>
-      <c r="BH19" s="79"/>
-      <c r="BI19" s="81"/>
-      <c r="BJ19" s="81"/>
-      <c r="BK19" s="79"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="37"/>
+      <c r="F19" s="37"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="37"/>
+      <c r="K19" s="37"/>
+      <c r="L19" s="37"/>
+      <c r="M19" s="37"/>
+      <c r="N19" s="37"/>
+      <c r="O19" s="37"/>
+      <c r="P19" s="37"/>
+      <c r="Q19" s="37"/>
+      <c r="R19" s="37"/>
+      <c r="S19" s="37"/>
+      <c r="T19" s="37"/>
+      <c r="U19" s="37"/>
+      <c r="V19" s="37"/>
+      <c r="W19" s="37"/>
+      <c r="X19" s="37"/>
+      <c r="Y19" s="37"/>
+      <c r="Z19" s="37"/>
+      <c r="AA19" s="37"/>
+      <c r="AB19" s="37"/>
+      <c r="AC19" s="37"/>
+      <c r="AD19" s="37"/>
+      <c r="AE19" s="37"/>
+      <c r="AF19" s="37"/>
+      <c r="AG19" s="37"/>
+      <c r="AH19" s="37"/>
+      <c r="AI19" s="37"/>
+      <c r="AJ19" s="37"/>
+      <c r="AK19" s="37"/>
+      <c r="AL19" s="37"/>
+      <c r="AM19" s="37"/>
+      <c r="AN19" s="37"/>
+      <c r="AO19" s="37"/>
+      <c r="AP19" s="37"/>
+      <c r="AQ19" s="37"/>
+      <c r="AR19" s="37"/>
+      <c r="AS19" s="37"/>
+      <c r="AT19" s="37"/>
+      <c r="AU19" s="37"/>
+      <c r="AV19" s="37"/>
+      <c r="AW19" s="37"/>
+      <c r="AX19" s="38"/>
+      <c r="AY19" s="36"/>
+      <c r="AZ19" s="37"/>
+      <c r="BA19" s="37"/>
+      <c r="BB19" s="37"/>
+      <c r="BC19" s="37"/>
+      <c r="BD19" s="38"/>
+      <c r="BE19" s="49"/>
+      <c r="BF19" s="49"/>
+      <c r="BG19" s="49"/>
+      <c r="BH19" s="49"/>
+      <c r="BI19" s="51"/>
+      <c r="BJ19" s="51"/>
+      <c r="BK19" s="49"/>
       <c r="BL19" s="25"/>
       <c r="BM19" s="26"/>
       <c r="BN19" s="27"/>
-      <c r="BO19" s="68"/>
-      <c r="BP19" s="68"/>
-      <c r="BQ19" s="68"/>
-      <c r="BR19" s="68"/>
-      <c r="BS19" s="68"/>
-      <c r="BT19" s="68"/>
-      <c r="BU19" s="68"/>
-      <c r="BV19" s="68"/>
-      <c r="BW19" s="68"/>
-      <c r="BX19" s="68"/>
-      <c r="BY19" s="68"/>
-      <c r="BZ19" s="68"/>
-      <c r="CA19" s="68"/>
-      <c r="CB19" s="40"/>
-      <c r="CC19" s="41"/>
+      <c r="BO19" s="32"/>
+      <c r="BP19" s="32"/>
+      <c r="BQ19" s="32"/>
+      <c r="BR19" s="32"/>
+      <c r="BS19" s="32"/>
+      <c r="BT19" s="32"/>
+      <c r="BU19" s="32"/>
+      <c r="BV19" s="32"/>
+      <c r="BW19" s="32"/>
+      <c r="BX19" s="32"/>
+      <c r="BY19" s="32"/>
+      <c r="BZ19" s="32"/>
+      <c r="CA19" s="32"/>
+      <c r="CB19" s="66"/>
+      <c r="CC19" s="67"/>
     </row>
     <row r="20" spans="1:82" ht="11.25" customHeight="1">
-      <c r="A20" s="75"/>
-      <c r="B20" s="76"/>
-      <c r="C20" s="76"/>
-      <c r="D20" s="76"/>
-      <c r="E20" s="76"/>
-      <c r="F20" s="76"/>
-      <c r="G20" s="76"/>
-      <c r="H20" s="76"/>
-      <c r="I20" s="76"/>
-      <c r="J20" s="76"/>
-      <c r="K20" s="76"/>
-      <c r="L20" s="76"/>
-      <c r="M20" s="76"/>
-      <c r="N20" s="76"/>
-      <c r="O20" s="76"/>
-      <c r="P20" s="76"/>
-      <c r="Q20" s="76"/>
-      <c r="R20" s="76"/>
-      <c r="S20" s="76"/>
-      <c r="T20" s="76"/>
-      <c r="U20" s="76"/>
-      <c r="V20" s="76"/>
-      <c r="W20" s="76"/>
-      <c r="X20" s="76"/>
-      <c r="Y20" s="76"/>
-      <c r="Z20" s="76"/>
-      <c r="AA20" s="76"/>
-      <c r="AB20" s="76"/>
-      <c r="AC20" s="76"/>
-      <c r="AD20" s="76"/>
-      <c r="AE20" s="76"/>
-      <c r="AF20" s="76"/>
-      <c r="AG20" s="76"/>
-      <c r="AH20" s="76"/>
-      <c r="AI20" s="76"/>
-      <c r="AJ20" s="76"/>
-      <c r="AK20" s="76"/>
-      <c r="AL20" s="76"/>
-      <c r="AM20" s="76"/>
-      <c r="AN20" s="76"/>
-      <c r="AO20" s="76"/>
-      <c r="AP20" s="76"/>
-      <c r="AQ20" s="76"/>
-      <c r="AR20" s="76"/>
-      <c r="AS20" s="76"/>
-      <c r="AT20" s="76"/>
-      <c r="AU20" s="76"/>
-      <c r="AV20" s="76"/>
-      <c r="AW20" s="76"/>
-      <c r="AX20" s="77"/>
-      <c r="AY20" s="75"/>
-      <c r="AZ20" s="76"/>
-      <c r="BA20" s="76"/>
-      <c r="BB20" s="76"/>
-      <c r="BC20" s="76"/>
-      <c r="BD20" s="77"/>
-      <c r="BE20" s="80"/>
-      <c r="BF20" s="80"/>
-      <c r="BG20" s="80"/>
-      <c r="BH20" s="80"/>
-      <c r="BI20" s="81"/>
-      <c r="BJ20" s="81"/>
-      <c r="BK20" s="80"/>
+      <c r="A20" s="39"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="40"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="40"/>
+      <c r="J20" s="40"/>
+      <c r="K20" s="40"/>
+      <c r="L20" s="40"/>
+      <c r="M20" s="40"/>
+      <c r="N20" s="40"/>
+      <c r="O20" s="40"/>
+      <c r="P20" s="40"/>
+      <c r="Q20" s="40"/>
+      <c r="R20" s="40"/>
+      <c r="S20" s="40"/>
+      <c r="T20" s="40"/>
+      <c r="U20" s="40"/>
+      <c r="V20" s="40"/>
+      <c r="W20" s="40"/>
+      <c r="X20" s="40"/>
+      <c r="Y20" s="40"/>
+      <c r="Z20" s="40"/>
+      <c r="AA20" s="40"/>
+      <c r="AB20" s="40"/>
+      <c r="AC20" s="40"/>
+      <c r="AD20" s="40"/>
+      <c r="AE20" s="40"/>
+      <c r="AF20" s="40"/>
+      <c r="AG20" s="40"/>
+      <c r="AH20" s="40"/>
+      <c r="AI20" s="40"/>
+      <c r="AJ20" s="40"/>
+      <c r="AK20" s="40"/>
+      <c r="AL20" s="40"/>
+      <c r="AM20" s="40"/>
+      <c r="AN20" s="40"/>
+      <c r="AO20" s="40"/>
+      <c r="AP20" s="40"/>
+      <c r="AQ20" s="40"/>
+      <c r="AR20" s="40"/>
+      <c r="AS20" s="40"/>
+      <c r="AT20" s="40"/>
+      <c r="AU20" s="40"/>
+      <c r="AV20" s="40"/>
+      <c r="AW20" s="40"/>
+      <c r="AX20" s="41"/>
+      <c r="AY20" s="39"/>
+      <c r="AZ20" s="40"/>
+      <c r="BA20" s="40"/>
+      <c r="BB20" s="40"/>
+      <c r="BC20" s="40"/>
+      <c r="BD20" s="41"/>
+      <c r="BE20" s="50"/>
+      <c r="BF20" s="50"/>
+      <c r="BG20" s="50"/>
+      <c r="BH20" s="50"/>
+      <c r="BI20" s="51"/>
+      <c r="BJ20" s="51"/>
+      <c r="BK20" s="50"/>
       <c r="BL20" s="28"/>
       <c r="BM20" s="29"/>
       <c r="BN20" s="30"/>
-      <c r="BO20" s="68"/>
-      <c r="BP20" s="68"/>
-      <c r="BQ20" s="68"/>
-      <c r="BR20" s="68"/>
-      <c r="BS20" s="68"/>
-      <c r="BT20" s="68"/>
-      <c r="BU20" s="68"/>
-      <c r="BV20" s="68"/>
-      <c r="BW20" s="68"/>
-      <c r="BX20" s="68"/>
-      <c r="BY20" s="68"/>
-      <c r="BZ20" s="68"/>
-      <c r="CA20" s="68"/>
-      <c r="CB20" s="42"/>
-      <c r="CC20" s="43"/>
+      <c r="BO20" s="32"/>
+      <c r="BP20" s="32"/>
+      <c r="BQ20" s="32"/>
+      <c r="BR20" s="32"/>
+      <c r="BS20" s="32"/>
+      <c r="BT20" s="32"/>
+      <c r="BU20" s="32"/>
+      <c r="BV20" s="32"/>
+      <c r="BW20" s="32"/>
+      <c r="BX20" s="32"/>
+      <c r="BY20" s="32"/>
+      <c r="BZ20" s="32"/>
+      <c r="CA20" s="32"/>
+      <c r="CB20" s="68"/>
+      <c r="CC20" s="69"/>
     </row>
     <row r="21" spans="1:82" ht="11.25" customHeight="1">
       <c r="A21" s="31" t="s">
@@ -5856,30 +5856,30 @@
         <v>97</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>465</v>
-      </c>
-      <c r="E21" s="61" t="s">
         <v>466</v>
       </c>
-      <c r="F21" s="65" t="s">
-        <v>229</v>
-      </c>
-      <c r="G21" s="65" t="s">
+      <c r="E21" s="56" t="s">
+        <v>467</v>
+      </c>
+      <c r="F21" s="73" t="s">
         <v>230</v>
       </c>
-      <c r="H21" s="65" t="s">
+      <c r="G21" s="73" t="s">
         <v>231</v>
       </c>
-      <c r="I21" s="65" t="s">
+      <c r="H21" s="73" t="s">
         <v>232</v>
       </c>
-      <c r="J21" s="35" t="s">
+      <c r="I21" s="73" t="s">
+        <v>233</v>
+      </c>
+      <c r="J21" s="42" t="s">
         <v>152</v>
       </c>
-      <c r="K21" s="35" t="s">
-        <v>467</v>
-      </c>
-      <c r="L21" s="35" t="s">
+      <c r="K21" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="L21" s="42" t="s">
         <v>150</v>
       </c>
       <c r="M21" s="31" t="s">
@@ -5900,8 +5900,8 @@
       <c r="R21" s="31" t="s">
         <v>147</v>
       </c>
-      <c r="S21" s="32" t="s">
-        <v>463</v>
+      <c r="S21" s="45" t="s">
+        <v>464</v>
       </c>
       <c r="T21" s="31" t="s">
         <v>183</v>
@@ -5912,125 +5912,125 @@
       <c r="V21" s="31" t="s">
         <v>171</v>
       </c>
-      <c r="W21" s="35" t="s">
+      <c r="W21" s="42" t="s">
         <v>156</v>
       </c>
-      <c r="X21" s="35" t="s">
-        <v>210</v>
-      </c>
-      <c r="Y21" s="35" t="s">
+      <c r="X21" s="42" t="s">
+        <v>211</v>
+      </c>
+      <c r="Y21" s="42" t="s">
         <v>165</v>
       </c>
-      <c r="Z21" s="35" t="s">
-        <v>211</v>
-      </c>
-      <c r="AA21" s="35" t="s">
+      <c r="Z21" s="42" t="s">
+        <v>212</v>
+      </c>
+      <c r="AA21" s="42" t="s">
         <v>164</v>
       </c>
-      <c r="AB21" s="32" t="s">
+      <c r="AB21" s="45" t="s">
         <v>172</v>
       </c>
-      <c r="AC21" s="32" t="s">
+      <c r="AC21" s="45" t="s">
         <v>173</v>
       </c>
-      <c r="AD21" s="32" t="s">
+      <c r="AD21" s="45" t="s">
         <v>166</v>
       </c>
-      <c r="AE21" s="32" t="s">
+      <c r="AE21" s="45" t="s">
         <v>167</v>
       </c>
-      <c r="AF21" s="32" t="s">
+      <c r="AF21" s="45" t="s">
         <v>176</v>
       </c>
-      <c r="AG21" s="35" t="s">
+      <c r="AG21" s="42" t="s">
         <v>159</v>
       </c>
-      <c r="AH21" s="32" t="s">
+      <c r="AH21" s="45" t="s">
         <v>162</v>
       </c>
-      <c r="AI21" s="32" t="s">
-        <v>217</v>
+      <c r="AI21" s="45" t="s">
+        <v>218</v>
       </c>
       <c r="AJ21" s="52" t="s">
-        <v>218</v>
-      </c>
-      <c r="AK21" s="44" t="s">
+        <v>219</v>
+      </c>
+      <c r="AK21" s="55" t="s">
+        <v>222</v>
+      </c>
+      <c r="AL21" s="58" t="s">
+        <v>160</v>
+      </c>
+      <c r="AM21" s="45" t="s">
+        <v>220</v>
+      </c>
+      <c r="AN21" s="52" t="s">
         <v>221</v>
       </c>
-      <c r="AL21" s="55" t="s">
-        <v>160</v>
-      </c>
-      <c r="AM21" s="32" t="s">
-        <v>219</v>
-      </c>
-      <c r="AN21" s="52" t="s">
-        <v>220</v>
-      </c>
-      <c r="AO21" s="44" t="s">
-        <v>222</v>
-      </c>
-      <c r="AP21" s="55" t="s">
+      <c r="AO21" s="55" t="s">
+        <v>223</v>
+      </c>
+      <c r="AP21" s="58" t="s">
         <v>161</v>
       </c>
-      <c r="AQ21" s="32" t="s">
+      <c r="AQ21" s="45" t="s">
+        <v>227</v>
+      </c>
+      <c r="AR21" s="52" t="s">
+        <v>224</v>
+      </c>
+      <c r="AS21" s="55" t="s">
+        <v>225</v>
+      </c>
+      <c r="AT21" s="45" t="s">
+        <v>163</v>
+      </c>
+      <c r="AU21" s="45" t="s">
         <v>226</v>
       </c>
-      <c r="AR21" s="52" t="s">
-        <v>223</v>
-      </c>
-      <c r="AS21" s="44" t="s">
-        <v>224</v>
-      </c>
-      <c r="AT21" s="32" t="s">
-        <v>163</v>
-      </c>
-      <c r="AU21" s="32" t="s">
-        <v>225</v>
-      </c>
       <c r="AV21" s="52" t="s">
-        <v>227</v>
-      </c>
-      <c r="AW21" s="44" t="s">
         <v>228</v>
+      </c>
+      <c r="AW21" s="55" t="s">
+        <v>229</v>
       </c>
       <c r="AX21" s="52" t="s">
         <v>177</v>
       </c>
-      <c r="AY21" s="44" t="s">
+      <c r="AY21" s="55" t="s">
+        <v>236</v>
+      </c>
+      <c r="AZ21" s="57" t="s">
+        <v>234</v>
+      </c>
+      <c r="BA21" s="55" t="s">
+        <v>237</v>
+      </c>
+      <c r="BB21" s="55" t="s">
         <v>235</v>
       </c>
-      <c r="AZ21" s="51" t="s">
-        <v>233</v>
-      </c>
-      <c r="BA21" s="44" t="s">
-        <v>236</v>
-      </c>
-      <c r="BB21" s="44" t="s">
-        <v>234</v>
-      </c>
-      <c r="BC21" s="44" t="s">
+      <c r="BC21" s="55" t="s">
         <v>188</v>
       </c>
-      <c r="BD21" s="44" t="s">
+      <c r="BD21" s="55" t="s">
         <v>189</v>
       </c>
-      <c r="BE21" s="58" t="s">
+      <c r="BE21" s="70" t="s">
         <v>190</v>
       </c>
-      <c r="BF21" s="32" t="s">
+      <c r="BF21" s="45" t="s">
         <v>151</v>
       </c>
-      <c r="BG21" s="32" t="s">
-        <v>239</v>
-      </c>
-      <c r="BH21" s="44" t="s">
-        <v>289</v>
-      </c>
-      <c r="BI21" s="44" t="s">
+      <c r="BG21" s="45" t="s">
+        <v>240</v>
+      </c>
+      <c r="BH21" s="55" t="s">
         <v>290</v>
       </c>
-      <c r="BJ21" s="44" t="s">
+      <c r="BI21" s="55" t="s">
         <v>291</v>
+      </c>
+      <c r="BJ21" s="55" t="s">
+        <v>292</v>
       </c>
       <c r="BK21" s="31" t="s">
         <v>186</v>
@@ -6044,53 +6044,53 @@
       <c r="BN21" s="31" t="s">
         <v>155</v>
       </c>
-      <c r="BO21" s="32" t="s">
-        <v>292</v>
-      </c>
-      <c r="BP21" s="32" t="s">
+      <c r="BO21" s="45" t="s">
+        <v>293</v>
+      </c>
+      <c r="BP21" s="45" t="s">
         <v>170</v>
       </c>
-      <c r="BQ21" s="32" t="s">
+      <c r="BQ21" s="45" t="s">
         <v>169</v>
       </c>
-      <c r="BR21" s="32" t="s">
-        <v>293</v>
-      </c>
-      <c r="BS21" s="32" t="s">
+      <c r="BR21" s="45" t="s">
+        <v>294</v>
+      </c>
+      <c r="BS21" s="45" t="s">
         <v>180</v>
       </c>
-      <c r="BT21" s="32" t="s">
+      <c r="BT21" s="45" t="s">
         <v>174</v>
       </c>
-      <c r="BU21" s="32" t="s">
+      <c r="BU21" s="45" t="s">
         <v>168</v>
       </c>
-      <c r="BV21" s="32" t="s">
+      <c r="BV21" s="45" t="s">
         <v>181</v>
       </c>
-      <c r="BW21" s="32" t="s">
+      <c r="BW21" s="45" t="s">
         <v>182</v>
       </c>
-      <c r="BX21" s="32" t="s">
+      <c r="BX21" s="45" t="s">
         <v>175</v>
       </c>
-      <c r="BY21" s="32" t="s">
+      <c r="BY21" s="45" t="s">
         <v>178</v>
       </c>
-      <c r="BZ21" s="32" t="s">
+      <c r="BZ21" s="45" t="s">
         <v>178</v>
       </c>
-      <c r="CA21" s="32" t="s">
+      <c r="CA21" s="45" t="s">
         <v>179</v>
       </c>
-      <c r="CB21" s="32" t="s">
-        <v>295</v>
-      </c>
-      <c r="CC21" s="32" t="s">
-        <v>295</v>
-      </c>
-      <c r="CD21" s="32" t="s">
-        <v>317</v>
+      <c r="CB21" s="45" t="s">
+        <v>296</v>
+      </c>
+      <c r="CC21" s="45" t="s">
+        <v>296</v>
+      </c>
+      <c r="CD21" s="45" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="22" spans="1:82">
@@ -6098,436 +6098,436 @@
       <c r="B22" s="31"/>
       <c r="C22" s="31"/>
       <c r="D22" s="31"/>
-      <c r="E22" s="61"/>
-      <c r="F22" s="66"/>
-      <c r="G22" s="66"/>
-      <c r="H22" s="66"/>
-      <c r="I22" s="66"/>
-      <c r="J22" s="36"/>
-      <c r="K22" s="36"/>
-      <c r="L22" s="36"/>
+      <c r="E22" s="56"/>
+      <c r="F22" s="74"/>
+      <c r="G22" s="74"/>
+      <c r="H22" s="74"/>
+      <c r="I22" s="74"/>
+      <c r="J22" s="43"/>
+      <c r="K22" s="43"/>
+      <c r="L22" s="43"/>
       <c r="M22" s="31"/>
       <c r="N22" s="31"/>
       <c r="O22" s="31"/>
       <c r="P22" s="31"/>
       <c r="Q22" s="31"/>
       <c r="R22" s="31"/>
-      <c r="S22" s="33"/>
+      <c r="S22" s="46"/>
       <c r="T22" s="31"/>
       <c r="U22" s="31"/>
       <c r="V22" s="31"/>
-      <c r="W22" s="36"/>
-      <c r="X22" s="36"/>
-      <c r="Y22" s="36"/>
-      <c r="Z22" s="36"/>
-      <c r="AA22" s="36"/>
-      <c r="AB22" s="33"/>
-      <c r="AC22" s="33"/>
-      <c r="AD22" s="33"/>
-      <c r="AE22" s="33"/>
-      <c r="AF22" s="33"/>
-      <c r="AG22" s="36"/>
-      <c r="AH22" s="33"/>
-      <c r="AI22" s="33"/>
+      <c r="W22" s="43"/>
+      <c r="X22" s="43"/>
+      <c r="Y22" s="43"/>
+      <c r="Z22" s="43"/>
+      <c r="AA22" s="43"/>
+      <c r="AB22" s="46"/>
+      <c r="AC22" s="46"/>
+      <c r="AD22" s="46"/>
+      <c r="AE22" s="46"/>
+      <c r="AF22" s="46"/>
+      <c r="AG22" s="43"/>
+      <c r="AH22" s="46"/>
+      <c r="AI22" s="46"/>
       <c r="AJ22" s="53"/>
-      <c r="AK22" s="44"/>
-      <c r="AL22" s="56"/>
-      <c r="AM22" s="33"/>
+      <c r="AK22" s="55"/>
+      <c r="AL22" s="59"/>
+      <c r="AM22" s="46"/>
       <c r="AN22" s="53"/>
-      <c r="AO22" s="44"/>
-      <c r="AP22" s="56"/>
-      <c r="AQ22" s="33"/>
+      <c r="AO22" s="55"/>
+      <c r="AP22" s="59"/>
+      <c r="AQ22" s="46"/>
       <c r="AR22" s="53"/>
-      <c r="AS22" s="44"/>
-      <c r="AT22" s="33"/>
-      <c r="AU22" s="33"/>
+      <c r="AS22" s="55"/>
+      <c r="AT22" s="46"/>
+      <c r="AU22" s="46"/>
       <c r="AV22" s="53"/>
-      <c r="AW22" s="44"/>
+      <c r="AW22" s="55"/>
       <c r="AX22" s="53"/>
-      <c r="AY22" s="44"/>
-      <c r="AZ22" s="51"/>
-      <c r="BA22" s="44"/>
-      <c r="BB22" s="44"/>
-      <c r="BC22" s="44"/>
-      <c r="BD22" s="44"/>
-      <c r="BE22" s="59"/>
-      <c r="BF22" s="33"/>
-      <c r="BG22" s="33"/>
-      <c r="BH22" s="44"/>
-      <c r="BI22" s="44"/>
-      <c r="BJ22" s="44"/>
+      <c r="AY22" s="55"/>
+      <c r="AZ22" s="57"/>
+      <c r="BA22" s="55"/>
+      <c r="BB22" s="55"/>
+      <c r="BC22" s="55"/>
+      <c r="BD22" s="55"/>
+      <c r="BE22" s="71"/>
+      <c r="BF22" s="46"/>
+      <c r="BG22" s="46"/>
+      <c r="BH22" s="55"/>
+      <c r="BI22" s="55"/>
+      <c r="BJ22" s="55"/>
       <c r="BK22" s="31"/>
       <c r="BL22" s="31"/>
       <c r="BM22" s="31"/>
       <c r="BN22" s="31"/>
-      <c r="BO22" s="33"/>
-      <c r="BP22" s="33"/>
-      <c r="BQ22" s="33"/>
-      <c r="BR22" s="33"/>
-      <c r="BS22" s="33"/>
-      <c r="BT22" s="33"/>
-      <c r="BU22" s="33"/>
-      <c r="BV22" s="33"/>
-      <c r="BW22" s="33"/>
-      <c r="BX22" s="33"/>
-      <c r="BY22" s="33"/>
-      <c r="BZ22" s="33"/>
-      <c r="CA22" s="33"/>
-      <c r="CB22" s="33"/>
-      <c r="CC22" s="33"/>
-      <c r="CD22" s="33"/>
+      <c r="BO22" s="46"/>
+      <c r="BP22" s="46"/>
+      <c r="BQ22" s="46"/>
+      <c r="BR22" s="46"/>
+      <c r="BS22" s="46"/>
+      <c r="BT22" s="46"/>
+      <c r="BU22" s="46"/>
+      <c r="BV22" s="46"/>
+      <c r="BW22" s="46"/>
+      <c r="BX22" s="46"/>
+      <c r="BY22" s="46"/>
+      <c r="BZ22" s="46"/>
+      <c r="CA22" s="46"/>
+      <c r="CB22" s="46"/>
+      <c r="CC22" s="46"/>
+      <c r="CD22" s="46"/>
     </row>
     <row r="23" spans="1:82">
       <c r="A23" s="31"/>
       <c r="B23" s="31"/>
       <c r="C23" s="31"/>
       <c r="D23" s="31"/>
-      <c r="E23" s="61"/>
-      <c r="F23" s="66"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="66"/>
-      <c r="I23" s="66"/>
-      <c r="J23" s="36"/>
-      <c r="K23" s="36"/>
-      <c r="L23" s="36"/>
+      <c r="E23" s="56"/>
+      <c r="F23" s="74"/>
+      <c r="G23" s="74"/>
+      <c r="H23" s="74"/>
+      <c r="I23" s="74"/>
+      <c r="J23" s="43"/>
+      <c r="K23" s="43"/>
+      <c r="L23" s="43"/>
       <c r="M23" s="31"/>
       <c r="N23" s="31"/>
       <c r="O23" s="31"/>
       <c r="P23" s="31"/>
       <c r="Q23" s="31"/>
       <c r="R23" s="31"/>
-      <c r="S23" s="33"/>
+      <c r="S23" s="46"/>
       <c r="T23" s="31"/>
       <c r="U23" s="31"/>
       <c r="V23" s="31"/>
-      <c r="W23" s="36"/>
-      <c r="X23" s="36"/>
-      <c r="Y23" s="36"/>
-      <c r="Z23" s="36"/>
-      <c r="AA23" s="36"/>
-      <c r="AB23" s="33"/>
-      <c r="AC23" s="33"/>
-      <c r="AD23" s="33"/>
-      <c r="AE23" s="33"/>
-      <c r="AF23" s="33"/>
-      <c r="AG23" s="36"/>
-      <c r="AH23" s="33"/>
-      <c r="AI23" s="33"/>
+      <c r="W23" s="43"/>
+      <c r="X23" s="43"/>
+      <c r="Y23" s="43"/>
+      <c r="Z23" s="43"/>
+      <c r="AA23" s="43"/>
+      <c r="AB23" s="46"/>
+      <c r="AC23" s="46"/>
+      <c r="AD23" s="46"/>
+      <c r="AE23" s="46"/>
+      <c r="AF23" s="46"/>
+      <c r="AG23" s="43"/>
+      <c r="AH23" s="46"/>
+      <c r="AI23" s="46"/>
       <c r="AJ23" s="53"/>
-      <c r="AK23" s="44"/>
-      <c r="AL23" s="56"/>
-      <c r="AM23" s="33"/>
+      <c r="AK23" s="55"/>
+      <c r="AL23" s="59"/>
+      <c r="AM23" s="46"/>
       <c r="AN23" s="53"/>
-      <c r="AO23" s="44"/>
-      <c r="AP23" s="56"/>
-      <c r="AQ23" s="33"/>
+      <c r="AO23" s="55"/>
+      <c r="AP23" s="59"/>
+      <c r="AQ23" s="46"/>
       <c r="AR23" s="53"/>
-      <c r="AS23" s="44"/>
-      <c r="AT23" s="33"/>
-      <c r="AU23" s="33"/>
+      <c r="AS23" s="55"/>
+      <c r="AT23" s="46"/>
+      <c r="AU23" s="46"/>
       <c r="AV23" s="53"/>
-      <c r="AW23" s="44"/>
+      <c r="AW23" s="55"/>
       <c r="AX23" s="53"/>
-      <c r="AY23" s="44"/>
-      <c r="AZ23" s="51"/>
-      <c r="BA23" s="44"/>
-      <c r="BB23" s="44"/>
-      <c r="BC23" s="44"/>
-      <c r="BD23" s="44"/>
-      <c r="BE23" s="59"/>
-      <c r="BF23" s="33"/>
-      <c r="BG23" s="33"/>
-      <c r="BH23" s="44"/>
-      <c r="BI23" s="44"/>
-      <c r="BJ23" s="44"/>
+      <c r="AY23" s="55"/>
+      <c r="AZ23" s="57"/>
+      <c r="BA23" s="55"/>
+      <c r="BB23" s="55"/>
+      <c r="BC23" s="55"/>
+      <c r="BD23" s="55"/>
+      <c r="BE23" s="71"/>
+      <c r="BF23" s="46"/>
+      <c r="BG23" s="46"/>
+      <c r="BH23" s="55"/>
+      <c r="BI23" s="55"/>
+      <c r="BJ23" s="55"/>
       <c r="BK23" s="31"/>
       <c r="BL23" s="31"/>
       <c r="BM23" s="31"/>
       <c r="BN23" s="31"/>
-      <c r="BO23" s="33"/>
-      <c r="BP23" s="33"/>
-      <c r="BQ23" s="33"/>
-      <c r="BR23" s="33"/>
-      <c r="BS23" s="33"/>
-      <c r="BT23" s="33"/>
-      <c r="BU23" s="33"/>
-      <c r="BV23" s="33"/>
-      <c r="BW23" s="33"/>
-      <c r="BX23" s="33"/>
-      <c r="BY23" s="33"/>
-      <c r="BZ23" s="33"/>
-      <c r="CA23" s="33"/>
-      <c r="CB23" s="33"/>
-      <c r="CC23" s="33"/>
-      <c r="CD23" s="33"/>
+      <c r="BO23" s="46"/>
+      <c r="BP23" s="46"/>
+      <c r="BQ23" s="46"/>
+      <c r="BR23" s="46"/>
+      <c r="BS23" s="46"/>
+      <c r="BT23" s="46"/>
+      <c r="BU23" s="46"/>
+      <c r="BV23" s="46"/>
+      <c r="BW23" s="46"/>
+      <c r="BX23" s="46"/>
+      <c r="BY23" s="46"/>
+      <c r="BZ23" s="46"/>
+      <c r="CA23" s="46"/>
+      <c r="CB23" s="46"/>
+      <c r="CC23" s="46"/>
+      <c r="CD23" s="46"/>
     </row>
     <row r="24" spans="1:82">
       <c r="A24" s="31"/>
       <c r="B24" s="31"/>
       <c r="C24" s="31"/>
       <c r="D24" s="31"/>
-      <c r="E24" s="61"/>
-      <c r="F24" s="66"/>
-      <c r="G24" s="66"/>
-      <c r="H24" s="66"/>
-      <c r="I24" s="66"/>
-      <c r="J24" s="36"/>
-      <c r="K24" s="36"/>
-      <c r="L24" s="36"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="74"/>
+      <c r="G24" s="74"/>
+      <c r="H24" s="74"/>
+      <c r="I24" s="74"/>
+      <c r="J24" s="43"/>
+      <c r="K24" s="43"/>
+      <c r="L24" s="43"/>
       <c r="M24" s="31"/>
       <c r="N24" s="31"/>
       <c r="O24" s="31"/>
       <c r="P24" s="31"/>
       <c r="Q24" s="31"/>
       <c r="R24" s="31"/>
-      <c r="S24" s="33"/>
+      <c r="S24" s="46"/>
       <c r="T24" s="31"/>
       <c r="U24" s="31"/>
       <c r="V24" s="31"/>
-      <c r="W24" s="36"/>
-      <c r="X24" s="36"/>
-      <c r="Y24" s="36"/>
-      <c r="Z24" s="36"/>
-      <c r="AA24" s="36"/>
-      <c r="AB24" s="33"/>
-      <c r="AC24" s="33"/>
-      <c r="AD24" s="33"/>
-      <c r="AE24" s="33"/>
-      <c r="AF24" s="33"/>
-      <c r="AG24" s="36"/>
-      <c r="AH24" s="33"/>
-      <c r="AI24" s="33"/>
+      <c r="W24" s="43"/>
+      <c r="X24" s="43"/>
+      <c r="Y24" s="43"/>
+      <c r="Z24" s="43"/>
+      <c r="AA24" s="43"/>
+      <c r="AB24" s="46"/>
+      <c r="AC24" s="46"/>
+      <c r="AD24" s="46"/>
+      <c r="AE24" s="46"/>
+      <c r="AF24" s="46"/>
+      <c r="AG24" s="43"/>
+      <c r="AH24" s="46"/>
+      <c r="AI24" s="46"/>
       <c r="AJ24" s="53"/>
-      <c r="AK24" s="44"/>
-      <c r="AL24" s="56"/>
-      <c r="AM24" s="33"/>
+      <c r="AK24" s="55"/>
+      <c r="AL24" s="59"/>
+      <c r="AM24" s="46"/>
       <c r="AN24" s="53"/>
-      <c r="AO24" s="44"/>
-      <c r="AP24" s="56"/>
-      <c r="AQ24" s="33"/>
+      <c r="AO24" s="55"/>
+      <c r="AP24" s="59"/>
+      <c r="AQ24" s="46"/>
       <c r="AR24" s="53"/>
-      <c r="AS24" s="44"/>
-      <c r="AT24" s="33"/>
-      <c r="AU24" s="33"/>
+      <c r="AS24" s="55"/>
+      <c r="AT24" s="46"/>
+      <c r="AU24" s="46"/>
       <c r="AV24" s="53"/>
-      <c r="AW24" s="44"/>
+      <c r="AW24" s="55"/>
       <c r="AX24" s="53"/>
-      <c r="AY24" s="44"/>
-      <c r="AZ24" s="51"/>
-      <c r="BA24" s="44"/>
-      <c r="BB24" s="44"/>
-      <c r="BC24" s="44"/>
-      <c r="BD24" s="44"/>
-      <c r="BE24" s="59"/>
-      <c r="BF24" s="33"/>
-      <c r="BG24" s="33"/>
-      <c r="BH24" s="44"/>
-      <c r="BI24" s="44"/>
-      <c r="BJ24" s="44"/>
+      <c r="AY24" s="55"/>
+      <c r="AZ24" s="57"/>
+      <c r="BA24" s="55"/>
+      <c r="BB24" s="55"/>
+      <c r="BC24" s="55"/>
+      <c r="BD24" s="55"/>
+      <c r="BE24" s="71"/>
+      <c r="BF24" s="46"/>
+      <c r="BG24" s="46"/>
+      <c r="BH24" s="55"/>
+      <c r="BI24" s="55"/>
+      <c r="BJ24" s="55"/>
       <c r="BK24" s="31"/>
       <c r="BL24" s="31"/>
       <c r="BM24" s="31"/>
       <c r="BN24" s="31"/>
-      <c r="BO24" s="33"/>
-      <c r="BP24" s="33"/>
-      <c r="BQ24" s="33"/>
-      <c r="BR24" s="33"/>
-      <c r="BS24" s="33"/>
-      <c r="BT24" s="33"/>
-      <c r="BU24" s="33"/>
-      <c r="BV24" s="33"/>
-      <c r="BW24" s="33"/>
-      <c r="BX24" s="33"/>
-      <c r="BY24" s="33"/>
-      <c r="BZ24" s="33"/>
-      <c r="CA24" s="33"/>
-      <c r="CB24" s="33"/>
-      <c r="CC24" s="33"/>
-      <c r="CD24" s="33"/>
+      <c r="BO24" s="46"/>
+      <c r="BP24" s="46"/>
+      <c r="BQ24" s="46"/>
+      <c r="BR24" s="46"/>
+      <c r="BS24" s="46"/>
+      <c r="BT24" s="46"/>
+      <c r="BU24" s="46"/>
+      <c r="BV24" s="46"/>
+      <c r="BW24" s="46"/>
+      <c r="BX24" s="46"/>
+      <c r="BY24" s="46"/>
+      <c r="BZ24" s="46"/>
+      <c r="CA24" s="46"/>
+      <c r="CB24" s="46"/>
+      <c r="CC24" s="46"/>
+      <c r="CD24" s="46"/>
     </row>
     <row r="25" spans="1:82">
       <c r="A25" s="31"/>
       <c r="B25" s="31"/>
       <c r="C25" s="31"/>
       <c r="D25" s="31"/>
-      <c r="E25" s="61"/>
-      <c r="F25" s="66"/>
-      <c r="G25" s="66"/>
-      <c r="H25" s="66"/>
-      <c r="I25" s="66"/>
-      <c r="J25" s="36"/>
-      <c r="K25" s="36"/>
-      <c r="L25" s="36"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="74"/>
+      <c r="G25" s="74"/>
+      <c r="H25" s="74"/>
+      <c r="I25" s="74"/>
+      <c r="J25" s="43"/>
+      <c r="K25" s="43"/>
+      <c r="L25" s="43"/>
       <c r="M25" s="31"/>
       <c r="N25" s="31"/>
       <c r="O25" s="31"/>
       <c r="P25" s="31"/>
       <c r="Q25" s="31"/>
       <c r="R25" s="31"/>
-      <c r="S25" s="33"/>
+      <c r="S25" s="46"/>
       <c r="T25" s="31"/>
       <c r="U25" s="31"/>
       <c r="V25" s="31"/>
-      <c r="W25" s="36"/>
-      <c r="X25" s="36"/>
-      <c r="Y25" s="36"/>
-      <c r="Z25" s="36"/>
-      <c r="AA25" s="36"/>
-      <c r="AB25" s="33"/>
-      <c r="AC25" s="33"/>
-      <c r="AD25" s="33"/>
-      <c r="AE25" s="33"/>
-      <c r="AF25" s="33"/>
-      <c r="AG25" s="36"/>
-      <c r="AH25" s="33"/>
-      <c r="AI25" s="33"/>
+      <c r="W25" s="43"/>
+      <c r="X25" s="43"/>
+      <c r="Y25" s="43"/>
+      <c r="Z25" s="43"/>
+      <c r="AA25" s="43"/>
+      <c r="AB25" s="46"/>
+      <c r="AC25" s="46"/>
+      <c r="AD25" s="46"/>
+      <c r="AE25" s="46"/>
+      <c r="AF25" s="46"/>
+      <c r="AG25" s="43"/>
+      <c r="AH25" s="46"/>
+      <c r="AI25" s="46"/>
       <c r="AJ25" s="53"/>
-      <c r="AK25" s="44"/>
-      <c r="AL25" s="56"/>
-      <c r="AM25" s="33"/>
+      <c r="AK25" s="55"/>
+      <c r="AL25" s="59"/>
+      <c r="AM25" s="46"/>
       <c r="AN25" s="53"/>
-      <c r="AO25" s="44"/>
-      <c r="AP25" s="56"/>
-      <c r="AQ25" s="33"/>
+      <c r="AO25" s="55"/>
+      <c r="AP25" s="59"/>
+      <c r="AQ25" s="46"/>
       <c r="AR25" s="53"/>
-      <c r="AS25" s="44"/>
-      <c r="AT25" s="33"/>
-      <c r="AU25" s="33"/>
+      <c r="AS25" s="55"/>
+      <c r="AT25" s="46"/>
+      <c r="AU25" s="46"/>
       <c r="AV25" s="53"/>
-      <c r="AW25" s="44"/>
+      <c r="AW25" s="55"/>
       <c r="AX25" s="53"/>
-      <c r="AY25" s="44"/>
-      <c r="AZ25" s="51"/>
-      <c r="BA25" s="44"/>
-      <c r="BB25" s="44"/>
-      <c r="BC25" s="44"/>
-      <c r="BD25" s="44"/>
-      <c r="BE25" s="59"/>
-      <c r="BF25" s="33"/>
-      <c r="BG25" s="33"/>
-      <c r="BH25" s="44"/>
-      <c r="BI25" s="44"/>
-      <c r="BJ25" s="44"/>
+      <c r="AY25" s="55"/>
+      <c r="AZ25" s="57"/>
+      <c r="BA25" s="55"/>
+      <c r="BB25" s="55"/>
+      <c r="BC25" s="55"/>
+      <c r="BD25" s="55"/>
+      <c r="BE25" s="71"/>
+      <c r="BF25" s="46"/>
+      <c r="BG25" s="46"/>
+      <c r="BH25" s="55"/>
+      <c r="BI25" s="55"/>
+      <c r="BJ25" s="55"/>
       <c r="BK25" s="31"/>
       <c r="BL25" s="31"/>
       <c r="BM25" s="31"/>
       <c r="BN25" s="31"/>
-      <c r="BO25" s="33"/>
-      <c r="BP25" s="33"/>
-      <c r="BQ25" s="33"/>
-      <c r="BR25" s="33"/>
-      <c r="BS25" s="33"/>
-      <c r="BT25" s="33"/>
-      <c r="BU25" s="33"/>
-      <c r="BV25" s="33"/>
-      <c r="BW25" s="33"/>
-      <c r="BX25" s="33"/>
-      <c r="BY25" s="33"/>
-      <c r="BZ25" s="33"/>
-      <c r="CA25" s="33"/>
-      <c r="CB25" s="33"/>
-      <c r="CC25" s="33"/>
-      <c r="CD25" s="33"/>
+      <c r="BO25" s="46"/>
+      <c r="BP25" s="46"/>
+      <c r="BQ25" s="46"/>
+      <c r="BR25" s="46"/>
+      <c r="BS25" s="46"/>
+      <c r="BT25" s="46"/>
+      <c r="BU25" s="46"/>
+      <c r="BV25" s="46"/>
+      <c r="BW25" s="46"/>
+      <c r="BX25" s="46"/>
+      <c r="BY25" s="46"/>
+      <c r="BZ25" s="46"/>
+      <c r="CA25" s="46"/>
+      <c r="CB25" s="46"/>
+      <c r="CC25" s="46"/>
+      <c r="CD25" s="46"/>
     </row>
     <row r="26" spans="1:82">
       <c r="A26" s="31"/>
       <c r="B26" s="31"/>
       <c r="C26" s="31"/>
       <c r="D26" s="31"/>
-      <c r="E26" s="61"/>
-      <c r="F26" s="66"/>
-      <c r="G26" s="66"/>
-      <c r="H26" s="66"/>
-      <c r="I26" s="66"/>
-      <c r="J26" s="37"/>
-      <c r="K26" s="37"/>
-      <c r="L26" s="37"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="74"/>
+      <c r="G26" s="74"/>
+      <c r="H26" s="74"/>
+      <c r="I26" s="74"/>
+      <c r="J26" s="44"/>
+      <c r="K26" s="44"/>
+      <c r="L26" s="44"/>
       <c r="M26" s="31"/>
       <c r="N26" s="31"/>
       <c r="O26" s="31"/>
       <c r="P26" s="31"/>
       <c r="Q26" s="31"/>
       <c r="R26" s="31"/>
-      <c r="S26" s="34"/>
+      <c r="S26" s="47"/>
       <c r="T26" s="31"/>
       <c r="U26" s="31"/>
       <c r="V26" s="31"/>
-      <c r="W26" s="37"/>
-      <c r="X26" s="37"/>
-      <c r="Y26" s="37"/>
-      <c r="Z26" s="37"/>
-      <c r="AA26" s="37"/>
-      <c r="AB26" s="34"/>
-      <c r="AC26" s="34"/>
-      <c r="AD26" s="34"/>
-      <c r="AE26" s="34"/>
-      <c r="AF26" s="34"/>
-      <c r="AG26" s="37"/>
-      <c r="AH26" s="34"/>
-      <c r="AI26" s="34"/>
+      <c r="W26" s="44"/>
+      <c r="X26" s="44"/>
+      <c r="Y26" s="44"/>
+      <c r="Z26" s="44"/>
+      <c r="AA26" s="44"/>
+      <c r="AB26" s="47"/>
+      <c r="AC26" s="47"/>
+      <c r="AD26" s="47"/>
+      <c r="AE26" s="47"/>
+      <c r="AF26" s="47"/>
+      <c r="AG26" s="44"/>
+      <c r="AH26" s="47"/>
+      <c r="AI26" s="47"/>
       <c r="AJ26" s="54"/>
-      <c r="AK26" s="44"/>
-      <c r="AL26" s="57"/>
-      <c r="AM26" s="34"/>
+      <c r="AK26" s="55"/>
+      <c r="AL26" s="60"/>
+      <c r="AM26" s="47"/>
       <c r="AN26" s="54"/>
-      <c r="AO26" s="44"/>
-      <c r="AP26" s="57"/>
-      <c r="AQ26" s="34"/>
+      <c r="AO26" s="55"/>
+      <c r="AP26" s="60"/>
+      <c r="AQ26" s="47"/>
       <c r="AR26" s="54"/>
-      <c r="AS26" s="44"/>
-      <c r="AT26" s="34"/>
-      <c r="AU26" s="34"/>
+      <c r="AS26" s="55"/>
+      <c r="AT26" s="47"/>
+      <c r="AU26" s="47"/>
       <c r="AV26" s="54"/>
-      <c r="AW26" s="44"/>
+      <c r="AW26" s="55"/>
       <c r="AX26" s="54"/>
-      <c r="AY26" s="44"/>
-      <c r="AZ26" s="51"/>
-      <c r="BA26" s="44"/>
-      <c r="BB26" s="44"/>
-      <c r="BC26" s="44"/>
-      <c r="BD26" s="44"/>
-      <c r="BE26" s="60"/>
-      <c r="BF26" s="34"/>
-      <c r="BG26" s="34"/>
-      <c r="BH26" s="44"/>
-      <c r="BI26" s="44"/>
-      <c r="BJ26" s="44"/>
+      <c r="AY26" s="55"/>
+      <c r="AZ26" s="57"/>
+      <c r="BA26" s="55"/>
+      <c r="BB26" s="55"/>
+      <c r="BC26" s="55"/>
+      <c r="BD26" s="55"/>
+      <c r="BE26" s="72"/>
+      <c r="BF26" s="47"/>
+      <c r="BG26" s="47"/>
+      <c r="BH26" s="55"/>
+      <c r="BI26" s="55"/>
+      <c r="BJ26" s="55"/>
       <c r="BK26" s="31"/>
       <c r="BL26" s="31"/>
       <c r="BM26" s="31"/>
       <c r="BN26" s="31"/>
-      <c r="BO26" s="34"/>
-      <c r="BP26" s="34"/>
-      <c r="BQ26" s="34"/>
-      <c r="BR26" s="34"/>
-      <c r="BS26" s="34"/>
-      <c r="BT26" s="34"/>
-      <c r="BU26" s="34"/>
-      <c r="BV26" s="34"/>
-      <c r="BW26" s="34"/>
-      <c r="BX26" s="34"/>
-      <c r="BY26" s="34"/>
-      <c r="BZ26" s="34"/>
-      <c r="CA26" s="34"/>
-      <c r="CB26" s="34"/>
-      <c r="CC26" s="34"/>
-      <c r="CD26" s="34"/>
+      <c r="BO26" s="47"/>
+      <c r="BP26" s="47"/>
+      <c r="BQ26" s="47"/>
+      <c r="BR26" s="47"/>
+      <c r="BS26" s="47"/>
+      <c r="BT26" s="47"/>
+      <c r="BU26" s="47"/>
+      <c r="BV26" s="47"/>
+      <c r="BW26" s="47"/>
+      <c r="BX26" s="47"/>
+      <c r="BY26" s="47"/>
+      <c r="BZ26" s="47"/>
+      <c r="CA26" s="47"/>
+      <c r="CB26" s="47"/>
+      <c r="CC26" s="47"/>
+      <c r="CD26" s="47"/>
     </row>
     <row r="27" spans="1:82" ht="11.25" customHeight="1">
-      <c r="F27" s="66"/>
-      <c r="G27" s="66"/>
-      <c r="H27" s="66"/>
-      <c r="I27" s="66"/>
-      <c r="AK27" s="44"/>
-      <c r="AO27" s="44"/>
-      <c r="AS27" s="44"/>
-      <c r="AW27" s="44"/>
-      <c r="AY27" s="44"/>
-      <c r="AZ27" s="51"/>
-      <c r="BA27" s="44"/>
-      <c r="BB27" s="44"/>
-      <c r="BC27" s="44"/>
-      <c r="BD27" s="44"/>
+      <c r="F27" s="74"/>
+      <c r="G27" s="74"/>
+      <c r="H27" s="74"/>
+      <c r="I27" s="74"/>
+      <c r="AK27" s="55"/>
+      <c r="AO27" s="55"/>
+      <c r="AS27" s="55"/>
+      <c r="AW27" s="55"/>
+      <c r="AY27" s="55"/>
+      <c r="AZ27" s="57"/>
+      <c r="BA27" s="55"/>
+      <c r="BB27" s="55"/>
+      <c r="BC27" s="55"/>
+      <c r="BD27" s="55"/>
     </row>
     <row r="28" spans="1:82" ht="11.25" customHeight="1">
       <c r="B28" s="7" t="s">
@@ -6536,255 +6536,255 @@
       <c r="C28" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F28" s="66"/>
-      <c r="G28" s="66"/>
-      <c r="H28" s="66"/>
-      <c r="I28" s="66"/>
+      <c r="F28" s="74"/>
+      <c r="G28" s="74"/>
+      <c r="H28" s="74"/>
+      <c r="I28" s="74"/>
       <c r="J28" s="31" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="V28" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="AE28" s="32" t="s">
-        <v>215</v>
-      </c>
-      <c r="AK28" s="44"/>
-      <c r="AO28" s="44"/>
-      <c r="AS28" s="44"/>
-      <c r="AW28" s="44"/>
-      <c r="AY28" s="44"/>
-      <c r="AZ28" s="51"/>
-      <c r="BA28" s="44"/>
-      <c r="BB28" s="44"/>
-      <c r="BC28" s="44"/>
-      <c r="BD28" s="44"/>
-      <c r="BJ28" s="32" t="s">
-        <v>246</v>
+      <c r="AE28" s="45" t="s">
+        <v>216</v>
+      </c>
+      <c r="AK28" s="55"/>
+      <c r="AO28" s="55"/>
+      <c r="AS28" s="55"/>
+      <c r="AW28" s="55"/>
+      <c r="AY28" s="55"/>
+      <c r="AZ28" s="57"/>
+      <c r="BA28" s="55"/>
+      <c r="BB28" s="55"/>
+      <c r="BC28" s="55"/>
+      <c r="BD28" s="55"/>
+      <c r="BJ28" s="45" t="s">
+        <v>247</v>
       </c>
       <c r="BK28" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="CB28" s="35" t="s">
-        <v>296</v>
-      </c>
-      <c r="CC28" s="35" t="s">
-        <v>296</v>
+      <c r="CB28" s="42" t="s">
+        <v>297</v>
+      </c>
+      <c r="CC28" s="42" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="29" spans="1:82" ht="11.25" customHeight="1">
-      <c r="B29" s="62" t="s">
+      <c r="B29" s="61" t="s">
         <v>187</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="F29" s="66"/>
-      <c r="G29" s="66"/>
-      <c r="H29" s="66"/>
-      <c r="I29" s="66"/>
+        <v>298</v>
+      </c>
+      <c r="F29" s="74"/>
+      <c r="G29" s="74"/>
+      <c r="H29" s="74"/>
+      <c r="I29" s="74"/>
       <c r="J29" s="31"/>
       <c r="V29" s="15" t="s">
-        <v>305</v>
-      </c>
-      <c r="AE29" s="33"/>
-      <c r="BJ29" s="33"/>
+        <v>306</v>
+      </c>
+      <c r="AE29" s="46"/>
+      <c r="BJ29" s="46"/>
       <c r="BK29" s="14" t="s">
-        <v>312</v>
-      </c>
-      <c r="BP29" s="45" t="s">
-        <v>464</v>
-      </c>
-      <c r="BQ29" s="46"/>
-      <c r="CB29" s="36"/>
-      <c r="CC29" s="36"/>
+        <v>313</v>
+      </c>
+      <c r="BP29" s="76" t="s">
+        <v>465</v>
+      </c>
+      <c r="BQ29" s="77"/>
+      <c r="CB29" s="43"/>
+      <c r="CC29" s="43"/>
     </row>
     <row r="30" spans="1:82" ht="11.25" customHeight="1">
-      <c r="B30" s="63"/>
+      <c r="B30" s="62"/>
       <c r="C30" s="5" t="s">
-        <v>298</v>
-      </c>
-      <c r="F30" s="66"/>
-      <c r="G30" s="66"/>
-      <c r="H30" s="66"/>
-      <c r="I30" s="66"/>
+        <v>299</v>
+      </c>
+      <c r="F30" s="74"/>
+      <c r="G30" s="74"/>
+      <c r="H30" s="74"/>
+      <c r="I30" s="74"/>
       <c r="J30" s="31"/>
       <c r="V30" s="17" t="s">
-        <v>306</v>
-      </c>
-      <c r="AE30" s="33"/>
-      <c r="BJ30" s="33"/>
+        <v>307</v>
+      </c>
+      <c r="AE30" s="46"/>
+      <c r="BJ30" s="46"/>
       <c r="BK30" s="6" t="s">
-        <v>313</v>
-      </c>
-      <c r="BP30" s="47"/>
-      <c r="BQ30" s="48"/>
-      <c r="CB30" s="36"/>
-      <c r="CC30" s="36"/>
+        <v>314</v>
+      </c>
+      <c r="BP30" s="78"/>
+      <c r="BQ30" s="79"/>
+      <c r="CB30" s="43"/>
+      <c r="CC30" s="43"/>
     </row>
     <row r="31" spans="1:82" ht="11.25" customHeight="1">
-      <c r="B31" s="63"/>
+      <c r="B31" s="62"/>
       <c r="C31" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="F31" s="66"/>
-      <c r="G31" s="66"/>
-      <c r="H31" s="66"/>
-      <c r="I31" s="66"/>
+        <v>300</v>
+      </c>
+      <c r="F31" s="74"/>
+      <c r="G31" s="74"/>
+      <c r="H31" s="74"/>
+      <c r="I31" s="74"/>
       <c r="J31" s="31"/>
       <c r="V31" s="17" t="s">
-        <v>307</v>
-      </c>
-      <c r="AE31" s="33"/>
-      <c r="BJ31" s="33"/>
-      <c r="BP31" s="47"/>
-      <c r="BQ31" s="48"/>
-      <c r="CB31" s="36"/>
-      <c r="CC31" s="36"/>
+        <v>308</v>
+      </c>
+      <c r="AE31" s="46"/>
+      <c r="BJ31" s="46"/>
+      <c r="BP31" s="78"/>
+      <c r="BQ31" s="79"/>
+      <c r="CB31" s="43"/>
+      <c r="CC31" s="43"/>
     </row>
     <row r="32" spans="1:82" ht="11.25" customHeight="1">
-      <c r="B32" s="63"/>
+      <c r="B32" s="62"/>
       <c r="C32" s="5" t="s">
-        <v>300</v>
-      </c>
-      <c r="F32" s="67"/>
-      <c r="G32" s="67"/>
-      <c r="H32" s="67"/>
-      <c r="I32" s="67"/>
+        <v>301</v>
+      </c>
+      <c r="F32" s="75"/>
+      <c r="G32" s="75"/>
+      <c r="H32" s="75"/>
+      <c r="I32" s="75"/>
       <c r="J32" s="31"/>
       <c r="V32" s="17" t="s">
-        <v>308</v>
-      </c>
-      <c r="AE32" s="33"/>
-      <c r="BJ32" s="33"/>
-      <c r="BP32" s="47"/>
-      <c r="BQ32" s="48"/>
-      <c r="CB32" s="36"/>
-      <c r="CC32" s="36"/>
+        <v>309</v>
+      </c>
+      <c r="AE32" s="46"/>
+      <c r="BJ32" s="46"/>
+      <c r="BP32" s="78"/>
+      <c r="BQ32" s="79"/>
+      <c r="CB32" s="43"/>
+      <c r="CC32" s="43"/>
     </row>
     <row r="33" spans="2:81" ht="11.25" customHeight="1">
-      <c r="B33" s="63"/>
+      <c r="B33" s="62"/>
       <c r="C33" s="5" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="J33" s="31"/>
       <c r="V33" s="17" t="s">
-        <v>309</v>
-      </c>
-      <c r="AE33" s="33"/>
-      <c r="BJ33" s="33"/>
-      <c r="BP33" s="47"/>
-      <c r="BQ33" s="48"/>
-      <c r="CB33" s="37"/>
-      <c r="CC33" s="37"/>
+        <v>310</v>
+      </c>
+      <c r="AE33" s="46"/>
+      <c r="BJ33" s="46"/>
+      <c r="BP33" s="78"/>
+      <c r="BQ33" s="79"/>
+      <c r="CB33" s="44"/>
+      <c r="CC33" s="44"/>
     </row>
     <row r="34" spans="2:81" ht="11.25" customHeight="1">
-      <c r="B34" s="63"/>
+      <c r="B34" s="62"/>
       <c r="C34" s="5" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="J34" s="31"/>
       <c r="V34" s="17" t="s">
-        <v>310</v>
-      </c>
-      <c r="AE34" s="33"/>
-      <c r="BJ34" s="34"/>
-      <c r="BP34" s="47"/>
-      <c r="BQ34" s="48"/>
+        <v>311</v>
+      </c>
+      <c r="AE34" s="46"/>
+      <c r="BJ34" s="47"/>
+      <c r="BP34" s="78"/>
+      <c r="BQ34" s="79"/>
       <c r="CC34" s="8"/>
     </row>
     <row r="35" spans="2:81" ht="11.25" customHeight="1">
-      <c r="B35" s="64"/>
+      <c r="B35" s="63"/>
       <c r="C35" s="5" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="J35" s="31"/>
       <c r="V35" s="16" t="s">
-        <v>311</v>
-      </c>
-      <c r="AE35" s="33"/>
-      <c r="BP35" s="49"/>
-      <c r="BQ35" s="50"/>
-      <c r="CB35" s="32" t="s">
-        <v>314</v>
-      </c>
-      <c r="CC35" s="32" t="s">
-        <v>314</v>
+        <v>312</v>
+      </c>
+      <c r="AE35" s="46"/>
+      <c r="BP35" s="80"/>
+      <c r="BQ35" s="81"/>
+      <c r="CB35" s="45" t="s">
+        <v>315</v>
+      </c>
+      <c r="CC35" s="45" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="36" spans="2:81">
       <c r="C36" s="5" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="J36" s="31"/>
-      <c r="AE36" s="33"/>
-      <c r="CB36" s="33"/>
-      <c r="CC36" s="33"/>
+      <c r="AE36" s="46"/>
+      <c r="CB36" s="46"/>
+      <c r="CC36" s="46"/>
     </row>
     <row r="37" spans="2:81">
       <c r="C37" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="AE37" s="34"/>
-      <c r="CB37" s="33"/>
-      <c r="CC37" s="33"/>
+      <c r="AE37" s="47"/>
+      <c r="CB37" s="46"/>
+      <c r="CC37" s="46"/>
     </row>
     <row r="38" spans="2:81">
       <c r="C38" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="CB38" s="33"/>
-      <c r="CC38" s="33"/>
+      <c r="CB38" s="46"/>
+      <c r="CC38" s="46"/>
     </row>
     <row r="39" spans="2:81">
       <c r="C39" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="AE39" s="35" t="s">
-        <v>216</v>
-      </c>
-      <c r="CB39" s="33"/>
-      <c r="CC39" s="33"/>
+      <c r="AE39" s="42" t="s">
+        <v>217</v>
+      </c>
+      <c r="CB39" s="46"/>
+      <c r="CC39" s="46"/>
     </row>
     <row r="40" spans="2:81">
       <c r="C40" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="AE40" s="36"/>
-      <c r="CB40" s="33"/>
-      <c r="CC40" s="33"/>
+      <c r="AE40" s="43"/>
+      <c r="CB40" s="46"/>
+      <c r="CC40" s="46"/>
     </row>
     <row r="41" spans="2:81">
       <c r="C41" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="AE41" s="36"/>
-      <c r="CB41" s="33"/>
-      <c r="CC41" s="33"/>
+      <c r="AE41" s="43"/>
+      <c r="CB41" s="46"/>
+      <c r="CC41" s="46"/>
     </row>
     <row r="42" spans="2:81">
       <c r="C42" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="AE42" s="36"/>
-      <c r="CB42" s="33"/>
-      <c r="CC42" s="33"/>
+      <c r="AE42" s="43"/>
+      <c r="CB42" s="46"/>
+      <c r="CC42" s="46"/>
     </row>
     <row r="43" spans="2:81">
       <c r="C43" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="AE43" s="36"/>
-      <c r="CB43" s="33"/>
-      <c r="CC43" s="33"/>
+      <c r="AE43" s="43"/>
+      <c r="CB43" s="46"/>
+      <c r="CC43" s="46"/>
     </row>
     <row r="44" spans="2:81">
       <c r="C44" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="AE44" s="37"/>
-      <c r="CB44" s="33"/>
-      <c r="CC44" s="33"/>
+      <c r="AE44" s="44"/>
+      <c r="CB44" s="46"/>
+      <c r="CC44" s="46"/>
     </row>
     <row r="45" spans="2:81">
       <c r="C45" s="5" t="s">
@@ -6793,24 +6793,24 @@
       <c r="BJ45" s="31" t="s">
         <v>185</v>
       </c>
-      <c r="CB45" s="33"/>
-      <c r="CC45" s="33"/>
+      <c r="CB45" s="46"/>
+      <c r="CC45" s="46"/>
     </row>
     <row r="46" spans="2:81">
       <c r="C46" s="5" t="s">
         <v>107</v>
       </c>
       <c r="BJ46" s="31"/>
-      <c r="CB46" s="33"/>
-      <c r="CC46" s="33"/>
+      <c r="CB46" s="46"/>
+      <c r="CC46" s="46"/>
     </row>
     <row r="47" spans="2:81">
       <c r="C47" s="5" t="s">
         <v>108</v>
       </c>
       <c r="BJ47" s="31"/>
-      <c r="CB47" s="34"/>
-      <c r="CC47" s="34"/>
+      <c r="CB47" s="47"/>
+      <c r="CC47" s="47"/>
     </row>
     <row r="48" spans="2:81">
       <c r="C48" s="5" t="s">
@@ -6822,33 +6822,33 @@
       <c r="C49" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="CB49" s="35" t="s">
-        <v>315</v>
-      </c>
-      <c r="CC49" s="35" t="s">
+      <c r="CB49" s="42" t="s">
         <v>316</v>
+      </c>
+      <c r="CC49" s="42" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="50" spans="3:81">
       <c r="C50" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="CB50" s="36"/>
-      <c r="CC50" s="36"/>
+      <c r="CB50" s="43"/>
+      <c r="CC50" s="43"/>
     </row>
     <row r="51" spans="3:81">
       <c r="C51" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="CB51" s="36"/>
-      <c r="CC51" s="36"/>
+      <c r="CB51" s="43"/>
+      <c r="CC51" s="43"/>
     </row>
     <row r="52" spans="3:81">
       <c r="C52" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="CB52" s="37"/>
-      <c r="CC52" s="37"/>
+      <c r="CB52" s="44"/>
+      <c r="CC52" s="44"/>
     </row>
     <row r="53" spans="3:81">
       <c r="C53" s="5" t="s">
@@ -6992,37 +6992,52 @@
     </row>
   </sheetData>
   <mergeCells count="108">
-    <mergeCell ref="BE18:BE20"/>
-    <mergeCell ref="AY18:BD20"/>
-    <mergeCell ref="BF18:BF20"/>
-    <mergeCell ref="BG18:BG20"/>
-    <mergeCell ref="BH18:BH20"/>
-    <mergeCell ref="BI18:BJ20"/>
-    <mergeCell ref="BK18:BK20"/>
-    <mergeCell ref="A21:A26"/>
-    <mergeCell ref="A18:AX20"/>
-    <mergeCell ref="AE39:AE44"/>
-    <mergeCell ref="T21:T26"/>
-    <mergeCell ref="M21:M26"/>
-    <mergeCell ref="N21:N26"/>
-    <mergeCell ref="O21:O26"/>
-    <mergeCell ref="P21:P26"/>
-    <mergeCell ref="Q21:Q26"/>
-    <mergeCell ref="R21:R26"/>
-    <mergeCell ref="AA21:AA26"/>
-    <mergeCell ref="K21:K26"/>
-    <mergeCell ref="J21:J26"/>
-    <mergeCell ref="D21:D26"/>
-    <mergeCell ref="B21:B26"/>
-    <mergeCell ref="C21:C26"/>
-    <mergeCell ref="L21:L26"/>
-    <mergeCell ref="AE28:AE37"/>
-    <mergeCell ref="AB21:AB26"/>
-    <mergeCell ref="AC21:AC26"/>
-    <mergeCell ref="AD21:AD26"/>
-    <mergeCell ref="AE21:AE26"/>
-    <mergeCell ref="AQ21:AQ26"/>
-    <mergeCell ref="AF21:AF26"/>
+    <mergeCell ref="CD21:CD26"/>
+    <mergeCell ref="CB35:CB47"/>
+    <mergeCell ref="CB49:CB52"/>
+    <mergeCell ref="CC28:CC33"/>
+    <mergeCell ref="CC35:CC47"/>
+    <mergeCell ref="CC49:CC52"/>
+    <mergeCell ref="BL21:BL26"/>
+    <mergeCell ref="BM21:BM26"/>
+    <mergeCell ref="BN21:BN26"/>
+    <mergeCell ref="BP21:BP26"/>
+    <mergeCell ref="CB18:CC20"/>
+    <mergeCell ref="CB21:CB26"/>
+    <mergeCell ref="CB28:CB33"/>
+    <mergeCell ref="BJ28:BJ34"/>
+    <mergeCell ref="CC21:CC26"/>
+    <mergeCell ref="BW21:BW26"/>
+    <mergeCell ref="BX21:BX26"/>
+    <mergeCell ref="BZ21:BZ26"/>
+    <mergeCell ref="CA21:CA26"/>
+    <mergeCell ref="BU21:BU26"/>
+    <mergeCell ref="BV21:BV26"/>
+    <mergeCell ref="BR21:BR26"/>
+    <mergeCell ref="BS21:BS26"/>
+    <mergeCell ref="BT21:BT26"/>
+    <mergeCell ref="BJ21:BJ26"/>
+    <mergeCell ref="BK21:BK26"/>
+    <mergeCell ref="BP29:BQ35"/>
+    <mergeCell ref="BY21:BY26"/>
+    <mergeCell ref="U21:U26"/>
+    <mergeCell ref="V21:V26"/>
+    <mergeCell ref="W21:W26"/>
+    <mergeCell ref="X21:X26"/>
+    <mergeCell ref="Y21:Y26"/>
+    <mergeCell ref="Z21:Z26"/>
+    <mergeCell ref="AK21:AK28"/>
+    <mergeCell ref="AO21:AO28"/>
+    <mergeCell ref="AS21:AS28"/>
+    <mergeCell ref="AW21:AW28"/>
+    <mergeCell ref="AZ21:AZ28"/>
+    <mergeCell ref="AM21:AM26"/>
+    <mergeCell ref="AN21:AN26"/>
+    <mergeCell ref="AP21:AP26"/>
+    <mergeCell ref="BE21:BE26"/>
+    <mergeCell ref="BF21:BF26"/>
+    <mergeCell ref="BG21:BG26"/>
+    <mergeCell ref="BH21:BH26"/>
     <mergeCell ref="BI21:BI26"/>
     <mergeCell ref="BB21:BB28"/>
     <mergeCell ref="BD21:BD28"/>
@@ -7047,59 +7062,44 @@
     <mergeCell ref="I21:I32"/>
     <mergeCell ref="AH21:AH26"/>
     <mergeCell ref="AI21:AI26"/>
-    <mergeCell ref="AW21:AW28"/>
-    <mergeCell ref="AZ21:AZ28"/>
-    <mergeCell ref="AM21:AM26"/>
-    <mergeCell ref="AN21:AN26"/>
-    <mergeCell ref="AP21:AP26"/>
-    <mergeCell ref="BE21:BE26"/>
-    <mergeCell ref="BF21:BF26"/>
-    <mergeCell ref="BG21:BG26"/>
-    <mergeCell ref="BH21:BH26"/>
+    <mergeCell ref="AJ21:AJ26"/>
+    <mergeCell ref="AL21:AL26"/>
     <mergeCell ref="AX21:AX26"/>
     <mergeCell ref="AR21:AR26"/>
-    <mergeCell ref="U21:U26"/>
-    <mergeCell ref="V21:V26"/>
-    <mergeCell ref="W21:W26"/>
-    <mergeCell ref="X21:X26"/>
-    <mergeCell ref="Y21:Y26"/>
-    <mergeCell ref="Z21:Z26"/>
-    <mergeCell ref="AK21:AK28"/>
-    <mergeCell ref="AO21:AO28"/>
-    <mergeCell ref="AS21:AS28"/>
-    <mergeCell ref="AJ21:AJ26"/>
-    <mergeCell ref="AL21:AL26"/>
-    <mergeCell ref="CB18:CC20"/>
-    <mergeCell ref="CB21:CB26"/>
-    <mergeCell ref="CB28:CB33"/>
-    <mergeCell ref="BJ28:BJ34"/>
-    <mergeCell ref="CC21:CC26"/>
-    <mergeCell ref="BW21:BW26"/>
-    <mergeCell ref="BX21:BX26"/>
-    <mergeCell ref="BZ21:BZ26"/>
-    <mergeCell ref="CA21:CA26"/>
-    <mergeCell ref="BU21:BU26"/>
-    <mergeCell ref="BV21:BV26"/>
-    <mergeCell ref="BR21:BR26"/>
-    <mergeCell ref="BS21:BS26"/>
-    <mergeCell ref="BT21:BT26"/>
-    <mergeCell ref="BJ21:BJ26"/>
-    <mergeCell ref="BK21:BK26"/>
-    <mergeCell ref="BP29:BQ35"/>
-    <mergeCell ref="BY21:BY26"/>
+    <mergeCell ref="B21:B26"/>
+    <mergeCell ref="C21:C26"/>
+    <mergeCell ref="L21:L26"/>
+    <mergeCell ref="AE28:AE37"/>
+    <mergeCell ref="AB21:AB26"/>
+    <mergeCell ref="AC21:AC26"/>
+    <mergeCell ref="AD21:AD26"/>
+    <mergeCell ref="AE21:AE26"/>
+    <mergeCell ref="AQ21:AQ26"/>
+    <mergeCell ref="AF21:AF26"/>
     <mergeCell ref="BO18:CA20"/>
+    <mergeCell ref="A18:AX20"/>
+    <mergeCell ref="AE39:AE44"/>
+    <mergeCell ref="T21:T26"/>
+    <mergeCell ref="M21:M26"/>
+    <mergeCell ref="N21:N26"/>
+    <mergeCell ref="O21:O26"/>
+    <mergeCell ref="P21:P26"/>
+    <mergeCell ref="Q21:Q26"/>
+    <mergeCell ref="R21:R26"/>
     <mergeCell ref="BO21:BO26"/>
+    <mergeCell ref="AA21:AA26"/>
     <mergeCell ref="BL18:BN20"/>
-    <mergeCell ref="CD21:CD26"/>
-    <mergeCell ref="CB35:CB47"/>
-    <mergeCell ref="CB49:CB52"/>
-    <mergeCell ref="CC28:CC33"/>
-    <mergeCell ref="CC35:CC47"/>
-    <mergeCell ref="CC49:CC52"/>
-    <mergeCell ref="BL21:BL26"/>
-    <mergeCell ref="BM21:BM26"/>
-    <mergeCell ref="BN21:BN26"/>
-    <mergeCell ref="BP21:BP26"/>
+    <mergeCell ref="K21:K26"/>
+    <mergeCell ref="J21:J26"/>
+    <mergeCell ref="D21:D26"/>
+    <mergeCell ref="BE18:BE20"/>
+    <mergeCell ref="AY18:BD20"/>
+    <mergeCell ref="BF18:BF20"/>
+    <mergeCell ref="BG18:BG20"/>
+    <mergeCell ref="BH18:BH20"/>
+    <mergeCell ref="BI18:BJ20"/>
+    <mergeCell ref="BK18:BK20"/>
+    <mergeCell ref="A21:A26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -7129,7 +7129,7 @@
         <v>NR_REFERENCIA_FISCAL,</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="K3" t="str">
         <f>CONCATENATE("'",J3,"',")</f>
@@ -7145,7 +7145,7 @@
         <v>CD_SITUACAO_NF,</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="K4" t="str">
         <f t="shared" ref="K4:K12" si="1">CONCATENATE("'",J4,"',")</f>
@@ -7170,14 +7170,14 @@
     </row>
     <row r="6" spans="3:11">
       <c r="C6" s="19" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
         <v>NR_REFERENCIA_FISCAL_FATURA,</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" si="1"/>
@@ -7186,14 +7186,14 @@
     </row>
     <row r="7" spans="3:11">
       <c r="C7" s="19" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
         <v>NR_ITEM_NF_FATURA,</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="K7" t="str">
         <f t="shared" si="1"/>
@@ -7209,7 +7209,7 @@
         <v>NR_NF_FATURA,</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="K8" t="str">
         <f t="shared" si="1"/>
@@ -7225,7 +7225,7 @@
         <v>NR_SERIE_NF_FATURA,</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="K9" t="str">
         <f t="shared" si="1"/>
@@ -7241,7 +7241,7 @@
         <v>NR_NF_REMESSA,</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="K10" t="str">
         <f t="shared" si="1"/>
@@ -7257,7 +7257,7 @@
         <v>NR_SERIE_NF_REMESSA,</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" si="1"/>
@@ -7273,7 +7273,7 @@
         <v>NR_ORDEM,</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="K12" t="str">
         <f t="shared" si="1"/>

</xml_diff>